<commit_message>
Mise à jour des fichier Excel.
Ordre du jour mis à jour.
</commit_message>
<xml_diff>
--- a/docs/M306_Planning_2022.xlsx
+++ b/docs/M306_Planning_2022.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CFPT\3ème_Année\2ème_semestre\M306 - Gestion de Projet\CFPT_M306\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IVAN.CLLVR\Desktop\Projet_M306\CFPT_M306\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
   <si>
     <t>Listes des tâches</t>
   </si>
@@ -59,12 +59,6 @@
   </si>
   <si>
     <t xml:space="preserve">Absences </t>
-  </si>
-  <si>
-    <t>Portes ouvertes</t>
-  </si>
-  <si>
-    <t>Vacances de février</t>
   </si>
   <si>
     <r>
@@ -173,7 +167,7 @@
     <numFmt numFmtId="166" formatCode="&quot;Semaine &quot;\ 0"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -225,11 +219,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="48"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -267,7 +256,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -290,12 +279,6 @@
       <patternFill patternType="solid">
         <fgColor indexed="9"/>
         <bgColor indexed="26"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -377,7 +360,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="59">
+  <borders count="54">
     <border>
       <left/>
       <right/>
@@ -499,63 +482,12 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1118,7 +1050,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1140,110 +1072,130 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1273,95 +1225,75 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="50" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="50" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="50" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="50" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="50" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="58" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="50" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="55" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="56" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="45" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="48" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="57" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="55" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="47" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="55" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="55" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="55" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="55" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1370,50 +1302,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="13" fillId="6" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="13" fillId="6" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="13" fillId="6" borderId="52" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="13" fillId="6" borderId="53" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="3" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="3" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="3" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="50" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="55" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1914,8 +1819,8 @@
   <dimension ref="A1:BM69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BQ13" sqref="BQ13"/>
+      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AK44" sqref="AK44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1933,10 +1838,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="84"/>
-      <c r="C1" s="98" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="93" t="s">
+      <c r="C1" s="70" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="88" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="81" t="s">
@@ -1946,188 +1851,188 @@
         <f>WEEKNUM(F2)</f>
         <v>6</v>
       </c>
-      <c r="G1" s="88"/>
-      <c r="H1" s="88"/>
-      <c r="I1" s="88"/>
-      <c r="J1" s="88"/>
-      <c r="K1" s="89"/>
-      <c r="L1" s="90">
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="76">
         <f>WEEKNUM(L2)</f>
         <v>7</v>
       </c>
-      <c r="M1" s="88"/>
-      <c r="N1" s="88"/>
-      <c r="O1" s="88"/>
-      <c r="P1" s="88"/>
-      <c r="Q1" s="89"/>
-      <c r="R1" s="90">
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="78"/>
+      <c r="R1" s="76">
         <f>WEEKNUM(R2)</f>
         <v>8</v>
       </c>
-      <c r="S1" s="88"/>
-      <c r="T1" s="88"/>
-      <c r="U1" s="88"/>
-      <c r="V1" s="88"/>
-      <c r="W1" s="89"/>
-      <c r="X1" s="90">
+      <c r="S1" s="77"/>
+      <c r="T1" s="77"/>
+      <c r="U1" s="77"/>
+      <c r="V1" s="77"/>
+      <c r="W1" s="78"/>
+      <c r="X1" s="76">
         <f>WEEKNUM(X2)</f>
         <v>9</v>
       </c>
-      <c r="Y1" s="88"/>
-      <c r="Z1" s="88"/>
-      <c r="AA1" s="88"/>
-      <c r="AB1" s="88"/>
-      <c r="AC1" s="89"/>
-      <c r="AD1" s="90">
+      <c r="Y1" s="77"/>
+      <c r="Z1" s="77"/>
+      <c r="AA1" s="77"/>
+      <c r="AB1" s="77"/>
+      <c r="AC1" s="78"/>
+      <c r="AD1" s="76">
         <f>WEEKNUM(AD2)</f>
         <v>10</v>
       </c>
-      <c r="AE1" s="88"/>
-      <c r="AF1" s="88"/>
-      <c r="AG1" s="88"/>
-      <c r="AH1" s="88"/>
-      <c r="AI1" s="89"/>
-      <c r="AJ1" s="90">
+      <c r="AE1" s="77"/>
+      <c r="AF1" s="77"/>
+      <c r="AG1" s="77"/>
+      <c r="AH1" s="77"/>
+      <c r="AI1" s="78"/>
+      <c r="AJ1" s="76">
         <f>WEEKNUM(AJ2)</f>
         <v>11</v>
       </c>
-      <c r="AK1" s="88"/>
-      <c r="AL1" s="88"/>
-      <c r="AM1" s="88"/>
-      <c r="AN1" s="88"/>
-      <c r="AO1" s="89"/>
-      <c r="AP1" s="90">
+      <c r="AK1" s="77"/>
+      <c r="AL1" s="77"/>
+      <c r="AM1" s="77"/>
+      <c r="AN1" s="77"/>
+      <c r="AO1" s="78"/>
+      <c r="AP1" s="76">
         <f>WEEKNUM(AP2)</f>
         <v>12</v>
       </c>
-      <c r="AQ1" s="88"/>
-      <c r="AR1" s="88"/>
-      <c r="AS1" s="88"/>
-      <c r="AT1" s="88"/>
-      <c r="AU1" s="89"/>
-      <c r="AV1" s="90">
+      <c r="AQ1" s="77"/>
+      <c r="AR1" s="77"/>
+      <c r="AS1" s="77"/>
+      <c r="AT1" s="77"/>
+      <c r="AU1" s="78"/>
+      <c r="AV1" s="76">
         <f>WEEKNUM(AV2)</f>
         <v>13</v>
       </c>
-      <c r="AW1" s="88"/>
-      <c r="AX1" s="88"/>
-      <c r="AY1" s="88"/>
-      <c r="AZ1" s="88"/>
-      <c r="BA1" s="89"/>
-      <c r="BB1" s="90">
+      <c r="AW1" s="77"/>
+      <c r="AX1" s="77"/>
+      <c r="AY1" s="77"/>
+      <c r="AZ1" s="77"/>
+      <c r="BA1" s="78"/>
+      <c r="BB1" s="76">
         <f>WEEKNUM(BB2)</f>
         <v>14</v>
       </c>
-      <c r="BC1" s="88"/>
-      <c r="BD1" s="88"/>
-      <c r="BE1" s="88"/>
-      <c r="BF1" s="88"/>
-      <c r="BG1" s="89"/>
-      <c r="BH1" s="90">
+      <c r="BC1" s="77"/>
+      <c r="BD1" s="77"/>
+      <c r="BE1" s="77"/>
+      <c r="BF1" s="77"/>
+      <c r="BG1" s="78"/>
+      <c r="BH1" s="76">
         <f>WEEKNUM(BH2)</f>
         <v>15</v>
       </c>
-      <c r="BI1" s="88"/>
-      <c r="BJ1" s="88"/>
-      <c r="BK1" s="88"/>
-      <c r="BL1" s="88"/>
-      <c r="BM1" s="89"/>
+      <c r="BI1" s="77"/>
+      <c r="BJ1" s="77"/>
+      <c r="BK1" s="77"/>
+      <c r="BL1" s="77"/>
+      <c r="BM1" s="78"/>
     </row>
     <row r="2" spans="1:65" ht="106.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="85"/>
       <c r="B2" s="86"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="94"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="89"/>
       <c r="E2" s="82"/>
-      <c r="F2" s="95">
+      <c r="F2" s="90">
         <v>44593</v>
       </c>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="91">
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="72">
         <f>F2+7</f>
         <v>44600</v>
       </c>
-      <c r="M2" s="92"/>
-      <c r="N2" s="92"/>
-      <c r="O2" s="96"/>
-      <c r="P2" s="96"/>
-      <c r="Q2" s="97"/>
-      <c r="R2" s="91">
+      <c r="M2" s="73"/>
+      <c r="N2" s="73"/>
+      <c r="O2" s="74"/>
+      <c r="P2" s="74"/>
+      <c r="Q2" s="75"/>
+      <c r="R2" s="72">
         <f>L2+7</f>
         <v>44607</v>
       </c>
-      <c r="S2" s="92"/>
-      <c r="T2" s="92"/>
-      <c r="U2" s="96"/>
-      <c r="V2" s="96"/>
-      <c r="W2" s="97"/>
-      <c r="X2" s="91">
+      <c r="S2" s="73"/>
+      <c r="T2" s="73"/>
+      <c r="U2" s="74"/>
+      <c r="V2" s="74"/>
+      <c r="W2" s="75"/>
+      <c r="X2" s="72">
         <f>R2+7</f>
         <v>44614</v>
       </c>
-      <c r="Y2" s="92"/>
-      <c r="Z2" s="92"/>
-      <c r="AA2" s="96"/>
-      <c r="AB2" s="96"/>
-      <c r="AC2" s="97"/>
-      <c r="AD2" s="91">
+      <c r="Y2" s="73"/>
+      <c r="Z2" s="73"/>
+      <c r="AA2" s="74"/>
+      <c r="AB2" s="74"/>
+      <c r="AC2" s="75"/>
+      <c r="AD2" s="72">
         <f>X2+7</f>
         <v>44621</v>
       </c>
-      <c r="AE2" s="92"/>
-      <c r="AF2" s="92"/>
-      <c r="AG2" s="96"/>
-      <c r="AH2" s="96"/>
-      <c r="AI2" s="97"/>
-      <c r="AJ2" s="91">
+      <c r="AE2" s="73"/>
+      <c r="AF2" s="73"/>
+      <c r="AG2" s="74"/>
+      <c r="AH2" s="74"/>
+      <c r="AI2" s="75"/>
+      <c r="AJ2" s="72">
         <f>AD2+7</f>
         <v>44628</v>
       </c>
-      <c r="AK2" s="92"/>
-      <c r="AL2" s="92"/>
-      <c r="AM2" s="96"/>
-      <c r="AN2" s="96"/>
-      <c r="AO2" s="97"/>
-      <c r="AP2" s="91">
+      <c r="AK2" s="73"/>
+      <c r="AL2" s="73"/>
+      <c r="AM2" s="74"/>
+      <c r="AN2" s="74"/>
+      <c r="AO2" s="75"/>
+      <c r="AP2" s="72">
         <f>AJ2+7</f>
         <v>44635</v>
       </c>
-      <c r="AQ2" s="92"/>
-      <c r="AR2" s="92"/>
-      <c r="AS2" s="96"/>
-      <c r="AT2" s="96"/>
-      <c r="AU2" s="97"/>
-      <c r="AV2" s="91">
+      <c r="AQ2" s="73"/>
+      <c r="AR2" s="73"/>
+      <c r="AS2" s="74"/>
+      <c r="AT2" s="74"/>
+      <c r="AU2" s="75"/>
+      <c r="AV2" s="72">
         <f>AP2+7</f>
         <v>44642</v>
       </c>
-      <c r="AW2" s="92"/>
-      <c r="AX2" s="92"/>
-      <c r="AY2" s="96"/>
-      <c r="AZ2" s="96"/>
-      <c r="BA2" s="97"/>
-      <c r="BB2" s="91">
+      <c r="AW2" s="73"/>
+      <c r="AX2" s="73"/>
+      <c r="AY2" s="74"/>
+      <c r="AZ2" s="74"/>
+      <c r="BA2" s="75"/>
+      <c r="BB2" s="72">
         <f>AV2+7</f>
         <v>44649</v>
       </c>
-      <c r="BC2" s="92"/>
-      <c r="BD2" s="92"/>
-      <c r="BE2" s="96"/>
-      <c r="BF2" s="96"/>
-      <c r="BG2" s="97"/>
-      <c r="BH2" s="91">
+      <c r="BC2" s="73"/>
+      <c r="BD2" s="73"/>
+      <c r="BE2" s="74"/>
+      <c r="BF2" s="74"/>
+      <c r="BG2" s="75"/>
+      <c r="BH2" s="72">
         <f>BB2+7</f>
         <v>44656</v>
       </c>
-      <c r="BI2" s="92"/>
-      <c r="BJ2" s="92"/>
-      <c r="BK2" s="96"/>
-      <c r="BL2" s="96"/>
-      <c r="BM2" s="97"/>
+      <c r="BI2" s="73"/>
+      <c r="BJ2" s="73"/>
+      <c r="BK2" s="74"/>
+      <c r="BL2" s="74"/>
+      <c r="BM2" s="75"/>
     </row>
     <row r="3" spans="1:65" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="79" t="s">
@@ -2139,7 +2044,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="60">
-        <f>SUM(COUNTIF($F3:$BA3,"X"))/2</f>
+        <f>SUM(COUNTIF($F3:$BM3,"X"))/2</f>
         <v>0</v>
       </c>
       <c r="F3" s="10"/>
@@ -2166,22 +2071,18 @@
       <c r="AA3" s="11"/>
       <c r="AB3" s="11"/>
       <c r="AC3" s="12"/>
-      <c r="AD3" s="70" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE3" s="71"/>
-      <c r="AF3" s="71"/>
-      <c r="AG3" s="71"/>
-      <c r="AH3" s="71"/>
-      <c r="AI3" s="72"/>
-      <c r="AJ3" s="70" t="s">
-        <v>11</v>
-      </c>
-      <c r="AK3" s="71"/>
-      <c r="AL3" s="71"/>
-      <c r="AM3" s="71"/>
-      <c r="AN3" s="71"/>
-      <c r="AO3" s="72"/>
+      <c r="AD3" s="10"/>
+      <c r="AE3" s="11"/>
+      <c r="AF3" s="11"/>
+      <c r="AG3" s="11"/>
+      <c r="AH3" s="11"/>
+      <c r="AI3" s="12"/>
+      <c r="AJ3" s="10"/>
+      <c r="AK3" s="11"/>
+      <c r="AL3" s="11"/>
+      <c r="AM3" s="11"/>
+      <c r="AN3" s="11"/>
+      <c r="AO3" s="12"/>
       <c r="AP3" s="10"/>
       <c r="AQ3" s="11"/>
       <c r="AR3" s="11"/>
@@ -2245,18 +2146,18 @@
       <c r="AA4" s="4"/>
       <c r="AB4" s="4"/>
       <c r="AC4" s="5"/>
-      <c r="AD4" s="73"/>
-      <c r="AE4" s="74"/>
-      <c r="AF4" s="74"/>
-      <c r="AG4" s="74"/>
-      <c r="AH4" s="74"/>
-      <c r="AI4" s="75"/>
-      <c r="AJ4" s="73"/>
-      <c r="AK4" s="74"/>
-      <c r="AL4" s="74"/>
-      <c r="AM4" s="74"/>
-      <c r="AN4" s="74"/>
-      <c r="AO4" s="75"/>
+      <c r="AD4" s="6"/>
+      <c r="AE4" s="4"/>
+      <c r="AF4" s="4"/>
+      <c r="AG4" s="4"/>
+      <c r="AH4" s="4"/>
+      <c r="AI4" s="5"/>
+      <c r="AJ4" s="6"/>
+      <c r="AK4" s="4"/>
+      <c r="AL4" s="4"/>
+      <c r="AM4" s="4"/>
+      <c r="AN4" s="4"/>
+      <c r="AO4" s="5"/>
       <c r="AP4" s="6"/>
       <c r="AQ4" s="4"/>
       <c r="AR4" s="4"/>
@@ -2285,10 +2186,10 @@
     <row r="5" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A5" s="23"/>
       <c r="B5" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" s="63" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D5" s="41">
         <f>IF($B5&gt;"",SUM(COUNTIF(F5:BM5,"P"))/2,"")</f>
@@ -2322,18 +2223,18 @@
       <c r="AA5" s="49"/>
       <c r="AB5" s="49"/>
       <c r="AC5" s="50"/>
-      <c r="AD5" s="73"/>
-      <c r="AE5" s="74"/>
-      <c r="AF5" s="74"/>
-      <c r="AG5" s="74"/>
-      <c r="AH5" s="74"/>
-      <c r="AI5" s="75"/>
-      <c r="AJ5" s="73"/>
-      <c r="AK5" s="74"/>
-      <c r="AL5" s="74"/>
-      <c r="AM5" s="74"/>
-      <c r="AN5" s="74"/>
-      <c r="AO5" s="75"/>
+      <c r="AD5" s="48"/>
+      <c r="AE5" s="49"/>
+      <c r="AF5" s="49"/>
+      <c r="AG5" s="49"/>
+      <c r="AH5" s="49"/>
+      <c r="AI5" s="50"/>
+      <c r="AJ5" s="48"/>
+      <c r="AK5" s="49"/>
+      <c r="AL5" s="49"/>
+      <c r="AM5" s="49"/>
+      <c r="AN5" s="49"/>
+      <c r="AO5" s="50"/>
       <c r="AP5" s="48"/>
       <c r="AQ5" s="49"/>
       <c r="AR5" s="49"/>
@@ -2362,10 +2263,10 @@
     <row r="6" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A6" s="23"/>
       <c r="B6" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C6" s="63" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D6" s="41">
         <f t="shared" ref="D6:D14" si="0">IF($B6&gt;"",SUM(COUNTIF(F6:BM6,"P"))/2,"")</f>
@@ -2376,10 +2277,10 @@
         <v>1</v>
       </c>
       <c r="F6" s="51" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G6" s="52" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H6" s="52"/>
       <c r="I6" s="52"/>
@@ -2403,18 +2304,18 @@
       <c r="AA6" s="52"/>
       <c r="AB6" s="52"/>
       <c r="AC6" s="53"/>
-      <c r="AD6" s="73"/>
-      <c r="AE6" s="74"/>
-      <c r="AF6" s="74"/>
-      <c r="AG6" s="74"/>
-      <c r="AH6" s="74"/>
-      <c r="AI6" s="75"/>
-      <c r="AJ6" s="73"/>
-      <c r="AK6" s="74"/>
-      <c r="AL6" s="74"/>
-      <c r="AM6" s="74"/>
-      <c r="AN6" s="74"/>
-      <c r="AO6" s="75"/>
+      <c r="AD6" s="51"/>
+      <c r="AE6" s="52"/>
+      <c r="AF6" s="52"/>
+      <c r="AG6" s="52"/>
+      <c r="AH6" s="52"/>
+      <c r="AI6" s="53"/>
+      <c r="AJ6" s="51"/>
+      <c r="AK6" s="52"/>
+      <c r="AL6" s="52"/>
+      <c r="AM6" s="52"/>
+      <c r="AN6" s="52"/>
+      <c r="AO6" s="53"/>
       <c r="AP6" s="51"/>
       <c r="AQ6" s="52"/>
       <c r="AR6" s="52"/>
@@ -2443,10 +2344,10 @@
     <row r="7" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A7" s="23"/>
       <c r="B7" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C7" s="63" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D7" s="41">
         <f t="shared" si="0"/>
@@ -2457,10 +2358,10 @@
         <v>1</v>
       </c>
       <c r="F7" s="51" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G7" s="52" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H7" s="52"/>
       <c r="I7" s="52"/>
@@ -2484,18 +2385,18 @@
       <c r="AA7" s="52"/>
       <c r="AB7" s="52"/>
       <c r="AC7" s="53"/>
-      <c r="AD7" s="73"/>
-      <c r="AE7" s="74"/>
-      <c r="AF7" s="74"/>
-      <c r="AG7" s="74"/>
-      <c r="AH7" s="74"/>
-      <c r="AI7" s="75"/>
-      <c r="AJ7" s="73"/>
-      <c r="AK7" s="74"/>
-      <c r="AL7" s="74"/>
-      <c r="AM7" s="74"/>
-      <c r="AN7" s="74"/>
-      <c r="AO7" s="75"/>
+      <c r="AD7" s="51"/>
+      <c r="AE7" s="52"/>
+      <c r="AF7" s="52"/>
+      <c r="AG7" s="52"/>
+      <c r="AH7" s="52"/>
+      <c r="AI7" s="53"/>
+      <c r="AJ7" s="51"/>
+      <c r="AK7" s="52"/>
+      <c r="AL7" s="52"/>
+      <c r="AM7" s="52"/>
+      <c r="AN7" s="52"/>
+      <c r="AO7" s="53"/>
       <c r="AP7" s="51"/>
       <c r="AQ7" s="52"/>
       <c r="AR7" s="52"/>
@@ -2524,10 +2425,10 @@
     <row r="8" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A8" s="23"/>
       <c r="B8" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C8" s="63" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D8" s="41">
         <f t="shared" si="0"/>
@@ -2538,7 +2439,7 @@
         <v>0.5</v>
       </c>
       <c r="F8" s="51" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G8" s="52"/>
       <c r="H8" s="52"/>
@@ -2563,18 +2464,18 @@
       <c r="AA8" s="52"/>
       <c r="AB8" s="52"/>
       <c r="AC8" s="53"/>
-      <c r="AD8" s="73"/>
-      <c r="AE8" s="74"/>
-      <c r="AF8" s="74"/>
-      <c r="AG8" s="74"/>
-      <c r="AH8" s="74"/>
-      <c r="AI8" s="75"/>
-      <c r="AJ8" s="73"/>
-      <c r="AK8" s="74"/>
-      <c r="AL8" s="74"/>
-      <c r="AM8" s="74"/>
-      <c r="AN8" s="74"/>
-      <c r="AO8" s="75"/>
+      <c r="AD8" s="51"/>
+      <c r="AE8" s="52"/>
+      <c r="AF8" s="52"/>
+      <c r="AG8" s="52"/>
+      <c r="AH8" s="52"/>
+      <c r="AI8" s="53"/>
+      <c r="AJ8" s="51"/>
+      <c r="AK8" s="52"/>
+      <c r="AL8" s="52"/>
+      <c r="AM8" s="52"/>
+      <c r="AN8" s="52"/>
+      <c r="AO8" s="53"/>
       <c r="AP8" s="51"/>
       <c r="AQ8" s="52"/>
       <c r="AR8" s="52"/>
@@ -2603,10 +2504,10 @@
     <row r="9" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A9" s="23"/>
       <c r="B9" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C9" s="63" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D9" s="41">
         <f t="shared" si="0"/>
@@ -2640,18 +2541,18 @@
       <c r="AA9" s="52"/>
       <c r="AB9" s="52"/>
       <c r="AC9" s="53"/>
-      <c r="AD9" s="73"/>
-      <c r="AE9" s="74"/>
-      <c r="AF9" s="74"/>
-      <c r="AG9" s="74"/>
-      <c r="AH9" s="74"/>
-      <c r="AI9" s="75"/>
-      <c r="AJ9" s="73"/>
-      <c r="AK9" s="74"/>
-      <c r="AL9" s="74"/>
-      <c r="AM9" s="74"/>
-      <c r="AN9" s="74"/>
-      <c r="AO9" s="75"/>
+      <c r="AD9" s="51"/>
+      <c r="AE9" s="52"/>
+      <c r="AF9" s="52"/>
+      <c r="AG9" s="52"/>
+      <c r="AH9" s="52"/>
+      <c r="AI9" s="53"/>
+      <c r="AJ9" s="51"/>
+      <c r="AK9" s="52"/>
+      <c r="AL9" s="52"/>
+      <c r="AM9" s="52"/>
+      <c r="AN9" s="52"/>
+      <c r="AO9" s="53"/>
       <c r="AP9" s="51"/>
       <c r="AQ9" s="52"/>
       <c r="AR9" s="52"/>
@@ -2680,7 +2581,7 @@
     <row r="10" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A10" s="23"/>
       <c r="B10" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C10" s="63"/>
       <c r="D10" s="41">
@@ -2715,18 +2616,18 @@
       <c r="AA10" s="52"/>
       <c r="AB10" s="52"/>
       <c r="AC10" s="53"/>
-      <c r="AD10" s="73"/>
-      <c r="AE10" s="74"/>
-      <c r="AF10" s="74"/>
-      <c r="AG10" s="74"/>
-      <c r="AH10" s="74"/>
-      <c r="AI10" s="75"/>
-      <c r="AJ10" s="73"/>
-      <c r="AK10" s="74"/>
-      <c r="AL10" s="74"/>
-      <c r="AM10" s="74"/>
-      <c r="AN10" s="74"/>
-      <c r="AO10" s="75"/>
+      <c r="AD10" s="51"/>
+      <c r="AE10" s="52"/>
+      <c r="AF10" s="52"/>
+      <c r="AG10" s="52"/>
+      <c r="AH10" s="52"/>
+      <c r="AI10" s="53"/>
+      <c r="AJ10" s="51"/>
+      <c r="AK10" s="52"/>
+      <c r="AL10" s="52"/>
+      <c r="AM10" s="52"/>
+      <c r="AN10" s="52"/>
+      <c r="AO10" s="53"/>
       <c r="AP10" s="51"/>
       <c r="AQ10" s="52"/>
       <c r="AR10" s="52"/>
@@ -2788,18 +2689,18 @@
       <c r="AA11" s="52"/>
       <c r="AB11" s="52"/>
       <c r="AC11" s="53"/>
-      <c r="AD11" s="73"/>
-      <c r="AE11" s="74"/>
-      <c r="AF11" s="74"/>
-      <c r="AG11" s="74"/>
-      <c r="AH11" s="74"/>
-      <c r="AI11" s="75"/>
-      <c r="AJ11" s="73"/>
-      <c r="AK11" s="74"/>
-      <c r="AL11" s="74"/>
-      <c r="AM11" s="74"/>
-      <c r="AN11" s="74"/>
-      <c r="AO11" s="75"/>
+      <c r="AD11" s="51"/>
+      <c r="AE11" s="52"/>
+      <c r="AF11" s="52"/>
+      <c r="AG11" s="52"/>
+      <c r="AH11" s="52"/>
+      <c r="AI11" s="53"/>
+      <c r="AJ11" s="51"/>
+      <c r="AK11" s="52"/>
+      <c r="AL11" s="52"/>
+      <c r="AM11" s="52"/>
+      <c r="AN11" s="52"/>
+      <c r="AO11" s="53"/>
       <c r="AP11" s="51"/>
       <c r="AQ11" s="52"/>
       <c r="AR11" s="52"/>
@@ -2861,18 +2762,18 @@
       <c r="AA12" s="52"/>
       <c r="AB12" s="52"/>
       <c r="AC12" s="53"/>
-      <c r="AD12" s="73"/>
-      <c r="AE12" s="74"/>
-      <c r="AF12" s="74"/>
-      <c r="AG12" s="74"/>
-      <c r="AH12" s="74"/>
-      <c r="AI12" s="75"/>
-      <c r="AJ12" s="73"/>
-      <c r="AK12" s="74"/>
-      <c r="AL12" s="74"/>
-      <c r="AM12" s="74"/>
-      <c r="AN12" s="74"/>
-      <c r="AO12" s="75"/>
+      <c r="AD12" s="51"/>
+      <c r="AE12" s="52"/>
+      <c r="AF12" s="52"/>
+      <c r="AG12" s="52"/>
+      <c r="AH12" s="52"/>
+      <c r="AI12" s="53"/>
+      <c r="AJ12" s="51"/>
+      <c r="AK12" s="52"/>
+      <c r="AL12" s="52"/>
+      <c r="AM12" s="52"/>
+      <c r="AN12" s="52"/>
+      <c r="AO12" s="53"/>
       <c r="AP12" s="51"/>
       <c r="AQ12" s="52"/>
       <c r="AR12" s="52"/>
@@ -2934,18 +2835,18 @@
       <c r="AA13" s="52"/>
       <c r="AB13" s="52"/>
       <c r="AC13" s="53"/>
-      <c r="AD13" s="73"/>
-      <c r="AE13" s="74"/>
-      <c r="AF13" s="74"/>
-      <c r="AG13" s="74"/>
-      <c r="AH13" s="74"/>
-      <c r="AI13" s="75"/>
-      <c r="AJ13" s="73"/>
-      <c r="AK13" s="74"/>
-      <c r="AL13" s="74"/>
-      <c r="AM13" s="74"/>
-      <c r="AN13" s="74"/>
-      <c r="AO13" s="75"/>
+      <c r="AD13" s="51"/>
+      <c r="AE13" s="52"/>
+      <c r="AF13" s="52"/>
+      <c r="AG13" s="52"/>
+      <c r="AH13" s="52"/>
+      <c r="AI13" s="53"/>
+      <c r="AJ13" s="51"/>
+      <c r="AK13" s="52"/>
+      <c r="AL13" s="52"/>
+      <c r="AM13" s="52"/>
+      <c r="AN13" s="52"/>
+      <c r="AO13" s="53"/>
       <c r="AP13" s="51"/>
       <c r="AQ13" s="52"/>
       <c r="AR13" s="52"/>
@@ -3007,18 +2908,18 @@
       <c r="AA14" s="55"/>
       <c r="AB14" s="55"/>
       <c r="AC14" s="56"/>
-      <c r="AD14" s="73"/>
-      <c r="AE14" s="74"/>
-      <c r="AF14" s="74"/>
-      <c r="AG14" s="74"/>
-      <c r="AH14" s="74"/>
-      <c r="AI14" s="75"/>
-      <c r="AJ14" s="73"/>
-      <c r="AK14" s="74"/>
-      <c r="AL14" s="74"/>
-      <c r="AM14" s="74"/>
-      <c r="AN14" s="74"/>
-      <c r="AO14" s="75"/>
+      <c r="AD14" s="54"/>
+      <c r="AE14" s="55"/>
+      <c r="AF14" s="55"/>
+      <c r="AG14" s="55"/>
+      <c r="AH14" s="55"/>
+      <c r="AI14" s="56"/>
+      <c r="AJ14" s="54"/>
+      <c r="AK14" s="55"/>
+      <c r="AL14" s="55"/>
+      <c r="AM14" s="55"/>
+      <c r="AN14" s="55"/>
+      <c r="AO14" s="56"/>
       <c r="AP14" s="54"/>
       <c r="AQ14" s="55"/>
       <c r="AR14" s="55"/>
@@ -3082,18 +2983,18 @@
       <c r="AA15" s="4"/>
       <c r="AB15" s="4"/>
       <c r="AC15" s="5"/>
-      <c r="AD15" s="73"/>
-      <c r="AE15" s="74"/>
-      <c r="AF15" s="74"/>
-      <c r="AG15" s="74"/>
-      <c r="AH15" s="74"/>
-      <c r="AI15" s="75"/>
-      <c r="AJ15" s="73"/>
-      <c r="AK15" s="74"/>
-      <c r="AL15" s="74"/>
-      <c r="AM15" s="74"/>
-      <c r="AN15" s="74"/>
-      <c r="AO15" s="75"/>
+      <c r="AD15" s="6"/>
+      <c r="AE15" s="4"/>
+      <c r="AF15" s="4"/>
+      <c r="AG15" s="4"/>
+      <c r="AH15" s="4"/>
+      <c r="AI15" s="5"/>
+      <c r="AJ15" s="6"/>
+      <c r="AK15" s="4"/>
+      <c r="AL15" s="4"/>
+      <c r="AM15" s="4"/>
+      <c r="AN15" s="4"/>
+      <c r="AO15" s="5"/>
       <c r="AP15" s="6"/>
       <c r="AQ15" s="4"/>
       <c r="AR15" s="4"/>
@@ -3122,10 +3023,10 @@
     <row r="16" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A16" s="23"/>
       <c r="B16" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C16" s="63" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D16" s="41">
         <f>IF($B16&gt;"",SUM(COUNTIF(F16:BM16,"P"))/2,"")</f>
@@ -3159,18 +3060,18 @@
       <c r="AA16" s="49"/>
       <c r="AB16" s="49"/>
       <c r="AC16" s="50"/>
-      <c r="AD16" s="73"/>
-      <c r="AE16" s="74"/>
-      <c r="AF16" s="74"/>
-      <c r="AG16" s="74"/>
-      <c r="AH16" s="74"/>
-      <c r="AI16" s="75"/>
-      <c r="AJ16" s="73"/>
-      <c r="AK16" s="74"/>
-      <c r="AL16" s="74"/>
-      <c r="AM16" s="74"/>
-      <c r="AN16" s="74"/>
-      <c r="AO16" s="75"/>
+      <c r="AD16" s="48"/>
+      <c r="AE16" s="49"/>
+      <c r="AF16" s="49"/>
+      <c r="AG16" s="49"/>
+      <c r="AH16" s="49"/>
+      <c r="AI16" s="50"/>
+      <c r="AJ16" s="48"/>
+      <c r="AK16" s="49"/>
+      <c r="AL16" s="49"/>
+      <c r="AM16" s="49"/>
+      <c r="AN16" s="49"/>
+      <c r="AO16" s="50"/>
       <c r="AP16" s="48"/>
       <c r="AQ16" s="49"/>
       <c r="AR16" s="49"/>
@@ -3199,10 +3100,10 @@
     <row r="17" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A17" s="23"/>
       <c r="B17" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C17" s="63" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D17" s="41">
         <f>IF($B17&gt;"",SUM(COUNTIF(F17:BM17,"P"))/2,"")</f>
@@ -3213,13 +3114,13 @@
         <v>1.5</v>
       </c>
       <c r="F17" s="51" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G17" s="52" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H17" s="52" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I17" s="52"/>
       <c r="J17" s="52"/>
@@ -3242,18 +3143,18 @@
       <c r="AA17" s="52"/>
       <c r="AB17" s="52"/>
       <c r="AC17" s="53"/>
-      <c r="AD17" s="73"/>
-      <c r="AE17" s="74"/>
-      <c r="AF17" s="74"/>
-      <c r="AG17" s="74"/>
-      <c r="AH17" s="74"/>
-      <c r="AI17" s="75"/>
-      <c r="AJ17" s="73"/>
-      <c r="AK17" s="74"/>
-      <c r="AL17" s="74"/>
-      <c r="AM17" s="74"/>
-      <c r="AN17" s="74"/>
-      <c r="AO17" s="75"/>
+      <c r="AD17" s="51"/>
+      <c r="AE17" s="52"/>
+      <c r="AF17" s="52"/>
+      <c r="AG17" s="52"/>
+      <c r="AH17" s="52"/>
+      <c r="AI17" s="53"/>
+      <c r="AJ17" s="51"/>
+      <c r="AK17" s="52"/>
+      <c r="AL17" s="52"/>
+      <c r="AM17" s="52"/>
+      <c r="AN17" s="52"/>
+      <c r="AO17" s="53"/>
       <c r="AP17" s="51"/>
       <c r="AQ17" s="52"/>
       <c r="AR17" s="52"/>
@@ -3282,10 +3183,10 @@
     <row r="18" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A18" s="23"/>
       <c r="B18" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C18" s="63" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D18" s="41">
         <f>IF($B18&gt;"",SUM(COUNTIF(F18:BM18,"P"))/2,"")</f>
@@ -3305,10 +3206,10 @@
       <c r="M18" s="52"/>
       <c r="N18" s="52"/>
       <c r="O18" s="52" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="P18" s="52" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q18" s="53"/>
       <c r="R18" s="51"/>
@@ -3323,18 +3224,18 @@
       <c r="AA18" s="52"/>
       <c r="AB18" s="52"/>
       <c r="AC18" s="53"/>
-      <c r="AD18" s="73"/>
-      <c r="AE18" s="74"/>
-      <c r="AF18" s="74"/>
-      <c r="AG18" s="74"/>
-      <c r="AH18" s="74"/>
-      <c r="AI18" s="75"/>
-      <c r="AJ18" s="73"/>
-      <c r="AK18" s="74"/>
-      <c r="AL18" s="74"/>
-      <c r="AM18" s="74"/>
-      <c r="AN18" s="74"/>
-      <c r="AO18" s="75"/>
+      <c r="AD18" s="51"/>
+      <c r="AE18" s="52"/>
+      <c r="AF18" s="52"/>
+      <c r="AG18" s="52"/>
+      <c r="AH18" s="52"/>
+      <c r="AI18" s="53"/>
+      <c r="AJ18" s="51"/>
+      <c r="AK18" s="52"/>
+      <c r="AL18" s="52"/>
+      <c r="AM18" s="52"/>
+      <c r="AN18" s="52"/>
+      <c r="AO18" s="53"/>
       <c r="AP18" s="51"/>
       <c r="AQ18" s="52"/>
       <c r="AR18" s="52"/>
@@ -3396,18 +3297,18 @@
       <c r="AA19" s="52"/>
       <c r="AB19" s="52"/>
       <c r="AC19" s="53"/>
-      <c r="AD19" s="73"/>
-      <c r="AE19" s="74"/>
-      <c r="AF19" s="74"/>
-      <c r="AG19" s="74"/>
-      <c r="AH19" s="74"/>
-      <c r="AI19" s="75"/>
-      <c r="AJ19" s="73"/>
-      <c r="AK19" s="74"/>
-      <c r="AL19" s="74"/>
-      <c r="AM19" s="74"/>
-      <c r="AN19" s="74"/>
-      <c r="AO19" s="75"/>
+      <c r="AD19" s="51"/>
+      <c r="AE19" s="52"/>
+      <c r="AF19" s="52"/>
+      <c r="AG19" s="52"/>
+      <c r="AH19" s="52"/>
+      <c r="AI19" s="53"/>
+      <c r="AJ19" s="51"/>
+      <c r="AK19" s="52"/>
+      <c r="AL19" s="52"/>
+      <c r="AM19" s="52"/>
+      <c r="AN19" s="52"/>
+      <c r="AO19" s="53"/>
       <c r="AP19" s="51"/>
       <c r="AQ19" s="52"/>
       <c r="AR19" s="52"/>
@@ -3469,18 +3370,18 @@
       <c r="AA20" s="52"/>
       <c r="AB20" s="52"/>
       <c r="AC20" s="53"/>
-      <c r="AD20" s="73"/>
-      <c r="AE20" s="74"/>
-      <c r="AF20" s="74"/>
-      <c r="AG20" s="74"/>
-      <c r="AH20" s="74"/>
-      <c r="AI20" s="75"/>
-      <c r="AJ20" s="73"/>
-      <c r="AK20" s="74"/>
-      <c r="AL20" s="74"/>
-      <c r="AM20" s="74"/>
-      <c r="AN20" s="74"/>
-      <c r="AO20" s="75"/>
+      <c r="AD20" s="51"/>
+      <c r="AE20" s="52"/>
+      <c r="AF20" s="52"/>
+      <c r="AG20" s="52"/>
+      <c r="AH20" s="52"/>
+      <c r="AI20" s="53"/>
+      <c r="AJ20" s="51"/>
+      <c r="AK20" s="52"/>
+      <c r="AL20" s="52"/>
+      <c r="AM20" s="52"/>
+      <c r="AN20" s="52"/>
+      <c r="AO20" s="53"/>
       <c r="AP20" s="51"/>
       <c r="AQ20" s="52"/>
       <c r="AR20" s="52"/>
@@ -3542,18 +3443,18 @@
       <c r="AA21" s="52"/>
       <c r="AB21" s="52"/>
       <c r="AC21" s="53"/>
-      <c r="AD21" s="73"/>
-      <c r="AE21" s="74"/>
-      <c r="AF21" s="74"/>
-      <c r="AG21" s="74"/>
-      <c r="AH21" s="74"/>
-      <c r="AI21" s="75"/>
-      <c r="AJ21" s="73"/>
-      <c r="AK21" s="74"/>
-      <c r="AL21" s="74"/>
-      <c r="AM21" s="74"/>
-      <c r="AN21" s="74"/>
-      <c r="AO21" s="75"/>
+      <c r="AD21" s="51"/>
+      <c r="AE21" s="52"/>
+      <c r="AF21" s="52"/>
+      <c r="AG21" s="52"/>
+      <c r="AH21" s="52"/>
+      <c r="AI21" s="53"/>
+      <c r="AJ21" s="51"/>
+      <c r="AK21" s="52"/>
+      <c r="AL21" s="52"/>
+      <c r="AM21" s="52"/>
+      <c r="AN21" s="52"/>
+      <c r="AO21" s="53"/>
       <c r="AP21" s="51"/>
       <c r="AQ21" s="52"/>
       <c r="AR21" s="52"/>
@@ -3615,18 +3516,18 @@
       <c r="AA22" s="52"/>
       <c r="AB22" s="52"/>
       <c r="AC22" s="53"/>
-      <c r="AD22" s="73"/>
-      <c r="AE22" s="74"/>
-      <c r="AF22" s="74"/>
-      <c r="AG22" s="74"/>
-      <c r="AH22" s="74"/>
-      <c r="AI22" s="75"/>
-      <c r="AJ22" s="73"/>
-      <c r="AK22" s="74"/>
-      <c r="AL22" s="74"/>
-      <c r="AM22" s="74"/>
-      <c r="AN22" s="74"/>
-      <c r="AO22" s="75"/>
+      <c r="AD22" s="51"/>
+      <c r="AE22" s="52"/>
+      <c r="AF22" s="52"/>
+      <c r="AG22" s="52"/>
+      <c r="AH22" s="52"/>
+      <c r="AI22" s="53"/>
+      <c r="AJ22" s="51"/>
+      <c r="AK22" s="52"/>
+      <c r="AL22" s="52"/>
+      <c r="AM22" s="52"/>
+      <c r="AN22" s="52"/>
+      <c r="AO22" s="53"/>
       <c r="AP22" s="51"/>
       <c r="AQ22" s="52"/>
       <c r="AR22" s="52"/>
@@ -3688,18 +3589,18 @@
       <c r="AA23" s="52"/>
       <c r="AB23" s="52"/>
       <c r="AC23" s="53"/>
-      <c r="AD23" s="73"/>
-      <c r="AE23" s="74"/>
-      <c r="AF23" s="74"/>
-      <c r="AG23" s="74"/>
-      <c r="AH23" s="74"/>
-      <c r="AI23" s="75"/>
-      <c r="AJ23" s="73"/>
-      <c r="AK23" s="74"/>
-      <c r="AL23" s="74"/>
-      <c r="AM23" s="74"/>
-      <c r="AN23" s="74"/>
-      <c r="AO23" s="75"/>
+      <c r="AD23" s="51"/>
+      <c r="AE23" s="52"/>
+      <c r="AF23" s="52"/>
+      <c r="AG23" s="52"/>
+      <c r="AH23" s="52"/>
+      <c r="AI23" s="53"/>
+      <c r="AJ23" s="51"/>
+      <c r="AK23" s="52"/>
+      <c r="AL23" s="52"/>
+      <c r="AM23" s="52"/>
+      <c r="AN23" s="52"/>
+      <c r="AO23" s="53"/>
       <c r="AP23" s="51"/>
       <c r="AQ23" s="52"/>
       <c r="AR23" s="52"/>
@@ -3761,18 +3662,18 @@
       <c r="AA24" s="52"/>
       <c r="AB24" s="52"/>
       <c r="AC24" s="53"/>
-      <c r="AD24" s="73"/>
-      <c r="AE24" s="74"/>
-      <c r="AF24" s="74"/>
-      <c r="AG24" s="74"/>
-      <c r="AH24" s="74"/>
-      <c r="AI24" s="75"/>
-      <c r="AJ24" s="73"/>
-      <c r="AK24" s="74"/>
-      <c r="AL24" s="74"/>
-      <c r="AM24" s="74"/>
-      <c r="AN24" s="74"/>
-      <c r="AO24" s="75"/>
+      <c r="AD24" s="51"/>
+      <c r="AE24" s="52"/>
+      <c r="AF24" s="52"/>
+      <c r="AG24" s="52"/>
+      <c r="AH24" s="52"/>
+      <c r="AI24" s="53"/>
+      <c r="AJ24" s="51"/>
+      <c r="AK24" s="52"/>
+      <c r="AL24" s="52"/>
+      <c r="AM24" s="52"/>
+      <c r="AN24" s="52"/>
+      <c r="AO24" s="53"/>
       <c r="AP24" s="51"/>
       <c r="AQ24" s="52"/>
       <c r="AR24" s="52"/>
@@ -3834,18 +3735,18 @@
       <c r="AA25" s="55"/>
       <c r="AB25" s="55"/>
       <c r="AC25" s="56"/>
-      <c r="AD25" s="73"/>
-      <c r="AE25" s="74"/>
-      <c r="AF25" s="74"/>
-      <c r="AG25" s="74"/>
-      <c r="AH25" s="74"/>
-      <c r="AI25" s="75"/>
-      <c r="AJ25" s="73"/>
-      <c r="AK25" s="74"/>
-      <c r="AL25" s="74"/>
-      <c r="AM25" s="74"/>
-      <c r="AN25" s="74"/>
-      <c r="AO25" s="75"/>
+      <c r="AD25" s="54"/>
+      <c r="AE25" s="55"/>
+      <c r="AF25" s="55"/>
+      <c r="AG25" s="55"/>
+      <c r="AH25" s="55"/>
+      <c r="AI25" s="56"/>
+      <c r="AJ25" s="54"/>
+      <c r="AK25" s="55"/>
+      <c r="AL25" s="55"/>
+      <c r="AM25" s="55"/>
+      <c r="AN25" s="55"/>
+      <c r="AO25" s="56"/>
       <c r="AP25" s="54"/>
       <c r="AQ25" s="55"/>
       <c r="AR25" s="55"/>
@@ -3909,18 +3810,18 @@
       <c r="AA26" s="4"/>
       <c r="AB26" s="4"/>
       <c r="AC26" s="5"/>
-      <c r="AD26" s="73"/>
-      <c r="AE26" s="74"/>
-      <c r="AF26" s="74"/>
-      <c r="AG26" s="74"/>
-      <c r="AH26" s="74"/>
-      <c r="AI26" s="75"/>
-      <c r="AJ26" s="73"/>
-      <c r="AK26" s="74"/>
-      <c r="AL26" s="74"/>
-      <c r="AM26" s="74"/>
-      <c r="AN26" s="74"/>
-      <c r="AO26" s="75"/>
+      <c r="AD26" s="6"/>
+      <c r="AE26" s="4"/>
+      <c r="AF26" s="4"/>
+      <c r="AG26" s="4"/>
+      <c r="AH26" s="4"/>
+      <c r="AI26" s="5"/>
+      <c r="AJ26" s="6"/>
+      <c r="AK26" s="4"/>
+      <c r="AL26" s="4"/>
+      <c r="AM26" s="4"/>
+      <c r="AN26" s="4"/>
+      <c r="AO26" s="5"/>
       <c r="AP26" s="6"/>
       <c r="AQ26" s="4"/>
       <c r="AR26" s="4"/>
@@ -3949,7 +3850,7 @@
     <row r="27" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A27" s="23"/>
       <c r="B27" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C27" s="63"/>
       <c r="D27" s="41">
@@ -3961,10 +3862,10 @@
         <v>1</v>
       </c>
       <c r="F27" s="48" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G27" s="49" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H27" s="49"/>
       <c r="I27" s="49"/>
@@ -3988,18 +3889,18 @@
       <c r="AA27" s="49"/>
       <c r="AB27" s="49"/>
       <c r="AC27" s="50"/>
-      <c r="AD27" s="73"/>
-      <c r="AE27" s="74"/>
-      <c r="AF27" s="74"/>
-      <c r="AG27" s="74"/>
-      <c r="AH27" s="74"/>
-      <c r="AI27" s="75"/>
-      <c r="AJ27" s="73"/>
-      <c r="AK27" s="74"/>
-      <c r="AL27" s="74"/>
-      <c r="AM27" s="74"/>
-      <c r="AN27" s="74"/>
-      <c r="AO27" s="75"/>
+      <c r="AD27" s="48"/>
+      <c r="AE27" s="49"/>
+      <c r="AF27" s="49"/>
+      <c r="AG27" s="49"/>
+      <c r="AH27" s="49"/>
+      <c r="AI27" s="50"/>
+      <c r="AJ27" s="48"/>
+      <c r="AK27" s="49"/>
+      <c r="AL27" s="49"/>
+      <c r="AM27" s="49"/>
+      <c r="AN27" s="49"/>
+      <c r="AO27" s="50"/>
       <c r="AP27" s="48"/>
       <c r="AQ27" s="49"/>
       <c r="AR27" s="49"/>
@@ -4028,7 +3929,7 @@
     <row r="28" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A28" s="23"/>
       <c r="B28" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C28" s="63"/>
       <c r="D28" s="41">
@@ -4040,10 +3941,10 @@
         <v>1</v>
       </c>
       <c r="F28" s="51" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G28" s="52" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H28" s="52"/>
       <c r="I28" s="52"/>
@@ -4067,18 +3968,18 @@
       <c r="AA28" s="52"/>
       <c r="AB28" s="52"/>
       <c r="AC28" s="53"/>
-      <c r="AD28" s="73"/>
-      <c r="AE28" s="74"/>
-      <c r="AF28" s="74"/>
-      <c r="AG28" s="74"/>
-      <c r="AH28" s="74"/>
-      <c r="AI28" s="75"/>
-      <c r="AJ28" s="73"/>
-      <c r="AK28" s="74"/>
-      <c r="AL28" s="74"/>
-      <c r="AM28" s="74"/>
-      <c r="AN28" s="74"/>
-      <c r="AO28" s="75"/>
+      <c r="AD28" s="51"/>
+      <c r="AE28" s="52"/>
+      <c r="AF28" s="52"/>
+      <c r="AG28" s="52"/>
+      <c r="AH28" s="52"/>
+      <c r="AI28" s="53"/>
+      <c r="AJ28" s="51"/>
+      <c r="AK28" s="52"/>
+      <c r="AL28" s="52"/>
+      <c r="AM28" s="52"/>
+      <c r="AN28" s="52"/>
+      <c r="AO28" s="53"/>
       <c r="AP28" s="51"/>
       <c r="AQ28" s="52"/>
       <c r="AR28" s="52"/>
@@ -4107,7 +4008,7 @@
     <row r="29" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A29" s="23"/>
       <c r="B29" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C29" s="63"/>
       <c r="D29" s="41">
@@ -4142,18 +4043,18 @@
       <c r="AA29" s="52"/>
       <c r="AB29" s="52"/>
       <c r="AC29" s="53"/>
-      <c r="AD29" s="73"/>
-      <c r="AE29" s="74"/>
-      <c r="AF29" s="74"/>
-      <c r="AG29" s="74"/>
-      <c r="AH29" s="74"/>
-      <c r="AI29" s="75"/>
-      <c r="AJ29" s="73"/>
-      <c r="AK29" s="74"/>
-      <c r="AL29" s="74"/>
-      <c r="AM29" s="74"/>
-      <c r="AN29" s="74"/>
-      <c r="AO29" s="75"/>
+      <c r="AD29" s="51"/>
+      <c r="AE29" s="52"/>
+      <c r="AF29" s="52"/>
+      <c r="AG29" s="52"/>
+      <c r="AH29" s="52"/>
+      <c r="AI29" s="53"/>
+      <c r="AJ29" s="51"/>
+      <c r="AK29" s="52"/>
+      <c r="AL29" s="52"/>
+      <c r="AM29" s="52"/>
+      <c r="AN29" s="52"/>
+      <c r="AO29" s="53"/>
       <c r="AP29" s="51"/>
       <c r="AQ29" s="52"/>
       <c r="AR29" s="52"/>
@@ -4215,18 +4116,18 @@
       <c r="AA30" s="52"/>
       <c r="AB30" s="52"/>
       <c r="AC30" s="53"/>
-      <c r="AD30" s="73"/>
-      <c r="AE30" s="74"/>
-      <c r="AF30" s="74"/>
-      <c r="AG30" s="74"/>
-      <c r="AH30" s="74"/>
-      <c r="AI30" s="75"/>
-      <c r="AJ30" s="73"/>
-      <c r="AK30" s="74"/>
-      <c r="AL30" s="74"/>
-      <c r="AM30" s="74"/>
-      <c r="AN30" s="74"/>
-      <c r="AO30" s="75"/>
+      <c r="AD30" s="51"/>
+      <c r="AE30" s="52"/>
+      <c r="AF30" s="52"/>
+      <c r="AG30" s="52"/>
+      <c r="AH30" s="52"/>
+      <c r="AI30" s="53"/>
+      <c r="AJ30" s="51"/>
+      <c r="AK30" s="52"/>
+      <c r="AL30" s="52"/>
+      <c r="AM30" s="52"/>
+      <c r="AN30" s="52"/>
+      <c r="AO30" s="53"/>
       <c r="AP30" s="51"/>
       <c r="AQ30" s="52"/>
       <c r="AR30" s="52"/>
@@ -4288,18 +4189,18 @@
       <c r="AA31" s="52"/>
       <c r="AB31" s="52"/>
       <c r="AC31" s="53"/>
-      <c r="AD31" s="73"/>
-      <c r="AE31" s="74"/>
-      <c r="AF31" s="74"/>
-      <c r="AG31" s="74"/>
-      <c r="AH31" s="74"/>
-      <c r="AI31" s="75"/>
-      <c r="AJ31" s="73"/>
-      <c r="AK31" s="74"/>
-      <c r="AL31" s="74"/>
-      <c r="AM31" s="74"/>
-      <c r="AN31" s="74"/>
-      <c r="AO31" s="75"/>
+      <c r="AD31" s="51"/>
+      <c r="AE31" s="52"/>
+      <c r="AF31" s="52"/>
+      <c r="AG31" s="52"/>
+      <c r="AH31" s="52"/>
+      <c r="AI31" s="53"/>
+      <c r="AJ31" s="51"/>
+      <c r="AK31" s="52"/>
+      <c r="AL31" s="52"/>
+      <c r="AM31" s="52"/>
+      <c r="AN31" s="52"/>
+      <c r="AO31" s="53"/>
       <c r="AP31" s="51"/>
       <c r="AQ31" s="52"/>
       <c r="AR31" s="52"/>
@@ -4361,18 +4262,18 @@
       <c r="AA32" s="52"/>
       <c r="AB32" s="52"/>
       <c r="AC32" s="53"/>
-      <c r="AD32" s="73"/>
-      <c r="AE32" s="74"/>
-      <c r="AF32" s="74"/>
-      <c r="AG32" s="74"/>
-      <c r="AH32" s="74"/>
-      <c r="AI32" s="75"/>
-      <c r="AJ32" s="73"/>
-      <c r="AK32" s="74"/>
-      <c r="AL32" s="74"/>
-      <c r="AM32" s="74"/>
-      <c r="AN32" s="74"/>
-      <c r="AO32" s="75"/>
+      <c r="AD32" s="51"/>
+      <c r="AE32" s="52"/>
+      <c r="AF32" s="52"/>
+      <c r="AG32" s="52"/>
+      <c r="AH32" s="52"/>
+      <c r="AI32" s="53"/>
+      <c r="AJ32" s="51"/>
+      <c r="AK32" s="52"/>
+      <c r="AL32" s="52"/>
+      <c r="AM32" s="52"/>
+      <c r="AN32" s="52"/>
+      <c r="AO32" s="53"/>
       <c r="AP32" s="51"/>
       <c r="AQ32" s="52"/>
       <c r="AR32" s="52"/>
@@ -4434,18 +4335,18 @@
       <c r="AA33" s="52"/>
       <c r="AB33" s="52"/>
       <c r="AC33" s="53"/>
-      <c r="AD33" s="73"/>
-      <c r="AE33" s="74"/>
-      <c r="AF33" s="74"/>
-      <c r="AG33" s="74"/>
-      <c r="AH33" s="74"/>
-      <c r="AI33" s="75"/>
-      <c r="AJ33" s="73"/>
-      <c r="AK33" s="74"/>
-      <c r="AL33" s="74"/>
-      <c r="AM33" s="74"/>
-      <c r="AN33" s="74"/>
-      <c r="AO33" s="75"/>
+      <c r="AD33" s="51"/>
+      <c r="AE33" s="52"/>
+      <c r="AF33" s="52"/>
+      <c r="AG33" s="52"/>
+      <c r="AH33" s="52"/>
+      <c r="AI33" s="53"/>
+      <c r="AJ33" s="51"/>
+      <c r="AK33" s="52"/>
+      <c r="AL33" s="52"/>
+      <c r="AM33" s="52"/>
+      <c r="AN33" s="52"/>
+      <c r="AO33" s="53"/>
       <c r="AP33" s="51"/>
       <c r="AQ33" s="52"/>
       <c r="AR33" s="52"/>
@@ -4507,18 +4408,18 @@
       <c r="AA34" s="52"/>
       <c r="AB34" s="52"/>
       <c r="AC34" s="53"/>
-      <c r="AD34" s="73"/>
-      <c r="AE34" s="74"/>
-      <c r="AF34" s="74"/>
-      <c r="AG34" s="74"/>
-      <c r="AH34" s="74"/>
-      <c r="AI34" s="75"/>
-      <c r="AJ34" s="73"/>
-      <c r="AK34" s="74"/>
-      <c r="AL34" s="74"/>
-      <c r="AM34" s="74"/>
-      <c r="AN34" s="74"/>
-      <c r="AO34" s="75"/>
+      <c r="AD34" s="51"/>
+      <c r="AE34" s="52"/>
+      <c r="AF34" s="52"/>
+      <c r="AG34" s="52"/>
+      <c r="AH34" s="52"/>
+      <c r="AI34" s="53"/>
+      <c r="AJ34" s="51"/>
+      <c r="AK34" s="52"/>
+      <c r="AL34" s="52"/>
+      <c r="AM34" s="52"/>
+      <c r="AN34" s="52"/>
+      <c r="AO34" s="53"/>
       <c r="AP34" s="51"/>
       <c r="AQ34" s="52"/>
       <c r="AR34" s="52"/>
@@ -4580,18 +4481,18 @@
       <c r="AA35" s="52"/>
       <c r="AB35" s="52"/>
       <c r="AC35" s="53"/>
-      <c r="AD35" s="73"/>
-      <c r="AE35" s="74"/>
-      <c r="AF35" s="74"/>
-      <c r="AG35" s="74"/>
-      <c r="AH35" s="74"/>
-      <c r="AI35" s="75"/>
-      <c r="AJ35" s="73"/>
-      <c r="AK35" s="74"/>
-      <c r="AL35" s="74"/>
-      <c r="AM35" s="74"/>
-      <c r="AN35" s="74"/>
-      <c r="AO35" s="75"/>
+      <c r="AD35" s="51"/>
+      <c r="AE35" s="52"/>
+      <c r="AF35" s="52"/>
+      <c r="AG35" s="52"/>
+      <c r="AH35" s="52"/>
+      <c r="AI35" s="53"/>
+      <c r="AJ35" s="51"/>
+      <c r="AK35" s="52"/>
+      <c r="AL35" s="52"/>
+      <c r="AM35" s="52"/>
+      <c r="AN35" s="52"/>
+      <c r="AO35" s="53"/>
       <c r="AP35" s="51"/>
       <c r="AQ35" s="52"/>
       <c r="AR35" s="52"/>
@@ -4653,18 +4554,18 @@
       <c r="AA36" s="55"/>
       <c r="AB36" s="55"/>
       <c r="AC36" s="56"/>
-      <c r="AD36" s="73"/>
-      <c r="AE36" s="74"/>
-      <c r="AF36" s="74"/>
-      <c r="AG36" s="74"/>
-      <c r="AH36" s="74"/>
-      <c r="AI36" s="75"/>
-      <c r="AJ36" s="73"/>
-      <c r="AK36" s="74"/>
-      <c r="AL36" s="74"/>
-      <c r="AM36" s="74"/>
-      <c r="AN36" s="74"/>
-      <c r="AO36" s="75"/>
+      <c r="AD36" s="54"/>
+      <c r="AE36" s="55"/>
+      <c r="AF36" s="55"/>
+      <c r="AG36" s="55"/>
+      <c r="AH36" s="55"/>
+      <c r="AI36" s="56"/>
+      <c r="AJ36" s="54"/>
+      <c r="AK36" s="55"/>
+      <c r="AL36" s="55"/>
+      <c r="AM36" s="55"/>
+      <c r="AN36" s="55"/>
+      <c r="AO36" s="56"/>
       <c r="AP36" s="54"/>
       <c r="AQ36" s="55"/>
       <c r="AR36" s="55"/>
@@ -4728,18 +4629,18 @@
       <c r="AA37" s="4"/>
       <c r="AB37" s="4"/>
       <c r="AC37" s="5"/>
-      <c r="AD37" s="73"/>
-      <c r="AE37" s="74"/>
-      <c r="AF37" s="74"/>
-      <c r="AG37" s="74"/>
-      <c r="AH37" s="74"/>
-      <c r="AI37" s="75"/>
-      <c r="AJ37" s="73"/>
-      <c r="AK37" s="74"/>
-      <c r="AL37" s="74"/>
-      <c r="AM37" s="74"/>
-      <c r="AN37" s="74"/>
-      <c r="AO37" s="75"/>
+      <c r="AD37" s="6"/>
+      <c r="AE37" s="4"/>
+      <c r="AF37" s="4"/>
+      <c r="AG37" s="4"/>
+      <c r="AH37" s="4"/>
+      <c r="AI37" s="5"/>
+      <c r="AJ37" s="6"/>
+      <c r="AK37" s="4"/>
+      <c r="AL37" s="4"/>
+      <c r="AM37" s="4"/>
+      <c r="AN37" s="4"/>
+      <c r="AO37" s="5"/>
       <c r="AP37" s="6"/>
       <c r="AQ37" s="4"/>
       <c r="AR37" s="4"/>
@@ -4768,10 +4669,10 @@
     <row r="38" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A38" s="31"/>
       <c r="B38" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C38" s="63" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D38" s="41">
         <f>IF($B38&gt;"",SUM(COUNTIF(F38:BM38,"P"))/2,"")</f>
@@ -4782,7 +4683,7 @@
         <v>0.5</v>
       </c>
       <c r="F38" s="48" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G38" s="49"/>
       <c r="H38" s="49"/>
@@ -4807,18 +4708,18 @@
       <c r="AA38" s="49"/>
       <c r="AB38" s="49"/>
       <c r="AC38" s="50"/>
-      <c r="AD38" s="73"/>
-      <c r="AE38" s="74"/>
-      <c r="AF38" s="74"/>
-      <c r="AG38" s="74"/>
-      <c r="AH38" s="74"/>
-      <c r="AI38" s="75"/>
-      <c r="AJ38" s="73"/>
-      <c r="AK38" s="74"/>
-      <c r="AL38" s="74"/>
-      <c r="AM38" s="74"/>
-      <c r="AN38" s="74"/>
-      <c r="AO38" s="75"/>
+      <c r="AD38" s="48"/>
+      <c r="AE38" s="49"/>
+      <c r="AF38" s="49"/>
+      <c r="AG38" s="49"/>
+      <c r="AH38" s="49"/>
+      <c r="AI38" s="50"/>
+      <c r="AJ38" s="48"/>
+      <c r="AK38" s="49"/>
+      <c r="AL38" s="49"/>
+      <c r="AM38" s="49"/>
+      <c r="AN38" s="49"/>
+      <c r="AO38" s="50"/>
       <c r="AP38" s="48"/>
       <c r="AQ38" s="49"/>
       <c r="AR38" s="49"/>
@@ -4847,10 +4748,10 @@
     <row r="39" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A39" s="31"/>
       <c r="B39" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C39" s="63" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D39" s="41">
         <f t="shared" ref="D39:D47" si="6">IF($B39&gt;"",SUM(COUNTIF(F39:BM39,"P"))/2,"")</f>
@@ -4872,7 +4773,7 @@
       <c r="O39" s="52"/>
       <c r="P39" s="52"/>
       <c r="Q39" s="53" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="R39" s="51"/>
       <c r="S39" s="52"/>
@@ -4880,30 +4781,30 @@
       <c r="U39" s="52"/>
       <c r="V39" s="52"/>
       <c r="W39" s="53"/>
-      <c r="X39" s="51" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y39" s="52" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z39" s="52" t="s">
-        <v>39</v>
-      </c>
+      <c r="X39" s="51"/>
+      <c r="Y39" s="52"/>
+      <c r="Z39" s="52"/>
       <c r="AA39" s="52"/>
       <c r="AB39" s="52"/>
       <c r="AC39" s="53"/>
-      <c r="AD39" s="73"/>
-      <c r="AE39" s="74"/>
-      <c r="AF39" s="74"/>
-      <c r="AG39" s="74"/>
-      <c r="AH39" s="74"/>
-      <c r="AI39" s="75"/>
-      <c r="AJ39" s="73"/>
-      <c r="AK39" s="74"/>
-      <c r="AL39" s="74"/>
-      <c r="AM39" s="74"/>
-      <c r="AN39" s="74"/>
-      <c r="AO39" s="75"/>
+      <c r="AD39" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE39" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF39" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG39" s="52"/>
+      <c r="AH39" s="52"/>
+      <c r="AI39" s="53"/>
+      <c r="AJ39" s="51"/>
+      <c r="AK39" s="52"/>
+      <c r="AL39" s="52"/>
+      <c r="AM39" s="52"/>
+      <c r="AN39" s="52"/>
+      <c r="AO39" s="53"/>
       <c r="AP39" s="51"/>
       <c r="AQ39" s="52"/>
       <c r="AR39" s="52"/>
@@ -4932,10 +4833,10 @@
     <row r="40" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A40" s="31"/>
       <c r="B40" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C40" s="63" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D40" s="41">
         <f t="shared" si="6"/>
@@ -4957,7 +4858,7 @@
       <c r="O40" s="52"/>
       <c r="P40" s="52"/>
       <c r="Q40" s="53" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="R40" s="51"/>
       <c r="S40" s="52"/>
@@ -4965,30 +4866,30 @@
       <c r="U40" s="52"/>
       <c r="V40" s="52"/>
       <c r="W40" s="53"/>
-      <c r="X40" s="51" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y40" s="52" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z40" s="52" t="s">
-        <v>39</v>
-      </c>
+      <c r="X40" s="51"/>
+      <c r="Y40" s="52"/>
+      <c r="Z40" s="52"/>
       <c r="AA40" s="52"/>
       <c r="AB40" s="52"/>
       <c r="AC40" s="53"/>
-      <c r="AD40" s="73"/>
-      <c r="AE40" s="74"/>
-      <c r="AF40" s="74"/>
-      <c r="AG40" s="74"/>
-      <c r="AH40" s="74"/>
-      <c r="AI40" s="75"/>
-      <c r="AJ40" s="73"/>
-      <c r="AK40" s="74"/>
-      <c r="AL40" s="74"/>
-      <c r="AM40" s="74"/>
-      <c r="AN40" s="74"/>
-      <c r="AO40" s="75"/>
+      <c r="AD40" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE40" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF40" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG40" s="52"/>
+      <c r="AH40" s="52"/>
+      <c r="AI40" s="53"/>
+      <c r="AJ40" s="51"/>
+      <c r="AK40" s="52"/>
+      <c r="AL40" s="52"/>
+      <c r="AM40" s="52"/>
+      <c r="AN40" s="52"/>
+      <c r="AO40" s="53"/>
       <c r="AP40" s="51"/>
       <c r="AQ40" s="52"/>
       <c r="AR40" s="52"/>
@@ -5017,10 +4918,10 @@
     <row r="41" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A41" s="23"/>
       <c r="B41" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C41" s="63" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D41" s="41">
         <f t="shared" si="6"/>
@@ -5042,7 +4943,7 @@
       <c r="O41" s="52"/>
       <c r="P41" s="52"/>
       <c r="Q41" s="53" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="R41" s="51"/>
       <c r="S41" s="52"/>
@@ -5050,30 +4951,30 @@
       <c r="U41" s="52"/>
       <c r="V41" s="52"/>
       <c r="W41" s="53"/>
-      <c r="X41" s="51" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y41" s="52" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z41" s="52" t="s">
-        <v>39</v>
-      </c>
+      <c r="X41" s="51"/>
+      <c r="Y41" s="52"/>
+      <c r="Z41" s="52"/>
       <c r="AA41" s="52"/>
       <c r="AB41" s="52"/>
       <c r="AC41" s="53"/>
-      <c r="AD41" s="73"/>
-      <c r="AE41" s="74"/>
-      <c r="AF41" s="74"/>
-      <c r="AG41" s="74"/>
-      <c r="AH41" s="74"/>
-      <c r="AI41" s="75"/>
-      <c r="AJ41" s="73"/>
-      <c r="AK41" s="74"/>
-      <c r="AL41" s="74"/>
-      <c r="AM41" s="74"/>
-      <c r="AN41" s="74"/>
-      <c r="AO41" s="75"/>
+      <c r="AD41" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE41" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF41" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG41" s="52"/>
+      <c r="AH41" s="52"/>
+      <c r="AI41" s="53"/>
+      <c r="AJ41" s="51"/>
+      <c r="AK41" s="52"/>
+      <c r="AL41" s="52"/>
+      <c r="AM41" s="52"/>
+      <c r="AN41" s="52"/>
+      <c r="AO41" s="53"/>
       <c r="AP41" s="51"/>
       <c r="AQ41" s="52"/>
       <c r="AR41" s="52"/>
@@ -5135,18 +5036,18 @@
       <c r="AA42" s="52"/>
       <c r="AB42" s="52"/>
       <c r="AC42" s="53"/>
-      <c r="AD42" s="73"/>
-      <c r="AE42" s="74"/>
-      <c r="AF42" s="74"/>
-      <c r="AG42" s="74"/>
-      <c r="AH42" s="74"/>
-      <c r="AI42" s="75"/>
-      <c r="AJ42" s="73"/>
-      <c r="AK42" s="74"/>
-      <c r="AL42" s="74"/>
-      <c r="AM42" s="74"/>
-      <c r="AN42" s="74"/>
-      <c r="AO42" s="75"/>
+      <c r="AD42" s="51"/>
+      <c r="AE42" s="52"/>
+      <c r="AF42" s="52"/>
+      <c r="AG42" s="52"/>
+      <c r="AH42" s="52"/>
+      <c r="AI42" s="53"/>
+      <c r="AJ42" s="51"/>
+      <c r="AK42" s="52"/>
+      <c r="AL42" s="52"/>
+      <c r="AM42" s="52"/>
+      <c r="AN42" s="52"/>
+      <c r="AO42" s="53"/>
       <c r="AP42" s="51"/>
       <c r="AQ42" s="52"/>
       <c r="AR42" s="52"/>
@@ -5208,18 +5109,18 @@
       <c r="AA43" s="52"/>
       <c r="AB43" s="52"/>
       <c r="AC43" s="53"/>
-      <c r="AD43" s="73"/>
-      <c r="AE43" s="74"/>
-      <c r="AF43" s="74"/>
-      <c r="AG43" s="74"/>
-      <c r="AH43" s="74"/>
-      <c r="AI43" s="75"/>
-      <c r="AJ43" s="73"/>
-      <c r="AK43" s="74"/>
-      <c r="AL43" s="74"/>
-      <c r="AM43" s="74"/>
-      <c r="AN43" s="74"/>
-      <c r="AO43" s="75"/>
+      <c r="AD43" s="51"/>
+      <c r="AE43" s="52"/>
+      <c r="AF43" s="52"/>
+      <c r="AG43" s="52"/>
+      <c r="AH43" s="52"/>
+      <c r="AI43" s="53"/>
+      <c r="AJ43" s="51"/>
+      <c r="AK43" s="52"/>
+      <c r="AL43" s="52"/>
+      <c r="AM43" s="52"/>
+      <c r="AN43" s="52"/>
+      <c r="AO43" s="53"/>
       <c r="AP43" s="51"/>
       <c r="AQ43" s="52"/>
       <c r="AR43" s="52"/>
@@ -5281,18 +5182,18 @@
       <c r="AA44" s="52"/>
       <c r="AB44" s="52"/>
       <c r="AC44" s="53"/>
-      <c r="AD44" s="73"/>
-      <c r="AE44" s="74"/>
-      <c r="AF44" s="74"/>
-      <c r="AG44" s="74"/>
-      <c r="AH44" s="74"/>
-      <c r="AI44" s="75"/>
-      <c r="AJ44" s="73"/>
-      <c r="AK44" s="74"/>
-      <c r="AL44" s="74"/>
-      <c r="AM44" s="74"/>
-      <c r="AN44" s="74"/>
-      <c r="AO44" s="75"/>
+      <c r="AD44" s="51"/>
+      <c r="AE44" s="52"/>
+      <c r="AF44" s="52"/>
+      <c r="AG44" s="52"/>
+      <c r="AH44" s="52"/>
+      <c r="AI44" s="53"/>
+      <c r="AJ44" s="51"/>
+      <c r="AK44" s="52"/>
+      <c r="AL44" s="52"/>
+      <c r="AM44" s="52"/>
+      <c r="AN44" s="52"/>
+      <c r="AO44" s="53"/>
       <c r="AP44" s="51"/>
       <c r="AQ44" s="52"/>
       <c r="AR44" s="52"/>
@@ -5354,18 +5255,18 @@
       <c r="AA45" s="52"/>
       <c r="AB45" s="52"/>
       <c r="AC45" s="53"/>
-      <c r="AD45" s="73"/>
-      <c r="AE45" s="74"/>
-      <c r="AF45" s="74"/>
-      <c r="AG45" s="74"/>
-      <c r="AH45" s="74"/>
-      <c r="AI45" s="75"/>
-      <c r="AJ45" s="73"/>
-      <c r="AK45" s="74"/>
-      <c r="AL45" s="74"/>
-      <c r="AM45" s="74"/>
-      <c r="AN45" s="74"/>
-      <c r="AO45" s="75"/>
+      <c r="AD45" s="51"/>
+      <c r="AE45" s="52"/>
+      <c r="AF45" s="52"/>
+      <c r="AG45" s="52"/>
+      <c r="AH45" s="52"/>
+      <c r="AI45" s="53"/>
+      <c r="AJ45" s="51"/>
+      <c r="AK45" s="52"/>
+      <c r="AL45" s="52"/>
+      <c r="AM45" s="52"/>
+      <c r="AN45" s="52"/>
+      <c r="AO45" s="53"/>
       <c r="AP45" s="51"/>
       <c r="AQ45" s="52"/>
       <c r="AR45" s="52"/>
@@ -5427,18 +5328,18 @@
       <c r="AA46" s="52"/>
       <c r="AB46" s="52"/>
       <c r="AC46" s="53"/>
-      <c r="AD46" s="73"/>
-      <c r="AE46" s="74"/>
-      <c r="AF46" s="74"/>
-      <c r="AG46" s="74"/>
-      <c r="AH46" s="74"/>
-      <c r="AI46" s="75"/>
-      <c r="AJ46" s="73"/>
-      <c r="AK46" s="74"/>
-      <c r="AL46" s="74"/>
-      <c r="AM46" s="74"/>
-      <c r="AN46" s="74"/>
-      <c r="AO46" s="75"/>
+      <c r="AD46" s="51"/>
+      <c r="AE46" s="52"/>
+      <c r="AF46" s="52"/>
+      <c r="AG46" s="52"/>
+      <c r="AH46" s="52"/>
+      <c r="AI46" s="53"/>
+      <c r="AJ46" s="51"/>
+      <c r="AK46" s="52"/>
+      <c r="AL46" s="52"/>
+      <c r="AM46" s="52"/>
+      <c r="AN46" s="52"/>
+      <c r="AO46" s="53"/>
       <c r="AP46" s="51"/>
       <c r="AQ46" s="52"/>
       <c r="AR46" s="52"/>
@@ -5500,18 +5401,18 @@
       <c r="AA47" s="55"/>
       <c r="AB47" s="55"/>
       <c r="AC47" s="56"/>
-      <c r="AD47" s="73"/>
-      <c r="AE47" s="74"/>
-      <c r="AF47" s="74"/>
-      <c r="AG47" s="74"/>
-      <c r="AH47" s="74"/>
-      <c r="AI47" s="75"/>
-      <c r="AJ47" s="73"/>
-      <c r="AK47" s="74"/>
-      <c r="AL47" s="74"/>
-      <c r="AM47" s="74"/>
-      <c r="AN47" s="74"/>
-      <c r="AO47" s="75"/>
+      <c r="AD47" s="54"/>
+      <c r="AE47" s="55"/>
+      <c r="AF47" s="55"/>
+      <c r="AG47" s="55"/>
+      <c r="AH47" s="55"/>
+      <c r="AI47" s="56"/>
+      <c r="AJ47" s="54"/>
+      <c r="AK47" s="55"/>
+      <c r="AL47" s="55"/>
+      <c r="AM47" s="55"/>
+      <c r="AN47" s="55"/>
+      <c r="AO47" s="56"/>
       <c r="AP47" s="54"/>
       <c r="AQ47" s="55"/>
       <c r="AR47" s="55"/>
@@ -5575,18 +5476,18 @@
       <c r="AA48" s="4"/>
       <c r="AB48" s="4"/>
       <c r="AC48" s="5"/>
-      <c r="AD48" s="73"/>
-      <c r="AE48" s="74"/>
-      <c r="AF48" s="74"/>
-      <c r="AG48" s="74"/>
-      <c r="AH48" s="74"/>
-      <c r="AI48" s="75"/>
-      <c r="AJ48" s="73"/>
-      <c r="AK48" s="74"/>
-      <c r="AL48" s="74"/>
-      <c r="AM48" s="74"/>
-      <c r="AN48" s="74"/>
-      <c r="AO48" s="75"/>
+      <c r="AD48" s="6"/>
+      <c r="AE48" s="4"/>
+      <c r="AF48" s="4"/>
+      <c r="AG48" s="4"/>
+      <c r="AH48" s="4"/>
+      <c r="AI48" s="5"/>
+      <c r="AJ48" s="6"/>
+      <c r="AK48" s="4"/>
+      <c r="AL48" s="4"/>
+      <c r="AM48" s="4"/>
+      <c r="AN48" s="4"/>
+      <c r="AO48" s="5"/>
       <c r="AP48" s="6"/>
       <c r="AQ48" s="4"/>
       <c r="AR48" s="4"/>
@@ -5615,7 +5516,7 @@
     <row r="49" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A49" s="23"/>
       <c r="B49" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C49" s="63"/>
       <c r="D49" s="41">
@@ -5650,18 +5551,18 @@
       <c r="AA49" s="49"/>
       <c r="AB49" s="49"/>
       <c r="AC49" s="50"/>
-      <c r="AD49" s="73"/>
-      <c r="AE49" s="74"/>
-      <c r="AF49" s="74"/>
-      <c r="AG49" s="74"/>
-      <c r="AH49" s="74"/>
-      <c r="AI49" s="75"/>
-      <c r="AJ49" s="73"/>
-      <c r="AK49" s="74"/>
-      <c r="AL49" s="74"/>
-      <c r="AM49" s="74"/>
-      <c r="AN49" s="74"/>
-      <c r="AO49" s="75"/>
+      <c r="AD49" s="48"/>
+      <c r="AE49" s="49"/>
+      <c r="AF49" s="49"/>
+      <c r="AG49" s="49"/>
+      <c r="AH49" s="49"/>
+      <c r="AI49" s="50"/>
+      <c r="AJ49" s="48"/>
+      <c r="AK49" s="49"/>
+      <c r="AL49" s="49"/>
+      <c r="AM49" s="49"/>
+      <c r="AN49" s="49"/>
+      <c r="AO49" s="50"/>
       <c r="AP49" s="48"/>
       <c r="AQ49" s="49"/>
       <c r="AR49" s="49"/>
@@ -5690,7 +5591,7 @@
     <row r="50" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A50" s="23"/>
       <c r="B50" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C50" s="63"/>
       <c r="D50" s="41">
@@ -5725,18 +5626,18 @@
       <c r="AA50" s="52"/>
       <c r="AB50" s="52"/>
       <c r="AC50" s="53"/>
-      <c r="AD50" s="73"/>
-      <c r="AE50" s="74"/>
-      <c r="AF50" s="74"/>
-      <c r="AG50" s="74"/>
-      <c r="AH50" s="74"/>
-      <c r="AI50" s="75"/>
-      <c r="AJ50" s="73"/>
-      <c r="AK50" s="74"/>
-      <c r="AL50" s="74"/>
-      <c r="AM50" s="74"/>
-      <c r="AN50" s="74"/>
-      <c r="AO50" s="75"/>
+      <c r="AD50" s="51"/>
+      <c r="AE50" s="52"/>
+      <c r="AF50" s="52"/>
+      <c r="AG50" s="52"/>
+      <c r="AH50" s="52"/>
+      <c r="AI50" s="53"/>
+      <c r="AJ50" s="51"/>
+      <c r="AK50" s="52"/>
+      <c r="AL50" s="52"/>
+      <c r="AM50" s="52"/>
+      <c r="AN50" s="52"/>
+      <c r="AO50" s="53"/>
       <c r="AP50" s="51"/>
       <c r="AQ50" s="52"/>
       <c r="AR50" s="52"/>
@@ -5798,18 +5699,18 @@
       <c r="AA51" s="52"/>
       <c r="AB51" s="52"/>
       <c r="AC51" s="53"/>
-      <c r="AD51" s="73"/>
-      <c r="AE51" s="74"/>
-      <c r="AF51" s="74"/>
-      <c r="AG51" s="74"/>
-      <c r="AH51" s="74"/>
-      <c r="AI51" s="75"/>
-      <c r="AJ51" s="73"/>
-      <c r="AK51" s="74"/>
-      <c r="AL51" s="74"/>
-      <c r="AM51" s="74"/>
-      <c r="AN51" s="74"/>
-      <c r="AO51" s="75"/>
+      <c r="AD51" s="51"/>
+      <c r="AE51" s="52"/>
+      <c r="AF51" s="52"/>
+      <c r="AG51" s="52"/>
+      <c r="AH51" s="52"/>
+      <c r="AI51" s="53"/>
+      <c r="AJ51" s="51"/>
+      <c r="AK51" s="52"/>
+      <c r="AL51" s="52"/>
+      <c r="AM51" s="52"/>
+      <c r="AN51" s="52"/>
+      <c r="AO51" s="53"/>
       <c r="AP51" s="51"/>
       <c r="AQ51" s="52"/>
       <c r="AR51" s="52"/>
@@ -5871,18 +5772,18 @@
       <c r="AA52" s="52"/>
       <c r="AB52" s="52"/>
       <c r="AC52" s="53"/>
-      <c r="AD52" s="73"/>
-      <c r="AE52" s="74"/>
-      <c r="AF52" s="74"/>
-      <c r="AG52" s="74"/>
-      <c r="AH52" s="74"/>
-      <c r="AI52" s="75"/>
-      <c r="AJ52" s="73"/>
-      <c r="AK52" s="74"/>
-      <c r="AL52" s="74"/>
-      <c r="AM52" s="74"/>
-      <c r="AN52" s="74"/>
-      <c r="AO52" s="75"/>
+      <c r="AD52" s="51"/>
+      <c r="AE52" s="52"/>
+      <c r="AF52" s="52"/>
+      <c r="AG52" s="52"/>
+      <c r="AH52" s="52"/>
+      <c r="AI52" s="53"/>
+      <c r="AJ52" s="51"/>
+      <c r="AK52" s="52"/>
+      <c r="AL52" s="52"/>
+      <c r="AM52" s="52"/>
+      <c r="AN52" s="52"/>
+      <c r="AO52" s="53"/>
       <c r="AP52" s="51"/>
       <c r="AQ52" s="52"/>
       <c r="AR52" s="52"/>
@@ -5944,18 +5845,18 @@
       <c r="AA53" s="52"/>
       <c r="AB53" s="52"/>
       <c r="AC53" s="53"/>
-      <c r="AD53" s="73"/>
-      <c r="AE53" s="74"/>
-      <c r="AF53" s="74"/>
-      <c r="AG53" s="74"/>
-      <c r="AH53" s="74"/>
-      <c r="AI53" s="75"/>
-      <c r="AJ53" s="73"/>
-      <c r="AK53" s="74"/>
-      <c r="AL53" s="74"/>
-      <c r="AM53" s="74"/>
-      <c r="AN53" s="74"/>
-      <c r="AO53" s="75"/>
+      <c r="AD53" s="51"/>
+      <c r="AE53" s="52"/>
+      <c r="AF53" s="52"/>
+      <c r="AG53" s="52"/>
+      <c r="AH53" s="52"/>
+      <c r="AI53" s="53"/>
+      <c r="AJ53" s="51"/>
+      <c r="AK53" s="52"/>
+      <c r="AL53" s="52"/>
+      <c r="AM53" s="52"/>
+      <c r="AN53" s="52"/>
+      <c r="AO53" s="53"/>
       <c r="AP53" s="51"/>
       <c r="AQ53" s="52"/>
       <c r="AR53" s="52"/>
@@ -6017,18 +5918,18 @@
       <c r="AA54" s="52"/>
       <c r="AB54" s="52"/>
       <c r="AC54" s="53"/>
-      <c r="AD54" s="73"/>
-      <c r="AE54" s="74"/>
-      <c r="AF54" s="74"/>
-      <c r="AG54" s="74"/>
-      <c r="AH54" s="74"/>
-      <c r="AI54" s="75"/>
-      <c r="AJ54" s="73"/>
-      <c r="AK54" s="74"/>
-      <c r="AL54" s="74"/>
-      <c r="AM54" s="74"/>
-      <c r="AN54" s="74"/>
-      <c r="AO54" s="75"/>
+      <c r="AD54" s="51"/>
+      <c r="AE54" s="52"/>
+      <c r="AF54" s="52"/>
+      <c r="AG54" s="52"/>
+      <c r="AH54" s="52"/>
+      <c r="AI54" s="53"/>
+      <c r="AJ54" s="51"/>
+      <c r="AK54" s="52"/>
+      <c r="AL54" s="52"/>
+      <c r="AM54" s="52"/>
+      <c r="AN54" s="52"/>
+      <c r="AO54" s="53"/>
       <c r="AP54" s="51"/>
       <c r="AQ54" s="52"/>
       <c r="AR54" s="52"/>
@@ -6090,18 +5991,18 @@
       <c r="AA55" s="52"/>
       <c r="AB55" s="52"/>
       <c r="AC55" s="53"/>
-      <c r="AD55" s="73"/>
-      <c r="AE55" s="74"/>
-      <c r="AF55" s="74"/>
-      <c r="AG55" s="74"/>
-      <c r="AH55" s="74"/>
-      <c r="AI55" s="75"/>
-      <c r="AJ55" s="73"/>
-      <c r="AK55" s="74"/>
-      <c r="AL55" s="74"/>
-      <c r="AM55" s="74"/>
-      <c r="AN55" s="74"/>
-      <c r="AO55" s="75"/>
+      <c r="AD55" s="51"/>
+      <c r="AE55" s="52"/>
+      <c r="AF55" s="52"/>
+      <c r="AG55" s="52"/>
+      <c r="AH55" s="52"/>
+      <c r="AI55" s="53"/>
+      <c r="AJ55" s="51"/>
+      <c r="AK55" s="52"/>
+      <c r="AL55" s="52"/>
+      <c r="AM55" s="52"/>
+      <c r="AN55" s="52"/>
+      <c r="AO55" s="53"/>
       <c r="AP55" s="51"/>
       <c r="AQ55" s="52"/>
       <c r="AR55" s="52"/>
@@ -6163,18 +6064,18 @@
       <c r="AA56" s="52"/>
       <c r="AB56" s="52"/>
       <c r="AC56" s="53"/>
-      <c r="AD56" s="73"/>
-      <c r="AE56" s="74"/>
-      <c r="AF56" s="74"/>
-      <c r="AG56" s="74"/>
-      <c r="AH56" s="74"/>
-      <c r="AI56" s="75"/>
-      <c r="AJ56" s="73"/>
-      <c r="AK56" s="74"/>
-      <c r="AL56" s="74"/>
-      <c r="AM56" s="74"/>
-      <c r="AN56" s="74"/>
-      <c r="AO56" s="75"/>
+      <c r="AD56" s="51"/>
+      <c r="AE56" s="52"/>
+      <c r="AF56" s="52"/>
+      <c r="AG56" s="52"/>
+      <c r="AH56" s="52"/>
+      <c r="AI56" s="53"/>
+      <c r="AJ56" s="51"/>
+      <c r="AK56" s="52"/>
+      <c r="AL56" s="52"/>
+      <c r="AM56" s="52"/>
+      <c r="AN56" s="52"/>
+      <c r="AO56" s="53"/>
       <c r="AP56" s="51"/>
       <c r="AQ56" s="52"/>
       <c r="AR56" s="52"/>
@@ -6236,18 +6137,18 @@
       <c r="AA57" s="52"/>
       <c r="AB57" s="52"/>
       <c r="AC57" s="53"/>
-      <c r="AD57" s="73"/>
-      <c r="AE57" s="74"/>
-      <c r="AF57" s="74"/>
-      <c r="AG57" s="74"/>
-      <c r="AH57" s="74"/>
-      <c r="AI57" s="75"/>
-      <c r="AJ57" s="73"/>
-      <c r="AK57" s="74"/>
-      <c r="AL57" s="74"/>
-      <c r="AM57" s="74"/>
-      <c r="AN57" s="74"/>
-      <c r="AO57" s="75"/>
+      <c r="AD57" s="51"/>
+      <c r="AE57" s="52"/>
+      <c r="AF57" s="52"/>
+      <c r="AG57" s="52"/>
+      <c r="AH57" s="52"/>
+      <c r="AI57" s="53"/>
+      <c r="AJ57" s="51"/>
+      <c r="AK57" s="52"/>
+      <c r="AL57" s="52"/>
+      <c r="AM57" s="52"/>
+      <c r="AN57" s="52"/>
+      <c r="AO57" s="53"/>
       <c r="AP57" s="51"/>
       <c r="AQ57" s="52"/>
       <c r="AR57" s="52"/>
@@ -6309,18 +6210,18 @@
       <c r="AA58" s="55"/>
       <c r="AB58" s="55"/>
       <c r="AC58" s="56"/>
-      <c r="AD58" s="73"/>
-      <c r="AE58" s="74"/>
-      <c r="AF58" s="74"/>
-      <c r="AG58" s="74"/>
-      <c r="AH58" s="74"/>
-      <c r="AI58" s="75"/>
-      <c r="AJ58" s="73"/>
-      <c r="AK58" s="74"/>
-      <c r="AL58" s="74"/>
-      <c r="AM58" s="74"/>
-      <c r="AN58" s="74"/>
-      <c r="AO58" s="75"/>
+      <c r="AD58" s="54"/>
+      <c r="AE58" s="55"/>
+      <c r="AF58" s="55"/>
+      <c r="AG58" s="55"/>
+      <c r="AH58" s="55"/>
+      <c r="AI58" s="56"/>
+      <c r="AJ58" s="54"/>
+      <c r="AK58" s="55"/>
+      <c r="AL58" s="55"/>
+      <c r="AM58" s="55"/>
+      <c r="AN58" s="55"/>
+      <c r="AO58" s="56"/>
       <c r="AP58" s="54"/>
       <c r="AQ58" s="55"/>
       <c r="AR58" s="55"/>
@@ -6384,18 +6285,18 @@
       <c r="AA59" s="4"/>
       <c r="AB59" s="4"/>
       <c r="AC59" s="5"/>
-      <c r="AD59" s="73"/>
-      <c r="AE59" s="74"/>
-      <c r="AF59" s="74"/>
-      <c r="AG59" s="74"/>
-      <c r="AH59" s="74"/>
-      <c r="AI59" s="75"/>
-      <c r="AJ59" s="73"/>
-      <c r="AK59" s="74"/>
-      <c r="AL59" s="74"/>
-      <c r="AM59" s="74"/>
-      <c r="AN59" s="74"/>
-      <c r="AO59" s="75"/>
+      <c r="AD59" s="6"/>
+      <c r="AE59" s="4"/>
+      <c r="AF59" s="4"/>
+      <c r="AG59" s="4"/>
+      <c r="AH59" s="4"/>
+      <c r="AI59" s="5"/>
+      <c r="AJ59" s="6"/>
+      <c r="AK59" s="4"/>
+      <c r="AL59" s="4"/>
+      <c r="AM59" s="4"/>
+      <c r="AN59" s="4"/>
+      <c r="AO59" s="5"/>
       <c r="AP59" s="6"/>
       <c r="AQ59" s="4"/>
       <c r="AR59" s="4"/>
@@ -6424,10 +6325,10 @@
     <row r="60" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A60" s="23"/>
       <c r="B60" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C60" s="63" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D60" s="41">
         <f>IF($B60&gt;"",SUM(COUNTIF(F60:BM60,"P"))/2,"")</f>
@@ -6461,18 +6362,18 @@
       <c r="AA60" s="49"/>
       <c r="AB60" s="49"/>
       <c r="AC60" s="50"/>
-      <c r="AD60" s="73"/>
-      <c r="AE60" s="74"/>
-      <c r="AF60" s="74"/>
-      <c r="AG60" s="74"/>
-      <c r="AH60" s="74"/>
-      <c r="AI60" s="75"/>
-      <c r="AJ60" s="73"/>
-      <c r="AK60" s="74"/>
-      <c r="AL60" s="74"/>
-      <c r="AM60" s="74"/>
-      <c r="AN60" s="74"/>
-      <c r="AO60" s="75"/>
+      <c r="AD60" s="48"/>
+      <c r="AE60" s="49"/>
+      <c r="AF60" s="49"/>
+      <c r="AG60" s="49"/>
+      <c r="AH60" s="49"/>
+      <c r="AI60" s="50"/>
+      <c r="AJ60" s="48"/>
+      <c r="AK60" s="49"/>
+      <c r="AL60" s="49"/>
+      <c r="AM60" s="49"/>
+      <c r="AN60" s="49"/>
+      <c r="AO60" s="50"/>
       <c r="AP60" s="48"/>
       <c r="AQ60" s="49"/>
       <c r="AR60" s="49"/>
@@ -6534,18 +6435,18 @@
       <c r="AA61" s="52"/>
       <c r="AB61" s="52"/>
       <c r="AC61" s="53"/>
-      <c r="AD61" s="73"/>
-      <c r="AE61" s="74"/>
-      <c r="AF61" s="74"/>
-      <c r="AG61" s="74"/>
-      <c r="AH61" s="74"/>
-      <c r="AI61" s="75"/>
-      <c r="AJ61" s="73"/>
-      <c r="AK61" s="74"/>
-      <c r="AL61" s="74"/>
-      <c r="AM61" s="74"/>
-      <c r="AN61" s="74"/>
-      <c r="AO61" s="75"/>
+      <c r="AD61" s="51"/>
+      <c r="AE61" s="52"/>
+      <c r="AF61" s="52"/>
+      <c r="AG61" s="52"/>
+      <c r="AH61" s="52"/>
+      <c r="AI61" s="53"/>
+      <c r="AJ61" s="51"/>
+      <c r="AK61" s="52"/>
+      <c r="AL61" s="52"/>
+      <c r="AM61" s="52"/>
+      <c r="AN61" s="52"/>
+      <c r="AO61" s="53"/>
       <c r="AP61" s="51"/>
       <c r="AQ61" s="52"/>
       <c r="AR61" s="52"/>
@@ -6607,18 +6508,18 @@
       <c r="AA62" s="52"/>
       <c r="AB62" s="52"/>
       <c r="AC62" s="53"/>
-      <c r="AD62" s="73"/>
-      <c r="AE62" s="74"/>
-      <c r="AF62" s="74"/>
-      <c r="AG62" s="74"/>
-      <c r="AH62" s="74"/>
-      <c r="AI62" s="75"/>
-      <c r="AJ62" s="73"/>
-      <c r="AK62" s="74"/>
-      <c r="AL62" s="74"/>
-      <c r="AM62" s="74"/>
-      <c r="AN62" s="74"/>
-      <c r="AO62" s="75"/>
+      <c r="AD62" s="51"/>
+      <c r="AE62" s="52"/>
+      <c r="AF62" s="52"/>
+      <c r="AG62" s="52"/>
+      <c r="AH62" s="52"/>
+      <c r="AI62" s="53"/>
+      <c r="AJ62" s="51"/>
+      <c r="AK62" s="52"/>
+      <c r="AL62" s="52"/>
+      <c r="AM62" s="52"/>
+      <c r="AN62" s="52"/>
+      <c r="AO62" s="53"/>
       <c r="AP62" s="51"/>
       <c r="AQ62" s="52"/>
       <c r="AR62" s="52"/>
@@ -6680,18 +6581,18 @@
       <c r="AA63" s="52"/>
       <c r="AB63" s="52"/>
       <c r="AC63" s="53"/>
-      <c r="AD63" s="73"/>
-      <c r="AE63" s="74"/>
-      <c r="AF63" s="74"/>
-      <c r="AG63" s="74"/>
-      <c r="AH63" s="74"/>
-      <c r="AI63" s="75"/>
-      <c r="AJ63" s="73"/>
-      <c r="AK63" s="74"/>
-      <c r="AL63" s="74"/>
-      <c r="AM63" s="74"/>
-      <c r="AN63" s="74"/>
-      <c r="AO63" s="75"/>
+      <c r="AD63" s="51"/>
+      <c r="AE63" s="52"/>
+      <c r="AF63" s="52"/>
+      <c r="AG63" s="52"/>
+      <c r="AH63" s="52"/>
+      <c r="AI63" s="53"/>
+      <c r="AJ63" s="51"/>
+      <c r="AK63" s="52"/>
+      <c r="AL63" s="52"/>
+      <c r="AM63" s="52"/>
+      <c r="AN63" s="52"/>
+      <c r="AO63" s="53"/>
       <c r="AP63" s="51"/>
       <c r="AQ63" s="52"/>
       <c r="AR63" s="52"/>
@@ -6753,18 +6654,18 @@
       <c r="AA64" s="52"/>
       <c r="AB64" s="52"/>
       <c r="AC64" s="53"/>
-      <c r="AD64" s="73"/>
-      <c r="AE64" s="74"/>
-      <c r="AF64" s="74"/>
-      <c r="AG64" s="74"/>
-      <c r="AH64" s="74"/>
-      <c r="AI64" s="75"/>
-      <c r="AJ64" s="73"/>
-      <c r="AK64" s="74"/>
-      <c r="AL64" s="74"/>
-      <c r="AM64" s="74"/>
-      <c r="AN64" s="74"/>
-      <c r="AO64" s="75"/>
+      <c r="AD64" s="51"/>
+      <c r="AE64" s="52"/>
+      <c r="AF64" s="52"/>
+      <c r="AG64" s="52"/>
+      <c r="AH64" s="52"/>
+      <c r="AI64" s="53"/>
+      <c r="AJ64" s="51"/>
+      <c r="AK64" s="52"/>
+      <c r="AL64" s="52"/>
+      <c r="AM64" s="52"/>
+      <c r="AN64" s="52"/>
+      <c r="AO64" s="53"/>
       <c r="AP64" s="51"/>
       <c r="AQ64" s="52"/>
       <c r="AR64" s="52"/>
@@ -6826,18 +6727,18 @@
       <c r="AA65" s="52"/>
       <c r="AB65" s="52"/>
       <c r="AC65" s="53"/>
-      <c r="AD65" s="73"/>
-      <c r="AE65" s="74"/>
-      <c r="AF65" s="74"/>
-      <c r="AG65" s="74"/>
-      <c r="AH65" s="74"/>
-      <c r="AI65" s="75"/>
-      <c r="AJ65" s="73"/>
-      <c r="AK65" s="74"/>
-      <c r="AL65" s="74"/>
-      <c r="AM65" s="74"/>
-      <c r="AN65" s="74"/>
-      <c r="AO65" s="75"/>
+      <c r="AD65" s="51"/>
+      <c r="AE65" s="52"/>
+      <c r="AF65" s="52"/>
+      <c r="AG65" s="52"/>
+      <c r="AH65" s="52"/>
+      <c r="AI65" s="53"/>
+      <c r="AJ65" s="51"/>
+      <c r="AK65" s="52"/>
+      <c r="AL65" s="52"/>
+      <c r="AM65" s="52"/>
+      <c r="AN65" s="52"/>
+      <c r="AO65" s="53"/>
       <c r="AP65" s="51"/>
       <c r="AQ65" s="52"/>
       <c r="AR65" s="52"/>
@@ -6899,18 +6800,18 @@
       <c r="AA66" s="52"/>
       <c r="AB66" s="52"/>
       <c r="AC66" s="53"/>
-      <c r="AD66" s="73"/>
-      <c r="AE66" s="74"/>
-      <c r="AF66" s="74"/>
-      <c r="AG66" s="74"/>
-      <c r="AH66" s="74"/>
-      <c r="AI66" s="75"/>
-      <c r="AJ66" s="73"/>
-      <c r="AK66" s="74"/>
-      <c r="AL66" s="74"/>
-      <c r="AM66" s="74"/>
-      <c r="AN66" s="74"/>
-      <c r="AO66" s="75"/>
+      <c r="AD66" s="51"/>
+      <c r="AE66" s="52"/>
+      <c r="AF66" s="52"/>
+      <c r="AG66" s="52"/>
+      <c r="AH66" s="52"/>
+      <c r="AI66" s="53"/>
+      <c r="AJ66" s="51"/>
+      <c r="AK66" s="52"/>
+      <c r="AL66" s="52"/>
+      <c r="AM66" s="52"/>
+      <c r="AN66" s="52"/>
+      <c r="AO66" s="53"/>
       <c r="AP66" s="51"/>
       <c r="AQ66" s="52"/>
       <c r="AR66" s="52"/>
@@ -6972,18 +6873,18 @@
       <c r="AA67" s="52"/>
       <c r="AB67" s="52"/>
       <c r="AC67" s="53"/>
-      <c r="AD67" s="73"/>
-      <c r="AE67" s="74"/>
-      <c r="AF67" s="74"/>
-      <c r="AG67" s="74"/>
-      <c r="AH67" s="74"/>
-      <c r="AI67" s="75"/>
-      <c r="AJ67" s="73"/>
-      <c r="AK67" s="74"/>
-      <c r="AL67" s="74"/>
-      <c r="AM67" s="74"/>
-      <c r="AN67" s="74"/>
-      <c r="AO67" s="75"/>
+      <c r="AD67" s="51"/>
+      <c r="AE67" s="52"/>
+      <c r="AF67" s="52"/>
+      <c r="AG67" s="52"/>
+      <c r="AH67" s="52"/>
+      <c r="AI67" s="53"/>
+      <c r="AJ67" s="51"/>
+      <c r="AK67" s="52"/>
+      <c r="AL67" s="52"/>
+      <c r="AM67" s="52"/>
+      <c r="AN67" s="52"/>
+      <c r="AO67" s="53"/>
       <c r="AP67" s="51"/>
       <c r="AQ67" s="52"/>
       <c r="AR67" s="52"/>
@@ -7045,18 +6946,18 @@
       <c r="AA68" s="52"/>
       <c r="AB68" s="52"/>
       <c r="AC68" s="53"/>
-      <c r="AD68" s="73"/>
-      <c r="AE68" s="74"/>
-      <c r="AF68" s="74"/>
-      <c r="AG68" s="74"/>
-      <c r="AH68" s="74"/>
-      <c r="AI68" s="75"/>
-      <c r="AJ68" s="73"/>
-      <c r="AK68" s="74"/>
-      <c r="AL68" s="74"/>
-      <c r="AM68" s="74"/>
-      <c r="AN68" s="74"/>
-      <c r="AO68" s="75"/>
+      <c r="AD68" s="51"/>
+      <c r="AE68" s="52"/>
+      <c r="AF68" s="52"/>
+      <c r="AG68" s="52"/>
+      <c r="AH68" s="52"/>
+      <c r="AI68" s="53"/>
+      <c r="AJ68" s="51"/>
+      <c r="AK68" s="52"/>
+      <c r="AL68" s="52"/>
+      <c r="AM68" s="52"/>
+      <c r="AN68" s="52"/>
+      <c r="AO68" s="53"/>
       <c r="AP68" s="51"/>
       <c r="AQ68" s="52"/>
       <c r="AR68" s="52"/>
@@ -7118,18 +7019,18 @@
       <c r="AA69" s="55"/>
       <c r="AB69" s="55"/>
       <c r="AC69" s="56"/>
-      <c r="AD69" s="76"/>
-      <c r="AE69" s="77"/>
-      <c r="AF69" s="77"/>
-      <c r="AG69" s="77"/>
-      <c r="AH69" s="77"/>
-      <c r="AI69" s="78"/>
-      <c r="AJ69" s="76"/>
-      <c r="AK69" s="77"/>
-      <c r="AL69" s="77"/>
-      <c r="AM69" s="77"/>
-      <c r="AN69" s="77"/>
-      <c r="AO69" s="78"/>
+      <c r="AD69" s="54"/>
+      <c r="AE69" s="55"/>
+      <c r="AF69" s="55"/>
+      <c r="AG69" s="55"/>
+      <c r="AH69" s="55"/>
+      <c r="AI69" s="56"/>
+      <c r="AJ69" s="54"/>
+      <c r="AK69" s="55"/>
+      <c r="AL69" s="55"/>
+      <c r="AM69" s="55"/>
+      <c r="AN69" s="55"/>
+      <c r="AO69" s="56"/>
       <c r="AP69" s="54"/>
       <c r="AQ69" s="55"/>
       <c r="AR69" s="55"/>
@@ -7157,7 +7058,26 @@
     </row>
   </sheetData>
   <sheetProtection insertRows="0"/>
-  <mergeCells count="37">
+  <mergeCells count="35">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="L1:Q1"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="R1:W1"/>
+    <mergeCell ref="X1:AC1"/>
+    <mergeCell ref="AJ2:AL2"/>
+    <mergeCell ref="AD1:AI1"/>
+    <mergeCell ref="AJ1:AO1"/>
+    <mergeCell ref="AD2:AF2"/>
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="X2:Z2"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="U2:W2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="BB2:BD2"/>
     <mergeCell ref="BE2:BG2"/>
@@ -7174,29 +7094,8 @@
     <mergeCell ref="AM2:AO2"/>
     <mergeCell ref="AP2:AR2"/>
     <mergeCell ref="AA2:AC2"/>
-    <mergeCell ref="AD2:AF2"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="X2:Z2"/>
-    <mergeCell ref="O2:Q2"/>
-    <mergeCell ref="U2:W2"/>
-    <mergeCell ref="AD3:AI69"/>
-    <mergeCell ref="AJ3:AO69"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="L1:Q1"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="R1:W1"/>
-    <mergeCell ref="X1:AC1"/>
-    <mergeCell ref="AJ2:AL2"/>
-    <mergeCell ref="AD1:AI1"/>
-    <mergeCell ref="AJ1:AO1"/>
   </mergeCells>
-  <conditionalFormatting sqref="F5:AC14 AP5:BM14">
+  <conditionalFormatting sqref="F5:BM14">
     <cfRule type="cellIs" dxfId="11" priority="159" stopIfTrue="1" operator="equal">
       <formula>"p"</formula>
     </cfRule>
@@ -7204,7 +7103,7 @@
       <formula>"r"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F16:AC25 AP16:BM25">
+  <conditionalFormatting sqref="F16:BM25">
     <cfRule type="cellIs" dxfId="9" priority="157" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
@@ -7212,7 +7111,7 @@
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F27:AC36 AP27:BM36">
+  <conditionalFormatting sqref="F27:BM36">
     <cfRule type="cellIs" dxfId="7" priority="155" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
@@ -7220,7 +7119,7 @@
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F38:AC47 AP38:BM47">
+  <conditionalFormatting sqref="F38:BM47">
     <cfRule type="cellIs" dxfId="5" priority="153" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
@@ -7228,7 +7127,7 @@
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AP49:BM58 F49:AC58">
+  <conditionalFormatting sqref="F49:BM58">
     <cfRule type="cellIs" dxfId="3" priority="151" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
@@ -7236,7 +7135,7 @@
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F60:AC69 AP60:BM69">
+  <conditionalFormatting sqref="F60:BM69">
     <cfRule type="cellIs" dxfId="1" priority="149" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Création fichier Conventions de nommage
Effacé ancien contenu du dossier Ivan car vide.
</commit_message>
<xml_diff>
--- a/docs/M306_Planning_2022.xlsx
+++ b/docs/M306_Planning_2022.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="38">
   <si>
     <t>Listes des tâches</t>
   </si>
@@ -149,9 +149,6 @@
   </si>
   <si>
     <t>Ivan</t>
-  </si>
-  <si>
-    <t>p</t>
   </si>
   <si>
     <t>Tâches</t>
@@ -1257,68 +1254,68 @@
     <xf numFmtId="0" fontId="2" fillId="16" borderId="50" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="47" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="48" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="45" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="45" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="5" borderId="48" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="5" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="5" borderId="47" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="5" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1819,8 +1816,8 @@
   <dimension ref="A1:BM69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AK44" sqref="AK44"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AI12" sqref="AI12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1834,211 +1831,211 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:65" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="70" t="s">
+      <c r="B1" s="75"/>
+      <c r="C1" s="89" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="88" t="s">
+      <c r="D1" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="81" t="s">
+      <c r="E1" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="87">
+      <c r="F1" s="78">
         <f>WEEKNUM(F2)</f>
         <v>6</v>
       </c>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="76">
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="80"/>
+      <c r="L1" s="81">
         <f>WEEKNUM(L2)</f>
         <v>7</v>
       </c>
-      <c r="M1" s="77"/>
-      <c r="N1" s="77"/>
-      <c r="O1" s="77"/>
-      <c r="P1" s="77"/>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="76">
+      <c r="M1" s="79"/>
+      <c r="N1" s="79"/>
+      <c r="O1" s="79"/>
+      <c r="P1" s="79"/>
+      <c r="Q1" s="80"/>
+      <c r="R1" s="81">
         <f>WEEKNUM(R2)</f>
         <v>8</v>
       </c>
-      <c r="S1" s="77"/>
-      <c r="T1" s="77"/>
-      <c r="U1" s="77"/>
-      <c r="V1" s="77"/>
-      <c r="W1" s="78"/>
-      <c r="X1" s="76">
+      <c r="S1" s="79"/>
+      <c r="T1" s="79"/>
+      <c r="U1" s="79"/>
+      <c r="V1" s="79"/>
+      <c r="W1" s="80"/>
+      <c r="X1" s="81">
         <f>WEEKNUM(X2)</f>
         <v>9</v>
       </c>
-      <c r="Y1" s="77"/>
-      <c r="Z1" s="77"/>
-      <c r="AA1" s="77"/>
-      <c r="AB1" s="77"/>
-      <c r="AC1" s="78"/>
-      <c r="AD1" s="76">
+      <c r="Y1" s="79"/>
+      <c r="Z1" s="79"/>
+      <c r="AA1" s="79"/>
+      <c r="AB1" s="79"/>
+      <c r="AC1" s="80"/>
+      <c r="AD1" s="81">
         <f>WEEKNUM(AD2)</f>
         <v>10</v>
       </c>
-      <c r="AE1" s="77"/>
-      <c r="AF1" s="77"/>
-      <c r="AG1" s="77"/>
-      <c r="AH1" s="77"/>
-      <c r="AI1" s="78"/>
-      <c r="AJ1" s="76">
+      <c r="AE1" s="79"/>
+      <c r="AF1" s="79"/>
+      <c r="AG1" s="79"/>
+      <c r="AH1" s="79"/>
+      <c r="AI1" s="80"/>
+      <c r="AJ1" s="81">
         <f>WEEKNUM(AJ2)</f>
         <v>11</v>
       </c>
-      <c r="AK1" s="77"/>
-      <c r="AL1" s="77"/>
-      <c r="AM1" s="77"/>
-      <c r="AN1" s="77"/>
-      <c r="AO1" s="78"/>
-      <c r="AP1" s="76">
+      <c r="AK1" s="79"/>
+      <c r="AL1" s="79"/>
+      <c r="AM1" s="79"/>
+      <c r="AN1" s="79"/>
+      <c r="AO1" s="80"/>
+      <c r="AP1" s="81">
         <f>WEEKNUM(AP2)</f>
         <v>12</v>
       </c>
-      <c r="AQ1" s="77"/>
-      <c r="AR1" s="77"/>
-      <c r="AS1" s="77"/>
-      <c r="AT1" s="77"/>
-      <c r="AU1" s="78"/>
-      <c r="AV1" s="76">
+      <c r="AQ1" s="79"/>
+      <c r="AR1" s="79"/>
+      <c r="AS1" s="79"/>
+      <c r="AT1" s="79"/>
+      <c r="AU1" s="80"/>
+      <c r="AV1" s="81">
         <f>WEEKNUM(AV2)</f>
         <v>13</v>
       </c>
-      <c r="AW1" s="77"/>
-      <c r="AX1" s="77"/>
-      <c r="AY1" s="77"/>
-      <c r="AZ1" s="77"/>
-      <c r="BA1" s="78"/>
-      <c r="BB1" s="76">
+      <c r="AW1" s="79"/>
+      <c r="AX1" s="79"/>
+      <c r="AY1" s="79"/>
+      <c r="AZ1" s="79"/>
+      <c r="BA1" s="80"/>
+      <c r="BB1" s="81">
         <f>WEEKNUM(BB2)</f>
         <v>14</v>
       </c>
-      <c r="BC1" s="77"/>
-      <c r="BD1" s="77"/>
-      <c r="BE1" s="77"/>
-      <c r="BF1" s="77"/>
-      <c r="BG1" s="78"/>
-      <c r="BH1" s="76">
+      <c r="BC1" s="79"/>
+      <c r="BD1" s="79"/>
+      <c r="BE1" s="79"/>
+      <c r="BF1" s="79"/>
+      <c r="BG1" s="80"/>
+      <c r="BH1" s="81">
         <f>WEEKNUM(BH2)</f>
         <v>15</v>
       </c>
-      <c r="BI1" s="77"/>
-      <c r="BJ1" s="77"/>
-      <c r="BK1" s="77"/>
-      <c r="BL1" s="77"/>
-      <c r="BM1" s="78"/>
+      <c r="BI1" s="79"/>
+      <c r="BJ1" s="79"/>
+      <c r="BK1" s="79"/>
+      <c r="BL1" s="79"/>
+      <c r="BM1" s="80"/>
     </row>
     <row r="2" spans="1:65" ht="106.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="85"/>
-      <c r="B2" s="86"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="90">
+      <c r="A2" s="76"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="86">
         <v>44593</v>
       </c>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="74"/>
-      <c r="J2" s="74"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="72">
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="87"/>
+      <c r="J2" s="87"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="82">
         <f>F2+7</f>
         <v>44600</v>
       </c>
-      <c r="M2" s="73"/>
-      <c r="N2" s="73"/>
-      <c r="O2" s="74"/>
-      <c r="P2" s="74"/>
-      <c r="Q2" s="75"/>
-      <c r="R2" s="72">
+      <c r="M2" s="83"/>
+      <c r="N2" s="83"/>
+      <c r="O2" s="87"/>
+      <c r="P2" s="87"/>
+      <c r="Q2" s="88"/>
+      <c r="R2" s="82">
         <f>L2+7</f>
         <v>44607</v>
       </c>
-      <c r="S2" s="73"/>
-      <c r="T2" s="73"/>
-      <c r="U2" s="74"/>
-      <c r="V2" s="74"/>
-      <c r="W2" s="75"/>
-      <c r="X2" s="72">
+      <c r="S2" s="83"/>
+      <c r="T2" s="83"/>
+      <c r="U2" s="87"/>
+      <c r="V2" s="87"/>
+      <c r="W2" s="88"/>
+      <c r="X2" s="82">
         <f>R2+7</f>
         <v>44614</v>
       </c>
-      <c r="Y2" s="73"/>
-      <c r="Z2" s="73"/>
-      <c r="AA2" s="74"/>
-      <c r="AB2" s="74"/>
-      <c r="AC2" s="75"/>
-      <c r="AD2" s="72">
+      <c r="Y2" s="83"/>
+      <c r="Z2" s="83"/>
+      <c r="AA2" s="87"/>
+      <c r="AB2" s="87"/>
+      <c r="AC2" s="88"/>
+      <c r="AD2" s="82">
         <f>X2+7</f>
         <v>44621</v>
       </c>
-      <c r="AE2" s="73"/>
-      <c r="AF2" s="73"/>
-      <c r="AG2" s="74"/>
-      <c r="AH2" s="74"/>
-      <c r="AI2" s="75"/>
-      <c r="AJ2" s="72">
+      <c r="AE2" s="83"/>
+      <c r="AF2" s="83"/>
+      <c r="AG2" s="87"/>
+      <c r="AH2" s="87"/>
+      <c r="AI2" s="88"/>
+      <c r="AJ2" s="82">
         <f>AD2+7</f>
         <v>44628</v>
       </c>
-      <c r="AK2" s="73"/>
-      <c r="AL2" s="73"/>
-      <c r="AM2" s="74"/>
-      <c r="AN2" s="74"/>
-      <c r="AO2" s="75"/>
-      <c r="AP2" s="72">
+      <c r="AK2" s="83"/>
+      <c r="AL2" s="83"/>
+      <c r="AM2" s="87"/>
+      <c r="AN2" s="87"/>
+      <c r="AO2" s="88"/>
+      <c r="AP2" s="82">
         <f>AJ2+7</f>
         <v>44635</v>
       </c>
-      <c r="AQ2" s="73"/>
-      <c r="AR2" s="73"/>
-      <c r="AS2" s="74"/>
-      <c r="AT2" s="74"/>
-      <c r="AU2" s="75"/>
-      <c r="AV2" s="72">
+      <c r="AQ2" s="83"/>
+      <c r="AR2" s="83"/>
+      <c r="AS2" s="87"/>
+      <c r="AT2" s="87"/>
+      <c r="AU2" s="88"/>
+      <c r="AV2" s="82">
         <f>AP2+7</f>
         <v>44642</v>
       </c>
-      <c r="AW2" s="73"/>
-      <c r="AX2" s="73"/>
-      <c r="AY2" s="74"/>
-      <c r="AZ2" s="74"/>
-      <c r="BA2" s="75"/>
-      <c r="BB2" s="72">
+      <c r="AW2" s="83"/>
+      <c r="AX2" s="83"/>
+      <c r="AY2" s="87"/>
+      <c r="AZ2" s="87"/>
+      <c r="BA2" s="88"/>
+      <c r="BB2" s="82">
         <f>AV2+7</f>
         <v>44649</v>
       </c>
-      <c r="BC2" s="73"/>
-      <c r="BD2" s="73"/>
-      <c r="BE2" s="74"/>
-      <c r="BF2" s="74"/>
-      <c r="BG2" s="75"/>
-      <c r="BH2" s="72">
+      <c r="BC2" s="83"/>
+      <c r="BD2" s="83"/>
+      <c r="BE2" s="87"/>
+      <c r="BF2" s="87"/>
+      <c r="BG2" s="88"/>
+      <c r="BH2" s="82">
         <f>BB2+7</f>
         <v>44656</v>
       </c>
-      <c r="BI2" s="73"/>
-      <c r="BJ2" s="73"/>
-      <c r="BK2" s="74"/>
-      <c r="BL2" s="74"/>
-      <c r="BM2" s="75"/>
+      <c r="BI2" s="83"/>
+      <c r="BJ2" s="83"/>
+      <c r="BK2" s="87"/>
+      <c r="BL2" s="87"/>
+      <c r="BM2" s="88"/>
     </row>
     <row r="3" spans="1:65" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="79" t="s">
+      <c r="A3" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="80"/>
+      <c r="B3" s="71"/>
       <c r="C3" s="61"/>
       <c r="D3" s="37" t="s">
         <v>7</v>
@@ -4008,7 +4005,7 @@
     <row r="29" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A29" s="23"/>
       <c r="B29" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C29" s="63"/>
       <c r="D29" s="41">
@@ -4599,11 +4596,11 @@
       <c r="C37" s="67"/>
       <c r="D37" s="45">
         <f>SUM(D38:D47)</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E37" s="17">
         <f>SUM(E38:E47)</f>
-        <v>0.5</v>
+        <v>6.5</v>
       </c>
       <c r="F37" s="6"/>
       <c r="G37" s="4"/>
@@ -4755,11 +4752,11 @@
       </c>
       <c r="D39" s="41">
         <f t="shared" ref="D39:D47" si="6">IF($B39&gt;"",SUM(COUNTIF(F39:BM39,"P"))/2,"")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E39" s="13">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F39" s="51"/>
       <c r="G39" s="52"/>
@@ -4773,7 +4770,7 @@
       <c r="O39" s="52"/>
       <c r="P39" s="52"/>
       <c r="Q39" s="53" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="R39" s="51"/>
       <c r="S39" s="52"/>
@@ -4788,13 +4785,13 @@
       <c r="AB39" s="52"/>
       <c r="AC39" s="53"/>
       <c r="AD39" s="51" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="AE39" s="52" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="AF39" s="52" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="AG39" s="52"/>
       <c r="AH39" s="52"/>
@@ -4840,11 +4837,11 @@
       </c>
       <c r="D40" s="41">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E40" s="13">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F40" s="51"/>
       <c r="G40" s="52"/>
@@ -4858,7 +4855,7 @@
       <c r="O40" s="52"/>
       <c r="P40" s="52"/>
       <c r="Q40" s="53" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="R40" s="51"/>
       <c r="S40" s="52"/>
@@ -4873,13 +4870,13 @@
       <c r="AB40" s="52"/>
       <c r="AC40" s="53"/>
       <c r="AD40" s="51" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="AE40" s="52" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="AF40" s="52" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="AG40" s="52"/>
       <c r="AH40" s="52"/>
@@ -4925,11 +4922,11 @@
       </c>
       <c r="D41" s="41">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E41" s="13">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F41" s="51"/>
       <c r="G41" s="52"/>
@@ -4943,7 +4940,7 @@
       <c r="O41" s="52"/>
       <c r="P41" s="52"/>
       <c r="Q41" s="53" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="R41" s="51"/>
       <c r="S41" s="52"/>
@@ -4958,13 +4955,13 @@
       <c r="AB41" s="52"/>
       <c r="AC41" s="53"/>
       <c r="AD41" s="51" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="AE41" s="52" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="AF41" s="52" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="AG41" s="52"/>
       <c r="AH41" s="52"/>
@@ -7059,6 +7056,30 @@
   </sheetData>
   <sheetProtection insertRows="0"/>
   <mergeCells count="35">
+    <mergeCell ref="AP1:AU1"/>
+    <mergeCell ref="AV1:BA1"/>
+    <mergeCell ref="AV2:AX2"/>
+    <mergeCell ref="AY2:BA2"/>
+    <mergeCell ref="AS2:AU2"/>
+    <mergeCell ref="AP2:AR2"/>
+    <mergeCell ref="BB2:BD2"/>
+    <mergeCell ref="BE2:BG2"/>
+    <mergeCell ref="BH2:BJ2"/>
+    <mergeCell ref="BK2:BM2"/>
+    <mergeCell ref="BB1:BG1"/>
+    <mergeCell ref="BH1:BM1"/>
+    <mergeCell ref="R1:W1"/>
+    <mergeCell ref="X1:AC1"/>
+    <mergeCell ref="AJ2:AL2"/>
+    <mergeCell ref="AD1:AI1"/>
+    <mergeCell ref="AJ1:AO1"/>
+    <mergeCell ref="AD2:AF2"/>
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="X2:Z2"/>
+    <mergeCell ref="U2:W2"/>
+    <mergeCell ref="AG2:AI2"/>
+    <mergeCell ref="AM2:AO2"/>
+    <mergeCell ref="AA2:AC2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="A1:B2"/>
@@ -7068,32 +7089,8 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="I2:K2"/>
-    <mergeCell ref="R1:W1"/>
-    <mergeCell ref="X1:AC1"/>
-    <mergeCell ref="AJ2:AL2"/>
-    <mergeCell ref="AD1:AI1"/>
-    <mergeCell ref="AJ1:AO1"/>
-    <mergeCell ref="AD2:AF2"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="X2:Z2"/>
     <mergeCell ref="O2:Q2"/>
-    <mergeCell ref="U2:W2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="BB2:BD2"/>
-    <mergeCell ref="BE2:BG2"/>
-    <mergeCell ref="BH2:BJ2"/>
-    <mergeCell ref="BK2:BM2"/>
-    <mergeCell ref="BB1:BG1"/>
-    <mergeCell ref="BH1:BM1"/>
-    <mergeCell ref="AG2:AI2"/>
-    <mergeCell ref="AP1:AU1"/>
-    <mergeCell ref="AV1:BA1"/>
-    <mergeCell ref="AV2:AX2"/>
-    <mergeCell ref="AY2:BA2"/>
-    <mergeCell ref="AS2:AU2"/>
-    <mergeCell ref="AM2:AO2"/>
-    <mergeCell ref="AP2:AR2"/>
-    <mergeCell ref="AA2:AC2"/>
   </mergeCells>
   <conditionalFormatting sqref="F5:BM14">
     <cfRule type="cellIs" dxfId="11" priority="159" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
Modification mineurs des fichiers
</commit_message>
<xml_diff>
--- a/docs/M306_Planning_2022.xlsx
+++ b/docs/M306_Planning_2022.xlsx
@@ -21,12 +21,12 @@
     <definedName name="Semestre2">#REF!</definedName>
     <definedName name="Test">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="40">
   <si>
     <t>Listes des tâches</t>
   </si>
@@ -152,6 +152,12 @@
   </si>
   <si>
     <t>Tâches</t>
+  </si>
+  <si>
+    <t>Vacances</t>
+  </si>
+  <si>
+    <t>Absence</t>
   </si>
 </sst>
 </file>
@@ -357,7 +363,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="54">
+  <borders count="59">
     <border>
       <left/>
       <right/>
@@ -1042,12 +1048,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1254,6 +1311,54 @@
     <xf numFmtId="0" fontId="2" fillId="16" borderId="50" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="48" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="47" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="45" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="55" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="56" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="57" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="58" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1281,21 +1386,6 @@
     <xf numFmtId="166" fontId="12" fillId="5" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="12" fillId="5" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="5" borderId="47" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="5" borderId="48" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
@@ -1304,12 +1394,6 @@
     </xf>
     <xf numFmtId="164" fontId="11" fillId="3" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="45" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1816,8 +1900,8 @@
   <dimension ref="A1:BM69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AI12" sqref="AI12"/>
+      <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R4" sqref="R4:AC69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1831,211 +1915,211 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:65" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="90" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="89" t="s">
+      <c r="B1" s="91"/>
+      <c r="C1" s="98" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="84" t="s">
+      <c r="D1" s="95" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="72" t="s">
+      <c r="E1" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="78">
+      <c r="F1" s="94">
         <f>WEEKNUM(F2)</f>
         <v>6</v>
       </c>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="81">
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="70">
         <f>WEEKNUM(L2)</f>
         <v>7</v>
       </c>
-      <c r="M1" s="79"/>
-      <c r="N1" s="79"/>
-      <c r="O1" s="79"/>
-      <c r="P1" s="79"/>
-      <c r="Q1" s="80"/>
-      <c r="R1" s="81">
+      <c r="M1" s="71"/>
+      <c r="N1" s="71"/>
+      <c r="O1" s="71"/>
+      <c r="P1" s="71"/>
+      <c r="Q1" s="72"/>
+      <c r="R1" s="70">
         <f>WEEKNUM(R2)</f>
         <v>8</v>
       </c>
-      <c r="S1" s="79"/>
-      <c r="T1" s="79"/>
-      <c r="U1" s="79"/>
-      <c r="V1" s="79"/>
-      <c r="W1" s="80"/>
-      <c r="X1" s="81">
+      <c r="S1" s="71"/>
+      <c r="T1" s="71"/>
+      <c r="U1" s="71"/>
+      <c r="V1" s="71"/>
+      <c r="W1" s="72"/>
+      <c r="X1" s="70">
         <f>WEEKNUM(X2)</f>
         <v>9</v>
       </c>
-      <c r="Y1" s="79"/>
-      <c r="Z1" s="79"/>
-      <c r="AA1" s="79"/>
-      <c r="AB1" s="79"/>
-      <c r="AC1" s="80"/>
-      <c r="AD1" s="81">
+      <c r="Y1" s="71"/>
+      <c r="Z1" s="71"/>
+      <c r="AA1" s="71"/>
+      <c r="AB1" s="71"/>
+      <c r="AC1" s="72"/>
+      <c r="AD1" s="70">
         <f>WEEKNUM(AD2)</f>
         <v>10</v>
       </c>
-      <c r="AE1" s="79"/>
-      <c r="AF1" s="79"/>
-      <c r="AG1" s="79"/>
-      <c r="AH1" s="79"/>
-      <c r="AI1" s="80"/>
-      <c r="AJ1" s="81">
+      <c r="AE1" s="71"/>
+      <c r="AF1" s="71"/>
+      <c r="AG1" s="71"/>
+      <c r="AH1" s="71"/>
+      <c r="AI1" s="72"/>
+      <c r="AJ1" s="70">
         <f>WEEKNUM(AJ2)</f>
         <v>11</v>
       </c>
-      <c r="AK1" s="79"/>
-      <c r="AL1" s="79"/>
-      <c r="AM1" s="79"/>
-      <c r="AN1" s="79"/>
-      <c r="AO1" s="80"/>
-      <c r="AP1" s="81">
+      <c r="AK1" s="71"/>
+      <c r="AL1" s="71"/>
+      <c r="AM1" s="71"/>
+      <c r="AN1" s="71"/>
+      <c r="AO1" s="72"/>
+      <c r="AP1" s="70">
         <f>WEEKNUM(AP2)</f>
         <v>12</v>
       </c>
-      <c r="AQ1" s="79"/>
-      <c r="AR1" s="79"/>
-      <c r="AS1" s="79"/>
-      <c r="AT1" s="79"/>
-      <c r="AU1" s="80"/>
-      <c r="AV1" s="81">
+      <c r="AQ1" s="71"/>
+      <c r="AR1" s="71"/>
+      <c r="AS1" s="71"/>
+      <c r="AT1" s="71"/>
+      <c r="AU1" s="72"/>
+      <c r="AV1" s="70">
         <f>WEEKNUM(AV2)</f>
         <v>13</v>
       </c>
-      <c r="AW1" s="79"/>
-      <c r="AX1" s="79"/>
-      <c r="AY1" s="79"/>
-      <c r="AZ1" s="79"/>
-      <c r="BA1" s="80"/>
-      <c r="BB1" s="81">
+      <c r="AW1" s="71"/>
+      <c r="AX1" s="71"/>
+      <c r="AY1" s="71"/>
+      <c r="AZ1" s="71"/>
+      <c r="BA1" s="72"/>
+      <c r="BB1" s="70">
         <f>WEEKNUM(BB2)</f>
         <v>14</v>
       </c>
-      <c r="BC1" s="79"/>
-      <c r="BD1" s="79"/>
-      <c r="BE1" s="79"/>
-      <c r="BF1" s="79"/>
-      <c r="BG1" s="80"/>
-      <c r="BH1" s="81">
+      <c r="BC1" s="71"/>
+      <c r="BD1" s="71"/>
+      <c r="BE1" s="71"/>
+      <c r="BF1" s="71"/>
+      <c r="BG1" s="72"/>
+      <c r="BH1" s="70">
         <f>WEEKNUM(BH2)</f>
         <v>15</v>
       </c>
-      <c r="BI1" s="79"/>
-      <c r="BJ1" s="79"/>
-      <c r="BK1" s="79"/>
-      <c r="BL1" s="79"/>
-      <c r="BM1" s="80"/>
+      <c r="BI1" s="71"/>
+      <c r="BJ1" s="71"/>
+      <c r="BK1" s="71"/>
+      <c r="BL1" s="71"/>
+      <c r="BM1" s="72"/>
     </row>
     <row r="2" spans="1:65" ht="106.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="76"/>
-      <c r="B2" s="77"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="86">
+      <c r="A2" s="92"/>
+      <c r="B2" s="93"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="97">
         <v>44593</v>
       </c>
-      <c r="G2" s="83"/>
-      <c r="H2" s="83"/>
-      <c r="I2" s="87"/>
-      <c r="J2" s="87"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="82">
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="76"/>
+      <c r="L2" s="73">
         <f>F2+7</f>
         <v>44600</v>
       </c>
-      <c r="M2" s="83"/>
-      <c r="N2" s="83"/>
-      <c r="O2" s="87"/>
-      <c r="P2" s="87"/>
-      <c r="Q2" s="88"/>
-      <c r="R2" s="82">
+      <c r="M2" s="74"/>
+      <c r="N2" s="74"/>
+      <c r="O2" s="75"/>
+      <c r="P2" s="75"/>
+      <c r="Q2" s="76"/>
+      <c r="R2" s="73">
         <f>L2+7</f>
         <v>44607</v>
       </c>
-      <c r="S2" s="83"/>
-      <c r="T2" s="83"/>
-      <c r="U2" s="87"/>
-      <c r="V2" s="87"/>
-      <c r="W2" s="88"/>
-      <c r="X2" s="82">
+      <c r="S2" s="74"/>
+      <c r="T2" s="74"/>
+      <c r="U2" s="75"/>
+      <c r="V2" s="75"/>
+      <c r="W2" s="76"/>
+      <c r="X2" s="73">
         <f>R2+7</f>
         <v>44614</v>
       </c>
-      <c r="Y2" s="83"/>
-      <c r="Z2" s="83"/>
-      <c r="AA2" s="87"/>
-      <c r="AB2" s="87"/>
-      <c r="AC2" s="88"/>
-      <c r="AD2" s="82">
+      <c r="Y2" s="74"/>
+      <c r="Z2" s="74"/>
+      <c r="AA2" s="75"/>
+      <c r="AB2" s="75"/>
+      <c r="AC2" s="76"/>
+      <c r="AD2" s="73">
         <f>X2+7</f>
         <v>44621</v>
       </c>
-      <c r="AE2" s="83"/>
-      <c r="AF2" s="83"/>
-      <c r="AG2" s="87"/>
-      <c r="AH2" s="87"/>
-      <c r="AI2" s="88"/>
-      <c r="AJ2" s="82">
+      <c r="AE2" s="74"/>
+      <c r="AF2" s="74"/>
+      <c r="AG2" s="75"/>
+      <c r="AH2" s="75"/>
+      <c r="AI2" s="76"/>
+      <c r="AJ2" s="73">
         <f>AD2+7</f>
         <v>44628</v>
       </c>
-      <c r="AK2" s="83"/>
-      <c r="AL2" s="83"/>
-      <c r="AM2" s="87"/>
-      <c r="AN2" s="87"/>
-      <c r="AO2" s="88"/>
-      <c r="AP2" s="82">
+      <c r="AK2" s="74"/>
+      <c r="AL2" s="74"/>
+      <c r="AM2" s="75"/>
+      <c r="AN2" s="75"/>
+      <c r="AO2" s="76"/>
+      <c r="AP2" s="73">
         <f>AJ2+7</f>
         <v>44635</v>
       </c>
-      <c r="AQ2" s="83"/>
-      <c r="AR2" s="83"/>
-      <c r="AS2" s="87"/>
-      <c r="AT2" s="87"/>
-      <c r="AU2" s="88"/>
-      <c r="AV2" s="82">
+      <c r="AQ2" s="74"/>
+      <c r="AR2" s="74"/>
+      <c r="AS2" s="75"/>
+      <c r="AT2" s="75"/>
+      <c r="AU2" s="76"/>
+      <c r="AV2" s="73">
         <f>AP2+7</f>
         <v>44642</v>
       </c>
-      <c r="AW2" s="83"/>
-      <c r="AX2" s="83"/>
-      <c r="AY2" s="87"/>
-      <c r="AZ2" s="87"/>
-      <c r="BA2" s="88"/>
-      <c r="BB2" s="82">
+      <c r="AW2" s="74"/>
+      <c r="AX2" s="74"/>
+      <c r="AY2" s="75"/>
+      <c r="AZ2" s="75"/>
+      <c r="BA2" s="76"/>
+      <c r="BB2" s="73">
         <f>AV2+7</f>
         <v>44649</v>
       </c>
-      <c r="BC2" s="83"/>
-      <c r="BD2" s="83"/>
-      <c r="BE2" s="87"/>
-      <c r="BF2" s="87"/>
-      <c r="BG2" s="88"/>
-      <c r="BH2" s="82">
+      <c r="BC2" s="74"/>
+      <c r="BD2" s="74"/>
+      <c r="BE2" s="75"/>
+      <c r="BF2" s="75"/>
+      <c r="BG2" s="76"/>
+      <c r="BH2" s="73">
         <f>BB2+7</f>
         <v>44656</v>
       </c>
-      <c r="BI2" s="83"/>
-      <c r="BJ2" s="83"/>
-      <c r="BK2" s="87"/>
-      <c r="BL2" s="87"/>
-      <c r="BM2" s="88"/>
+      <c r="BI2" s="74"/>
+      <c r="BJ2" s="74"/>
+      <c r="BK2" s="75"/>
+      <c r="BL2" s="75"/>
+      <c r="BM2" s="76"/>
     </row>
     <row r="3" spans="1:65" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="70" t="s">
+      <c r="A3" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="71"/>
+      <c r="B3" s="87"/>
       <c r="C3" s="61"/>
       <c r="D3" s="37" t="s">
         <v>7</v>
@@ -2131,18 +2215,22 @@
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="5"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="4"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="4"/>
-      <c r="V4" s="4"/>
-      <c r="W4" s="5"/>
-      <c r="X4" s="6"/>
-      <c r="Y4" s="4"/>
-      <c r="Z4" s="4"/>
-      <c r="AA4" s="4"/>
-      <c r="AB4" s="4"/>
-      <c r="AC4" s="5"/>
+      <c r="R4" s="77" t="s">
+        <v>38</v>
+      </c>
+      <c r="S4" s="78"/>
+      <c r="T4" s="78"/>
+      <c r="U4" s="78"/>
+      <c r="V4" s="78"/>
+      <c r="W4" s="79"/>
+      <c r="X4" s="77" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y4" s="78"/>
+      <c r="Z4" s="78"/>
+      <c r="AA4" s="78"/>
+      <c r="AB4" s="78"/>
+      <c r="AC4" s="79"/>
       <c r="AD4" s="6"/>
       <c r="AE4" s="4"/>
       <c r="AF4" s="4"/>
@@ -2208,18 +2296,18 @@
       <c r="O5" s="49"/>
       <c r="P5" s="49"/>
       <c r="Q5" s="50"/>
-      <c r="R5" s="48"/>
-      <c r="S5" s="49"/>
-      <c r="T5" s="49"/>
-      <c r="U5" s="49"/>
-      <c r="V5" s="49"/>
-      <c r="W5" s="50"/>
-      <c r="X5" s="48"/>
-      <c r="Y5" s="49"/>
-      <c r="Z5" s="49"/>
-      <c r="AA5" s="49"/>
-      <c r="AB5" s="49"/>
-      <c r="AC5" s="50"/>
+      <c r="R5" s="80"/>
+      <c r="S5" s="81"/>
+      <c r="T5" s="81"/>
+      <c r="U5" s="81"/>
+      <c r="V5" s="81"/>
+      <c r="W5" s="82"/>
+      <c r="X5" s="80"/>
+      <c r="Y5" s="81"/>
+      <c r="Z5" s="81"/>
+      <c r="AA5" s="81"/>
+      <c r="AB5" s="81"/>
+      <c r="AC5" s="82"/>
       <c r="AD5" s="48"/>
       <c r="AE5" s="49"/>
       <c r="AF5" s="49"/>
@@ -2289,18 +2377,18 @@
       <c r="O6" s="52"/>
       <c r="P6" s="52"/>
       <c r="Q6" s="53"/>
-      <c r="R6" s="51"/>
-      <c r="S6" s="52"/>
-      <c r="T6" s="52"/>
-      <c r="U6" s="52"/>
-      <c r="V6" s="52"/>
-      <c r="W6" s="53"/>
-      <c r="X6" s="51"/>
-      <c r="Y6" s="52"/>
-      <c r="Z6" s="52"/>
-      <c r="AA6" s="52"/>
-      <c r="AB6" s="52"/>
-      <c r="AC6" s="53"/>
+      <c r="R6" s="80"/>
+      <c r="S6" s="81"/>
+      <c r="T6" s="81"/>
+      <c r="U6" s="81"/>
+      <c r="V6" s="81"/>
+      <c r="W6" s="82"/>
+      <c r="X6" s="80"/>
+      <c r="Y6" s="81"/>
+      <c r="Z6" s="81"/>
+      <c r="AA6" s="81"/>
+      <c r="AB6" s="81"/>
+      <c r="AC6" s="82"/>
       <c r="AD6" s="51"/>
       <c r="AE6" s="52"/>
       <c r="AF6" s="52"/>
@@ -2370,18 +2458,18 @@
       <c r="O7" s="52"/>
       <c r="P7" s="52"/>
       <c r="Q7" s="53"/>
-      <c r="R7" s="51"/>
-      <c r="S7" s="52"/>
-      <c r="T7" s="52"/>
-      <c r="U7" s="52"/>
-      <c r="V7" s="52"/>
-      <c r="W7" s="53"/>
-      <c r="X7" s="51"/>
-      <c r="Y7" s="52"/>
-      <c r="Z7" s="52"/>
-      <c r="AA7" s="52"/>
-      <c r="AB7" s="52"/>
-      <c r="AC7" s="53"/>
+      <c r="R7" s="80"/>
+      <c r="S7" s="81"/>
+      <c r="T7" s="81"/>
+      <c r="U7" s="81"/>
+      <c r="V7" s="81"/>
+      <c r="W7" s="82"/>
+      <c r="X7" s="80"/>
+      <c r="Y7" s="81"/>
+      <c r="Z7" s="81"/>
+      <c r="AA7" s="81"/>
+      <c r="AB7" s="81"/>
+      <c r="AC7" s="82"/>
       <c r="AD7" s="51"/>
       <c r="AE7" s="52"/>
       <c r="AF7" s="52"/>
@@ -2449,18 +2537,18 @@
       <c r="O8" s="52"/>
       <c r="P8" s="52"/>
       <c r="Q8" s="53"/>
-      <c r="R8" s="51"/>
-      <c r="S8" s="52"/>
-      <c r="T8" s="52"/>
-      <c r="U8" s="52"/>
-      <c r="V8" s="52"/>
-      <c r="W8" s="53"/>
-      <c r="X8" s="51"/>
-      <c r="Y8" s="52"/>
-      <c r="Z8" s="52"/>
-      <c r="AA8" s="52"/>
-      <c r="AB8" s="52"/>
-      <c r="AC8" s="53"/>
+      <c r="R8" s="80"/>
+      <c r="S8" s="81"/>
+      <c r="T8" s="81"/>
+      <c r="U8" s="81"/>
+      <c r="V8" s="81"/>
+      <c r="W8" s="82"/>
+      <c r="X8" s="80"/>
+      <c r="Y8" s="81"/>
+      <c r="Z8" s="81"/>
+      <c r="AA8" s="81"/>
+      <c r="AB8" s="81"/>
+      <c r="AC8" s="82"/>
       <c r="AD8" s="51"/>
       <c r="AE8" s="52"/>
       <c r="AF8" s="52"/>
@@ -2526,18 +2614,18 @@
       <c r="O9" s="52"/>
       <c r="P9" s="52"/>
       <c r="Q9" s="53"/>
-      <c r="R9" s="51"/>
-      <c r="S9" s="52"/>
-      <c r="T9" s="52"/>
-      <c r="U9" s="52"/>
-      <c r="V9" s="52"/>
-      <c r="W9" s="53"/>
-      <c r="X9" s="51"/>
-      <c r="Y9" s="52"/>
-      <c r="Z9" s="52"/>
-      <c r="AA9" s="52"/>
-      <c r="AB9" s="52"/>
-      <c r="AC9" s="53"/>
+      <c r="R9" s="80"/>
+      <c r="S9" s="81"/>
+      <c r="T9" s="81"/>
+      <c r="U9" s="81"/>
+      <c r="V9" s="81"/>
+      <c r="W9" s="82"/>
+      <c r="X9" s="80"/>
+      <c r="Y9" s="81"/>
+      <c r="Z9" s="81"/>
+      <c r="AA9" s="81"/>
+      <c r="AB9" s="81"/>
+      <c r="AC9" s="82"/>
       <c r="AD9" s="51"/>
       <c r="AE9" s="52"/>
       <c r="AF9" s="52"/>
@@ -2601,18 +2689,18 @@
       <c r="O10" s="52"/>
       <c r="P10" s="52"/>
       <c r="Q10" s="53"/>
-      <c r="R10" s="51"/>
-      <c r="S10" s="52"/>
-      <c r="T10" s="52"/>
-      <c r="U10" s="52"/>
-      <c r="V10" s="52"/>
-      <c r="W10" s="53"/>
-      <c r="X10" s="51"/>
-      <c r="Y10" s="52"/>
-      <c r="Z10" s="52"/>
-      <c r="AA10" s="52"/>
-      <c r="AB10" s="52"/>
-      <c r="AC10" s="53"/>
+      <c r="R10" s="80"/>
+      <c r="S10" s="81"/>
+      <c r="T10" s="81"/>
+      <c r="U10" s="81"/>
+      <c r="V10" s="81"/>
+      <c r="W10" s="82"/>
+      <c r="X10" s="80"/>
+      <c r="Y10" s="81"/>
+      <c r="Z10" s="81"/>
+      <c r="AA10" s="81"/>
+      <c r="AB10" s="81"/>
+      <c r="AC10" s="82"/>
       <c r="AD10" s="51"/>
       <c r="AE10" s="52"/>
       <c r="AF10" s="52"/>
@@ -2674,18 +2762,18 @@
       <c r="O11" s="52"/>
       <c r="P11" s="52"/>
       <c r="Q11" s="53"/>
-      <c r="R11" s="51"/>
-      <c r="S11" s="52"/>
-      <c r="T11" s="52"/>
-      <c r="U11" s="52"/>
-      <c r="V11" s="52"/>
-      <c r="W11" s="53"/>
-      <c r="X11" s="51"/>
-      <c r="Y11" s="52"/>
-      <c r="Z11" s="52"/>
-      <c r="AA11" s="52"/>
-      <c r="AB11" s="52"/>
-      <c r="AC11" s="53"/>
+      <c r="R11" s="80"/>
+      <c r="S11" s="81"/>
+      <c r="T11" s="81"/>
+      <c r="U11" s="81"/>
+      <c r="V11" s="81"/>
+      <c r="W11" s="82"/>
+      <c r="X11" s="80"/>
+      <c r="Y11" s="81"/>
+      <c r="Z11" s="81"/>
+      <c r="AA11" s="81"/>
+      <c r="AB11" s="81"/>
+      <c r="AC11" s="82"/>
       <c r="AD11" s="51"/>
       <c r="AE11" s="52"/>
       <c r="AF11" s="52"/>
@@ -2747,18 +2835,18 @@
       <c r="O12" s="52"/>
       <c r="P12" s="52"/>
       <c r="Q12" s="53"/>
-      <c r="R12" s="51"/>
-      <c r="S12" s="52"/>
-      <c r="T12" s="52"/>
-      <c r="U12" s="52"/>
-      <c r="V12" s="52"/>
-      <c r="W12" s="53"/>
-      <c r="X12" s="51"/>
-      <c r="Y12" s="52"/>
-      <c r="Z12" s="52"/>
-      <c r="AA12" s="52"/>
-      <c r="AB12" s="52"/>
-      <c r="AC12" s="53"/>
+      <c r="R12" s="80"/>
+      <c r="S12" s="81"/>
+      <c r="T12" s="81"/>
+      <c r="U12" s="81"/>
+      <c r="V12" s="81"/>
+      <c r="W12" s="82"/>
+      <c r="X12" s="80"/>
+      <c r="Y12" s="81"/>
+      <c r="Z12" s="81"/>
+      <c r="AA12" s="81"/>
+      <c r="AB12" s="81"/>
+      <c r="AC12" s="82"/>
       <c r="AD12" s="51"/>
       <c r="AE12" s="52"/>
       <c r="AF12" s="52"/>
@@ -2820,18 +2908,18 @@
       <c r="O13" s="52"/>
       <c r="P13" s="52"/>
       <c r="Q13" s="53"/>
-      <c r="R13" s="51"/>
-      <c r="S13" s="52"/>
-      <c r="T13" s="52"/>
-      <c r="U13" s="52"/>
-      <c r="V13" s="52"/>
-      <c r="W13" s="53"/>
-      <c r="X13" s="51"/>
-      <c r="Y13" s="52"/>
-      <c r="Z13" s="52"/>
-      <c r="AA13" s="52"/>
-      <c r="AB13" s="52"/>
-      <c r="AC13" s="53"/>
+      <c r="R13" s="80"/>
+      <c r="S13" s="81"/>
+      <c r="T13" s="81"/>
+      <c r="U13" s="81"/>
+      <c r="V13" s="81"/>
+      <c r="W13" s="82"/>
+      <c r="X13" s="80"/>
+      <c r="Y13" s="81"/>
+      <c r="Z13" s="81"/>
+      <c r="AA13" s="81"/>
+      <c r="AB13" s="81"/>
+      <c r="AC13" s="82"/>
       <c r="AD13" s="51"/>
       <c r="AE13" s="52"/>
       <c r="AF13" s="52"/>
@@ -2893,18 +2981,18 @@
       <c r="O14" s="55"/>
       <c r="P14" s="55"/>
       <c r="Q14" s="56"/>
-      <c r="R14" s="54"/>
-      <c r="S14" s="55"/>
-      <c r="T14" s="55"/>
-      <c r="U14" s="55"/>
-      <c r="V14" s="55"/>
-      <c r="W14" s="56"/>
-      <c r="X14" s="54"/>
-      <c r="Y14" s="55"/>
-      <c r="Z14" s="55"/>
-      <c r="AA14" s="55"/>
-      <c r="AB14" s="55"/>
-      <c r="AC14" s="56"/>
+      <c r="R14" s="80"/>
+      <c r="S14" s="81"/>
+      <c r="T14" s="81"/>
+      <c r="U14" s="81"/>
+      <c r="V14" s="81"/>
+      <c r="W14" s="82"/>
+      <c r="X14" s="80"/>
+      <c r="Y14" s="81"/>
+      <c r="Z14" s="81"/>
+      <c r="AA14" s="81"/>
+      <c r="AB14" s="81"/>
+      <c r="AC14" s="82"/>
       <c r="AD14" s="54"/>
       <c r="AE14" s="55"/>
       <c r="AF14" s="55"/>
@@ -2968,18 +3056,18 @@
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
       <c r="Q15" s="5"/>
-      <c r="R15" s="6"/>
-      <c r="S15" s="4"/>
-      <c r="T15" s="4"/>
-      <c r="U15" s="4"/>
-      <c r="V15" s="4"/>
-      <c r="W15" s="5"/>
-      <c r="X15" s="6"/>
-      <c r="Y15" s="4"/>
-      <c r="Z15" s="4"/>
-      <c r="AA15" s="4"/>
-      <c r="AB15" s="4"/>
-      <c r="AC15" s="5"/>
+      <c r="R15" s="80"/>
+      <c r="S15" s="81"/>
+      <c r="T15" s="81"/>
+      <c r="U15" s="81"/>
+      <c r="V15" s="81"/>
+      <c r="W15" s="82"/>
+      <c r="X15" s="80"/>
+      <c r="Y15" s="81"/>
+      <c r="Z15" s="81"/>
+      <c r="AA15" s="81"/>
+      <c r="AB15" s="81"/>
+      <c r="AC15" s="82"/>
       <c r="AD15" s="6"/>
       <c r="AE15" s="4"/>
       <c r="AF15" s="4"/>
@@ -3045,18 +3133,18 @@
       <c r="O16" s="49"/>
       <c r="P16" s="49"/>
       <c r="Q16" s="50"/>
-      <c r="R16" s="48"/>
-      <c r="S16" s="49"/>
-      <c r="T16" s="49"/>
-      <c r="U16" s="49"/>
-      <c r="V16" s="49"/>
-      <c r="W16" s="50"/>
-      <c r="X16" s="48"/>
-      <c r="Y16" s="49"/>
-      <c r="Z16" s="49"/>
-      <c r="AA16" s="49"/>
-      <c r="AB16" s="49"/>
-      <c r="AC16" s="50"/>
+      <c r="R16" s="80"/>
+      <c r="S16" s="81"/>
+      <c r="T16" s="81"/>
+      <c r="U16" s="81"/>
+      <c r="V16" s="81"/>
+      <c r="W16" s="82"/>
+      <c r="X16" s="80"/>
+      <c r="Y16" s="81"/>
+      <c r="Z16" s="81"/>
+      <c r="AA16" s="81"/>
+      <c r="AB16" s="81"/>
+      <c r="AC16" s="82"/>
       <c r="AD16" s="48"/>
       <c r="AE16" s="49"/>
       <c r="AF16" s="49"/>
@@ -3128,18 +3216,18 @@
       <c r="O17" s="52"/>
       <c r="P17" s="52"/>
       <c r="Q17" s="53"/>
-      <c r="R17" s="51"/>
-      <c r="S17" s="52"/>
-      <c r="T17" s="52"/>
-      <c r="U17" s="52"/>
-      <c r="V17" s="52"/>
-      <c r="W17" s="53"/>
-      <c r="X17" s="51"/>
-      <c r="Y17" s="52"/>
-      <c r="Z17" s="52"/>
-      <c r="AA17" s="52"/>
-      <c r="AB17" s="52"/>
-      <c r="AC17" s="53"/>
+      <c r="R17" s="80"/>
+      <c r="S17" s="81"/>
+      <c r="T17" s="81"/>
+      <c r="U17" s="81"/>
+      <c r="V17" s="81"/>
+      <c r="W17" s="82"/>
+      <c r="X17" s="80"/>
+      <c r="Y17" s="81"/>
+      <c r="Z17" s="81"/>
+      <c r="AA17" s="81"/>
+      <c r="AB17" s="81"/>
+      <c r="AC17" s="82"/>
       <c r="AD17" s="51"/>
       <c r="AE17" s="52"/>
       <c r="AF17" s="52"/>
@@ -3209,18 +3297,18 @@
         <v>31</v>
       </c>
       <c r="Q18" s="53"/>
-      <c r="R18" s="51"/>
-      <c r="S18" s="52"/>
-      <c r="T18" s="52"/>
-      <c r="U18" s="52"/>
-      <c r="V18" s="52"/>
-      <c r="W18" s="53"/>
-      <c r="X18" s="51"/>
-      <c r="Y18" s="52"/>
-      <c r="Z18" s="52"/>
-      <c r="AA18" s="52"/>
-      <c r="AB18" s="52"/>
-      <c r="AC18" s="53"/>
+      <c r="R18" s="80"/>
+      <c r="S18" s="81"/>
+      <c r="T18" s="81"/>
+      <c r="U18" s="81"/>
+      <c r="V18" s="81"/>
+      <c r="W18" s="82"/>
+      <c r="X18" s="80"/>
+      <c r="Y18" s="81"/>
+      <c r="Z18" s="81"/>
+      <c r="AA18" s="81"/>
+      <c r="AB18" s="81"/>
+      <c r="AC18" s="82"/>
       <c r="AD18" s="51"/>
       <c r="AE18" s="52"/>
       <c r="AF18" s="52"/>
@@ -3282,18 +3370,18 @@
       <c r="O19" s="52"/>
       <c r="P19" s="52"/>
       <c r="Q19" s="53"/>
-      <c r="R19" s="51"/>
-      <c r="S19" s="52"/>
-      <c r="T19" s="52"/>
-      <c r="U19" s="52"/>
-      <c r="V19" s="52"/>
-      <c r="W19" s="53"/>
-      <c r="X19" s="51"/>
-      <c r="Y19" s="52"/>
-      <c r="Z19" s="52"/>
-      <c r="AA19" s="52"/>
-      <c r="AB19" s="52"/>
-      <c r="AC19" s="53"/>
+      <c r="R19" s="80"/>
+      <c r="S19" s="81"/>
+      <c r="T19" s="81"/>
+      <c r="U19" s="81"/>
+      <c r="V19" s="81"/>
+      <c r="W19" s="82"/>
+      <c r="X19" s="80"/>
+      <c r="Y19" s="81"/>
+      <c r="Z19" s="81"/>
+      <c r="AA19" s="81"/>
+      <c r="AB19" s="81"/>
+      <c r="AC19" s="82"/>
       <c r="AD19" s="51"/>
       <c r="AE19" s="52"/>
       <c r="AF19" s="52"/>
@@ -3355,18 +3443,18 @@
       <c r="O20" s="52"/>
       <c r="P20" s="52"/>
       <c r="Q20" s="53"/>
-      <c r="R20" s="51"/>
-      <c r="S20" s="52"/>
-      <c r="T20" s="52"/>
-      <c r="U20" s="52"/>
-      <c r="V20" s="52"/>
-      <c r="W20" s="53"/>
-      <c r="X20" s="51"/>
-      <c r="Y20" s="52"/>
-      <c r="Z20" s="52"/>
-      <c r="AA20" s="52"/>
-      <c r="AB20" s="52"/>
-      <c r="AC20" s="53"/>
+      <c r="R20" s="80"/>
+      <c r="S20" s="81"/>
+      <c r="T20" s="81"/>
+      <c r="U20" s="81"/>
+      <c r="V20" s="81"/>
+      <c r="W20" s="82"/>
+      <c r="X20" s="80"/>
+      <c r="Y20" s="81"/>
+      <c r="Z20" s="81"/>
+      <c r="AA20" s="81"/>
+      <c r="AB20" s="81"/>
+      <c r="AC20" s="82"/>
       <c r="AD20" s="51"/>
       <c r="AE20" s="52"/>
       <c r="AF20" s="52"/>
@@ -3428,18 +3516,18 @@
       <c r="O21" s="52"/>
       <c r="P21" s="52"/>
       <c r="Q21" s="53"/>
-      <c r="R21" s="51"/>
-      <c r="S21" s="52"/>
-      <c r="T21" s="52"/>
-      <c r="U21" s="52"/>
-      <c r="V21" s="52"/>
-      <c r="W21" s="53"/>
-      <c r="X21" s="51"/>
-      <c r="Y21" s="52"/>
-      <c r="Z21" s="52"/>
-      <c r="AA21" s="52"/>
-      <c r="AB21" s="52"/>
-      <c r="AC21" s="53"/>
+      <c r="R21" s="80"/>
+      <c r="S21" s="81"/>
+      <c r="T21" s="81"/>
+      <c r="U21" s="81"/>
+      <c r="V21" s="81"/>
+      <c r="W21" s="82"/>
+      <c r="X21" s="80"/>
+      <c r="Y21" s="81"/>
+      <c r="Z21" s="81"/>
+      <c r="AA21" s="81"/>
+      <c r="AB21" s="81"/>
+      <c r="AC21" s="82"/>
       <c r="AD21" s="51"/>
       <c r="AE21" s="52"/>
       <c r="AF21" s="52"/>
@@ -3501,18 +3589,18 @@
       <c r="O22" s="52"/>
       <c r="P22" s="52"/>
       <c r="Q22" s="53"/>
-      <c r="R22" s="51"/>
-      <c r="S22" s="52"/>
-      <c r="T22" s="52"/>
-      <c r="U22" s="52"/>
-      <c r="V22" s="52"/>
-      <c r="W22" s="53"/>
-      <c r="X22" s="51"/>
-      <c r="Y22" s="52"/>
-      <c r="Z22" s="52"/>
-      <c r="AA22" s="52"/>
-      <c r="AB22" s="52"/>
-      <c r="AC22" s="53"/>
+      <c r="R22" s="80"/>
+      <c r="S22" s="81"/>
+      <c r="T22" s="81"/>
+      <c r="U22" s="81"/>
+      <c r="V22" s="81"/>
+      <c r="W22" s="82"/>
+      <c r="X22" s="80"/>
+      <c r="Y22" s="81"/>
+      <c r="Z22" s="81"/>
+      <c r="AA22" s="81"/>
+      <c r="AB22" s="81"/>
+      <c r="AC22" s="82"/>
       <c r="AD22" s="51"/>
       <c r="AE22" s="52"/>
       <c r="AF22" s="52"/>
@@ -3574,18 +3662,18 @@
       <c r="O23" s="52"/>
       <c r="P23" s="52"/>
       <c r="Q23" s="53"/>
-      <c r="R23" s="51"/>
-      <c r="S23" s="52"/>
-      <c r="T23" s="52"/>
-      <c r="U23" s="52"/>
-      <c r="V23" s="52"/>
-      <c r="W23" s="53"/>
-      <c r="X23" s="51"/>
-      <c r="Y23" s="52"/>
-      <c r="Z23" s="52"/>
-      <c r="AA23" s="52"/>
-      <c r="AB23" s="52"/>
-      <c r="AC23" s="53"/>
+      <c r="R23" s="80"/>
+      <c r="S23" s="81"/>
+      <c r="T23" s="81"/>
+      <c r="U23" s="81"/>
+      <c r="V23" s="81"/>
+      <c r="W23" s="82"/>
+      <c r="X23" s="80"/>
+      <c r="Y23" s="81"/>
+      <c r="Z23" s="81"/>
+      <c r="AA23" s="81"/>
+      <c r="AB23" s="81"/>
+      <c r="AC23" s="82"/>
       <c r="AD23" s="51"/>
       <c r="AE23" s="52"/>
       <c r="AF23" s="52"/>
@@ -3647,18 +3735,18 @@
       <c r="O24" s="52"/>
       <c r="P24" s="52"/>
       <c r="Q24" s="53"/>
-      <c r="R24" s="51"/>
-      <c r="S24" s="52"/>
-      <c r="T24" s="52"/>
-      <c r="U24" s="52"/>
-      <c r="V24" s="52"/>
-      <c r="W24" s="53"/>
-      <c r="X24" s="51"/>
-      <c r="Y24" s="52"/>
-      <c r="Z24" s="52"/>
-      <c r="AA24" s="52"/>
-      <c r="AB24" s="52"/>
-      <c r="AC24" s="53"/>
+      <c r="R24" s="80"/>
+      <c r="S24" s="81"/>
+      <c r="T24" s="81"/>
+      <c r="U24" s="81"/>
+      <c r="V24" s="81"/>
+      <c r="W24" s="82"/>
+      <c r="X24" s="80"/>
+      <c r="Y24" s="81"/>
+      <c r="Z24" s="81"/>
+      <c r="AA24" s="81"/>
+      <c r="AB24" s="81"/>
+      <c r="AC24" s="82"/>
       <c r="AD24" s="51"/>
       <c r="AE24" s="52"/>
       <c r="AF24" s="52"/>
@@ -3720,18 +3808,18 @@
       <c r="O25" s="55"/>
       <c r="P25" s="55"/>
       <c r="Q25" s="56"/>
-      <c r="R25" s="54"/>
-      <c r="S25" s="55"/>
-      <c r="T25" s="55"/>
-      <c r="U25" s="55"/>
-      <c r="V25" s="55"/>
-      <c r="W25" s="56"/>
-      <c r="X25" s="54"/>
-      <c r="Y25" s="55"/>
-      <c r="Z25" s="55"/>
-      <c r="AA25" s="55"/>
-      <c r="AB25" s="55"/>
-      <c r="AC25" s="56"/>
+      <c r="R25" s="80"/>
+      <c r="S25" s="81"/>
+      <c r="T25" s="81"/>
+      <c r="U25" s="81"/>
+      <c r="V25" s="81"/>
+      <c r="W25" s="82"/>
+      <c r="X25" s="80"/>
+      <c r="Y25" s="81"/>
+      <c r="Z25" s="81"/>
+      <c r="AA25" s="81"/>
+      <c r="AB25" s="81"/>
+      <c r="AC25" s="82"/>
       <c r="AD25" s="54"/>
       <c r="AE25" s="55"/>
       <c r="AF25" s="55"/>
@@ -3795,18 +3883,18 @@
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
       <c r="Q26" s="5"/>
-      <c r="R26" s="6"/>
-      <c r="S26" s="4"/>
-      <c r="T26" s="4"/>
-      <c r="U26" s="4"/>
-      <c r="V26" s="4"/>
-      <c r="W26" s="5"/>
-      <c r="X26" s="6"/>
-      <c r="Y26" s="4"/>
-      <c r="Z26" s="4"/>
-      <c r="AA26" s="4"/>
-      <c r="AB26" s="4"/>
-      <c r="AC26" s="5"/>
+      <c r="R26" s="80"/>
+      <c r="S26" s="81"/>
+      <c r="T26" s="81"/>
+      <c r="U26" s="81"/>
+      <c r="V26" s="81"/>
+      <c r="W26" s="82"/>
+      <c r="X26" s="80"/>
+      <c r="Y26" s="81"/>
+      <c r="Z26" s="81"/>
+      <c r="AA26" s="81"/>
+      <c r="AB26" s="81"/>
+      <c r="AC26" s="82"/>
       <c r="AD26" s="6"/>
       <c r="AE26" s="4"/>
       <c r="AF26" s="4"/>
@@ -3874,18 +3962,18 @@
       <c r="O27" s="49"/>
       <c r="P27" s="49"/>
       <c r="Q27" s="50"/>
-      <c r="R27" s="48"/>
-      <c r="S27" s="49"/>
-      <c r="T27" s="49"/>
-      <c r="U27" s="49"/>
-      <c r="V27" s="49"/>
-      <c r="W27" s="50"/>
-      <c r="X27" s="48"/>
-      <c r="Y27" s="49"/>
-      <c r="Z27" s="49"/>
-      <c r="AA27" s="49"/>
-      <c r="AB27" s="49"/>
-      <c r="AC27" s="50"/>
+      <c r="R27" s="80"/>
+      <c r="S27" s="81"/>
+      <c r="T27" s="81"/>
+      <c r="U27" s="81"/>
+      <c r="V27" s="81"/>
+      <c r="W27" s="82"/>
+      <c r="X27" s="80"/>
+      <c r="Y27" s="81"/>
+      <c r="Z27" s="81"/>
+      <c r="AA27" s="81"/>
+      <c r="AB27" s="81"/>
+      <c r="AC27" s="82"/>
       <c r="AD27" s="48"/>
       <c r="AE27" s="49"/>
       <c r="AF27" s="49"/>
@@ -3953,18 +4041,18 @@
       <c r="O28" s="52"/>
       <c r="P28" s="52"/>
       <c r="Q28" s="53"/>
-      <c r="R28" s="51"/>
-      <c r="S28" s="52"/>
-      <c r="T28" s="52"/>
-      <c r="U28" s="52"/>
-      <c r="V28" s="52"/>
-      <c r="W28" s="53"/>
-      <c r="X28" s="51"/>
-      <c r="Y28" s="52"/>
-      <c r="Z28" s="52"/>
-      <c r="AA28" s="52"/>
-      <c r="AB28" s="52"/>
-      <c r="AC28" s="53"/>
+      <c r="R28" s="80"/>
+      <c r="S28" s="81"/>
+      <c r="T28" s="81"/>
+      <c r="U28" s="81"/>
+      <c r="V28" s="81"/>
+      <c r="W28" s="82"/>
+      <c r="X28" s="80"/>
+      <c r="Y28" s="81"/>
+      <c r="Z28" s="81"/>
+      <c r="AA28" s="81"/>
+      <c r="AB28" s="81"/>
+      <c r="AC28" s="82"/>
       <c r="AD28" s="51"/>
       <c r="AE28" s="52"/>
       <c r="AF28" s="52"/>
@@ -4028,18 +4116,18 @@
       <c r="O29" s="52"/>
       <c r="P29" s="52"/>
       <c r="Q29" s="53"/>
-      <c r="R29" s="51"/>
-      <c r="S29" s="52"/>
-      <c r="T29" s="52"/>
-      <c r="U29" s="52"/>
-      <c r="V29" s="52"/>
-      <c r="W29" s="53"/>
-      <c r="X29" s="51"/>
-      <c r="Y29" s="52"/>
-      <c r="Z29" s="52"/>
-      <c r="AA29" s="52"/>
-      <c r="AB29" s="52"/>
-      <c r="AC29" s="53"/>
+      <c r="R29" s="80"/>
+      <c r="S29" s="81"/>
+      <c r="T29" s="81"/>
+      <c r="U29" s="81"/>
+      <c r="V29" s="81"/>
+      <c r="W29" s="82"/>
+      <c r="X29" s="80"/>
+      <c r="Y29" s="81"/>
+      <c r="Z29" s="81"/>
+      <c r="AA29" s="81"/>
+      <c r="AB29" s="81"/>
+      <c r="AC29" s="82"/>
       <c r="AD29" s="51"/>
       <c r="AE29" s="52"/>
       <c r="AF29" s="52"/>
@@ -4101,18 +4189,18 @@
       <c r="O30" s="52"/>
       <c r="P30" s="52"/>
       <c r="Q30" s="53"/>
-      <c r="R30" s="51"/>
-      <c r="S30" s="52"/>
-      <c r="T30" s="52"/>
-      <c r="U30" s="52"/>
-      <c r="V30" s="52"/>
-      <c r="W30" s="53"/>
-      <c r="X30" s="51"/>
-      <c r="Y30" s="52"/>
-      <c r="Z30" s="52"/>
-      <c r="AA30" s="52"/>
-      <c r="AB30" s="52"/>
-      <c r="AC30" s="53"/>
+      <c r="R30" s="80"/>
+      <c r="S30" s="81"/>
+      <c r="T30" s="81"/>
+      <c r="U30" s="81"/>
+      <c r="V30" s="81"/>
+      <c r="W30" s="82"/>
+      <c r="X30" s="80"/>
+      <c r="Y30" s="81"/>
+      <c r="Z30" s="81"/>
+      <c r="AA30" s="81"/>
+      <c r="AB30" s="81"/>
+      <c r="AC30" s="82"/>
       <c r="AD30" s="51"/>
       <c r="AE30" s="52"/>
       <c r="AF30" s="52"/>
@@ -4174,18 +4262,18 @@
       <c r="O31" s="52"/>
       <c r="P31" s="52"/>
       <c r="Q31" s="53"/>
-      <c r="R31" s="51"/>
-      <c r="S31" s="52"/>
-      <c r="T31" s="52"/>
-      <c r="U31" s="52"/>
-      <c r="V31" s="52"/>
-      <c r="W31" s="53"/>
-      <c r="X31" s="51"/>
-      <c r="Y31" s="52"/>
-      <c r="Z31" s="52"/>
-      <c r="AA31" s="52"/>
-      <c r="AB31" s="52"/>
-      <c r="AC31" s="53"/>
+      <c r="R31" s="80"/>
+      <c r="S31" s="81"/>
+      <c r="T31" s="81"/>
+      <c r="U31" s="81"/>
+      <c r="V31" s="81"/>
+      <c r="W31" s="82"/>
+      <c r="X31" s="80"/>
+      <c r="Y31" s="81"/>
+      <c r="Z31" s="81"/>
+      <c r="AA31" s="81"/>
+      <c r="AB31" s="81"/>
+      <c r="AC31" s="82"/>
       <c r="AD31" s="51"/>
       <c r="AE31" s="52"/>
       <c r="AF31" s="52"/>
@@ -4247,18 +4335,18 @@
       <c r="O32" s="52"/>
       <c r="P32" s="52"/>
       <c r="Q32" s="53"/>
-      <c r="R32" s="51"/>
-      <c r="S32" s="52"/>
-      <c r="T32" s="52"/>
-      <c r="U32" s="52"/>
-      <c r="V32" s="52"/>
-      <c r="W32" s="53"/>
-      <c r="X32" s="51"/>
-      <c r="Y32" s="52"/>
-      <c r="Z32" s="52"/>
-      <c r="AA32" s="52"/>
-      <c r="AB32" s="52"/>
-      <c r="AC32" s="53"/>
+      <c r="R32" s="80"/>
+      <c r="S32" s="81"/>
+      <c r="T32" s="81"/>
+      <c r="U32" s="81"/>
+      <c r="V32" s="81"/>
+      <c r="W32" s="82"/>
+      <c r="X32" s="80"/>
+      <c r="Y32" s="81"/>
+      <c r="Z32" s="81"/>
+      <c r="AA32" s="81"/>
+      <c r="AB32" s="81"/>
+      <c r="AC32" s="82"/>
       <c r="AD32" s="51"/>
       <c r="AE32" s="52"/>
       <c r="AF32" s="52"/>
@@ -4320,18 +4408,18 @@
       <c r="O33" s="52"/>
       <c r="P33" s="52"/>
       <c r="Q33" s="53"/>
-      <c r="R33" s="51"/>
-      <c r="S33" s="52"/>
-      <c r="T33" s="52"/>
-      <c r="U33" s="52"/>
-      <c r="V33" s="52"/>
-      <c r="W33" s="53"/>
-      <c r="X33" s="51"/>
-      <c r="Y33" s="52"/>
-      <c r="Z33" s="52"/>
-      <c r="AA33" s="52"/>
-      <c r="AB33" s="52"/>
-      <c r="AC33" s="53"/>
+      <c r="R33" s="80"/>
+      <c r="S33" s="81"/>
+      <c r="T33" s="81"/>
+      <c r="U33" s="81"/>
+      <c r="V33" s="81"/>
+      <c r="W33" s="82"/>
+      <c r="X33" s="80"/>
+      <c r="Y33" s="81"/>
+      <c r="Z33" s="81"/>
+      <c r="AA33" s="81"/>
+      <c r="AB33" s="81"/>
+      <c r="AC33" s="82"/>
       <c r="AD33" s="51"/>
       <c r="AE33" s="52"/>
       <c r="AF33" s="52"/>
@@ -4393,18 +4481,18 @@
       <c r="O34" s="52"/>
       <c r="P34" s="52"/>
       <c r="Q34" s="53"/>
-      <c r="R34" s="51"/>
-      <c r="S34" s="52"/>
-      <c r="T34" s="52"/>
-      <c r="U34" s="52"/>
-      <c r="V34" s="52"/>
-      <c r="W34" s="53"/>
-      <c r="X34" s="51"/>
-      <c r="Y34" s="52"/>
-      <c r="Z34" s="52"/>
-      <c r="AA34" s="52"/>
-      <c r="AB34" s="52"/>
-      <c r="AC34" s="53"/>
+      <c r="R34" s="80"/>
+      <c r="S34" s="81"/>
+      <c r="T34" s="81"/>
+      <c r="U34" s="81"/>
+      <c r="V34" s="81"/>
+      <c r="W34" s="82"/>
+      <c r="X34" s="80"/>
+      <c r="Y34" s="81"/>
+      <c r="Z34" s="81"/>
+      <c r="AA34" s="81"/>
+      <c r="AB34" s="81"/>
+      <c r="AC34" s="82"/>
       <c r="AD34" s="51"/>
       <c r="AE34" s="52"/>
       <c r="AF34" s="52"/>
@@ -4466,18 +4554,18 @@
       <c r="O35" s="52"/>
       <c r="P35" s="52"/>
       <c r="Q35" s="53"/>
-      <c r="R35" s="51"/>
-      <c r="S35" s="52"/>
-      <c r="T35" s="52"/>
-      <c r="U35" s="52"/>
-      <c r="V35" s="52"/>
-      <c r="W35" s="53"/>
-      <c r="X35" s="51"/>
-      <c r="Y35" s="52"/>
-      <c r="Z35" s="52"/>
-      <c r="AA35" s="52"/>
-      <c r="AB35" s="52"/>
-      <c r="AC35" s="53"/>
+      <c r="R35" s="80"/>
+      <c r="S35" s="81"/>
+      <c r="T35" s="81"/>
+      <c r="U35" s="81"/>
+      <c r="V35" s="81"/>
+      <c r="W35" s="82"/>
+      <c r="X35" s="80"/>
+      <c r="Y35" s="81"/>
+      <c r="Z35" s="81"/>
+      <c r="AA35" s="81"/>
+      <c r="AB35" s="81"/>
+      <c r="AC35" s="82"/>
       <c r="AD35" s="51"/>
       <c r="AE35" s="52"/>
       <c r="AF35" s="52"/>
@@ -4539,18 +4627,18 @@
       <c r="O36" s="55"/>
       <c r="P36" s="55"/>
       <c r="Q36" s="56"/>
-      <c r="R36" s="54"/>
-      <c r="S36" s="55"/>
-      <c r="T36" s="55"/>
-      <c r="U36" s="55"/>
-      <c r="V36" s="55"/>
-      <c r="W36" s="56"/>
-      <c r="X36" s="54"/>
-      <c r="Y36" s="55"/>
-      <c r="Z36" s="55"/>
-      <c r="AA36" s="55"/>
-      <c r="AB36" s="55"/>
-      <c r="AC36" s="56"/>
+      <c r="R36" s="80"/>
+      <c r="S36" s="81"/>
+      <c r="T36" s="81"/>
+      <c r="U36" s="81"/>
+      <c r="V36" s="81"/>
+      <c r="W36" s="82"/>
+      <c r="X36" s="80"/>
+      <c r="Y36" s="81"/>
+      <c r="Z36" s="81"/>
+      <c r="AA36" s="81"/>
+      <c r="AB36" s="81"/>
+      <c r="AC36" s="82"/>
       <c r="AD36" s="54"/>
       <c r="AE36" s="55"/>
       <c r="AF36" s="55"/>
@@ -4614,18 +4702,18 @@
       <c r="O37" s="4"/>
       <c r="P37" s="4"/>
       <c r="Q37" s="5"/>
-      <c r="R37" s="6"/>
-      <c r="S37" s="4"/>
-      <c r="T37" s="4"/>
-      <c r="U37" s="4"/>
-      <c r="V37" s="4"/>
-      <c r="W37" s="5"/>
-      <c r="X37" s="6"/>
-      <c r="Y37" s="4"/>
-      <c r="Z37" s="4"/>
-      <c r="AA37" s="4"/>
-      <c r="AB37" s="4"/>
-      <c r="AC37" s="5"/>
+      <c r="R37" s="80"/>
+      <c r="S37" s="81"/>
+      <c r="T37" s="81"/>
+      <c r="U37" s="81"/>
+      <c r="V37" s="81"/>
+      <c r="W37" s="82"/>
+      <c r="X37" s="80"/>
+      <c r="Y37" s="81"/>
+      <c r="Z37" s="81"/>
+      <c r="AA37" s="81"/>
+      <c r="AB37" s="81"/>
+      <c r="AC37" s="82"/>
       <c r="AD37" s="6"/>
       <c r="AE37" s="4"/>
       <c r="AF37" s="4"/>
@@ -4693,18 +4781,18 @@
       <c r="O38" s="49"/>
       <c r="P38" s="49"/>
       <c r="Q38" s="50"/>
-      <c r="R38" s="48"/>
-      <c r="S38" s="49"/>
-      <c r="T38" s="49"/>
-      <c r="U38" s="49"/>
-      <c r="V38" s="49"/>
-      <c r="W38" s="50"/>
-      <c r="X38" s="48"/>
-      <c r="Y38" s="49"/>
-      <c r="Z38" s="49"/>
-      <c r="AA38" s="49"/>
-      <c r="AB38" s="49"/>
-      <c r="AC38" s="50"/>
+      <c r="R38" s="80"/>
+      <c r="S38" s="81"/>
+      <c r="T38" s="81"/>
+      <c r="U38" s="81"/>
+      <c r="V38" s="81"/>
+      <c r="W38" s="82"/>
+      <c r="X38" s="80"/>
+      <c r="Y38" s="81"/>
+      <c r="Z38" s="81"/>
+      <c r="AA38" s="81"/>
+      <c r="AB38" s="81"/>
+      <c r="AC38" s="82"/>
       <c r="AD38" s="48"/>
       <c r="AE38" s="49"/>
       <c r="AF38" s="49"/>
@@ -4772,18 +4860,18 @@
       <c r="Q39" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="R39" s="51"/>
-      <c r="S39" s="52"/>
-      <c r="T39" s="52"/>
-      <c r="U39" s="52"/>
-      <c r="V39" s="52"/>
-      <c r="W39" s="53"/>
-      <c r="X39" s="51"/>
-      <c r="Y39" s="52"/>
-      <c r="Z39" s="52"/>
-      <c r="AA39" s="52"/>
-      <c r="AB39" s="52"/>
-      <c r="AC39" s="53"/>
+      <c r="R39" s="80"/>
+      <c r="S39" s="81"/>
+      <c r="T39" s="81"/>
+      <c r="U39" s="81"/>
+      <c r="V39" s="81"/>
+      <c r="W39" s="82"/>
+      <c r="X39" s="80"/>
+      <c r="Y39" s="81"/>
+      <c r="Z39" s="81"/>
+      <c r="AA39" s="81"/>
+      <c r="AB39" s="81"/>
+      <c r="AC39" s="82"/>
       <c r="AD39" s="51" t="s">
         <v>31</v>
       </c>
@@ -4857,18 +4945,18 @@
       <c r="Q40" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="R40" s="51"/>
-      <c r="S40" s="52"/>
-      <c r="T40" s="52"/>
-      <c r="U40" s="52"/>
-      <c r="V40" s="52"/>
-      <c r="W40" s="53"/>
-      <c r="X40" s="51"/>
-      <c r="Y40" s="52"/>
-      <c r="Z40" s="52"/>
-      <c r="AA40" s="52"/>
-      <c r="AB40" s="52"/>
-      <c r="AC40" s="53"/>
+      <c r="R40" s="80"/>
+      <c r="S40" s="81"/>
+      <c r="T40" s="81"/>
+      <c r="U40" s="81"/>
+      <c r="V40" s="81"/>
+      <c r="W40" s="82"/>
+      <c r="X40" s="80"/>
+      <c r="Y40" s="81"/>
+      <c r="Z40" s="81"/>
+      <c r="AA40" s="81"/>
+      <c r="AB40" s="81"/>
+      <c r="AC40" s="82"/>
       <c r="AD40" s="51" t="s">
         <v>31</v>
       </c>
@@ -4942,18 +5030,18 @@
       <c r="Q41" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="R41" s="51"/>
-      <c r="S41" s="52"/>
-      <c r="T41" s="52"/>
-      <c r="U41" s="52"/>
-      <c r="V41" s="52"/>
-      <c r="W41" s="53"/>
-      <c r="X41" s="51"/>
-      <c r="Y41" s="52"/>
-      <c r="Z41" s="52"/>
-      <c r="AA41" s="52"/>
-      <c r="AB41" s="52"/>
-      <c r="AC41" s="53"/>
+      <c r="R41" s="80"/>
+      <c r="S41" s="81"/>
+      <c r="T41" s="81"/>
+      <c r="U41" s="81"/>
+      <c r="V41" s="81"/>
+      <c r="W41" s="82"/>
+      <c r="X41" s="80"/>
+      <c r="Y41" s="81"/>
+      <c r="Z41" s="81"/>
+      <c r="AA41" s="81"/>
+      <c r="AB41" s="81"/>
+      <c r="AC41" s="82"/>
       <c r="AD41" s="51" t="s">
         <v>31</v>
       </c>
@@ -5021,18 +5109,18 @@
       <c r="O42" s="52"/>
       <c r="P42" s="52"/>
       <c r="Q42" s="53"/>
-      <c r="R42" s="51"/>
-      <c r="S42" s="52"/>
-      <c r="T42" s="52"/>
-      <c r="U42" s="52"/>
-      <c r="V42" s="52"/>
-      <c r="W42" s="53"/>
-      <c r="X42" s="51"/>
-      <c r="Y42" s="52"/>
-      <c r="Z42" s="52"/>
-      <c r="AA42" s="52"/>
-      <c r="AB42" s="52"/>
-      <c r="AC42" s="53"/>
+      <c r="R42" s="80"/>
+      <c r="S42" s="81"/>
+      <c r="T42" s="81"/>
+      <c r="U42" s="81"/>
+      <c r="V42" s="81"/>
+      <c r="W42" s="82"/>
+      <c r="X42" s="80"/>
+      <c r="Y42" s="81"/>
+      <c r="Z42" s="81"/>
+      <c r="AA42" s="81"/>
+      <c r="AB42" s="81"/>
+      <c r="AC42" s="82"/>
       <c r="AD42" s="51"/>
       <c r="AE42" s="52"/>
       <c r="AF42" s="52"/>
@@ -5094,18 +5182,18 @@
       <c r="O43" s="52"/>
       <c r="P43" s="52"/>
       <c r="Q43" s="53"/>
-      <c r="R43" s="51"/>
-      <c r="S43" s="52"/>
-      <c r="T43" s="52"/>
-      <c r="U43" s="52"/>
-      <c r="V43" s="52"/>
-      <c r="W43" s="53"/>
-      <c r="X43" s="51"/>
-      <c r="Y43" s="52"/>
-      <c r="Z43" s="52"/>
-      <c r="AA43" s="52"/>
-      <c r="AB43" s="52"/>
-      <c r="AC43" s="53"/>
+      <c r="R43" s="80"/>
+      <c r="S43" s="81"/>
+      <c r="T43" s="81"/>
+      <c r="U43" s="81"/>
+      <c r="V43" s="81"/>
+      <c r="W43" s="82"/>
+      <c r="X43" s="80"/>
+      <c r="Y43" s="81"/>
+      <c r="Z43" s="81"/>
+      <c r="AA43" s="81"/>
+      <c r="AB43" s="81"/>
+      <c r="AC43" s="82"/>
       <c r="AD43" s="51"/>
       <c r="AE43" s="52"/>
       <c r="AF43" s="52"/>
@@ -5167,18 +5255,18 @@
       <c r="O44" s="52"/>
       <c r="P44" s="52"/>
       <c r="Q44" s="53"/>
-      <c r="R44" s="51"/>
-      <c r="S44" s="52"/>
-      <c r="T44" s="52"/>
-      <c r="U44" s="52"/>
-      <c r="V44" s="52"/>
-      <c r="W44" s="53"/>
-      <c r="X44" s="51"/>
-      <c r="Y44" s="52"/>
-      <c r="Z44" s="52"/>
-      <c r="AA44" s="52"/>
-      <c r="AB44" s="52"/>
-      <c r="AC44" s="53"/>
+      <c r="R44" s="80"/>
+      <c r="S44" s="81"/>
+      <c r="T44" s="81"/>
+      <c r="U44" s="81"/>
+      <c r="V44" s="81"/>
+      <c r="W44" s="82"/>
+      <c r="X44" s="80"/>
+      <c r="Y44" s="81"/>
+      <c r="Z44" s="81"/>
+      <c r="AA44" s="81"/>
+      <c r="AB44" s="81"/>
+      <c r="AC44" s="82"/>
       <c r="AD44" s="51"/>
       <c r="AE44" s="52"/>
       <c r="AF44" s="52"/>
@@ -5240,18 +5328,18 @@
       <c r="O45" s="52"/>
       <c r="P45" s="52"/>
       <c r="Q45" s="53"/>
-      <c r="R45" s="51"/>
-      <c r="S45" s="52"/>
-      <c r="T45" s="52"/>
-      <c r="U45" s="52"/>
-      <c r="V45" s="52"/>
-      <c r="W45" s="53"/>
-      <c r="X45" s="51"/>
-      <c r="Y45" s="52"/>
-      <c r="Z45" s="52"/>
-      <c r="AA45" s="52"/>
-      <c r="AB45" s="52"/>
-      <c r="AC45" s="53"/>
+      <c r="R45" s="80"/>
+      <c r="S45" s="81"/>
+      <c r="T45" s="81"/>
+      <c r="U45" s="81"/>
+      <c r="V45" s="81"/>
+      <c r="W45" s="82"/>
+      <c r="X45" s="80"/>
+      <c r="Y45" s="81"/>
+      <c r="Z45" s="81"/>
+      <c r="AA45" s="81"/>
+      <c r="AB45" s="81"/>
+      <c r="AC45" s="82"/>
       <c r="AD45" s="51"/>
       <c r="AE45" s="52"/>
       <c r="AF45" s="52"/>
@@ -5313,18 +5401,18 @@
       <c r="O46" s="52"/>
       <c r="P46" s="52"/>
       <c r="Q46" s="53"/>
-      <c r="R46" s="51"/>
-      <c r="S46" s="52"/>
-      <c r="T46" s="52"/>
-      <c r="U46" s="52"/>
-      <c r="V46" s="52"/>
-      <c r="W46" s="53"/>
-      <c r="X46" s="51"/>
-      <c r="Y46" s="52"/>
-      <c r="Z46" s="52"/>
-      <c r="AA46" s="52"/>
-      <c r="AB46" s="52"/>
-      <c r="AC46" s="53"/>
+      <c r="R46" s="80"/>
+      <c r="S46" s="81"/>
+      <c r="T46" s="81"/>
+      <c r="U46" s="81"/>
+      <c r="V46" s="81"/>
+      <c r="W46" s="82"/>
+      <c r="X46" s="80"/>
+      <c r="Y46" s="81"/>
+      <c r="Z46" s="81"/>
+      <c r="AA46" s="81"/>
+      <c r="AB46" s="81"/>
+      <c r="AC46" s="82"/>
       <c r="AD46" s="51"/>
       <c r="AE46" s="52"/>
       <c r="AF46" s="52"/>
@@ -5386,18 +5474,18 @@
       <c r="O47" s="55"/>
       <c r="P47" s="55"/>
       <c r="Q47" s="56"/>
-      <c r="R47" s="54"/>
-      <c r="S47" s="55"/>
-      <c r="T47" s="55"/>
-      <c r="U47" s="55"/>
-      <c r="V47" s="55"/>
-      <c r="W47" s="56"/>
-      <c r="X47" s="54"/>
-      <c r="Y47" s="55"/>
-      <c r="Z47" s="55"/>
-      <c r="AA47" s="55"/>
-      <c r="AB47" s="55"/>
-      <c r="AC47" s="56"/>
+      <c r="R47" s="80"/>
+      <c r="S47" s="81"/>
+      <c r="T47" s="81"/>
+      <c r="U47" s="81"/>
+      <c r="V47" s="81"/>
+      <c r="W47" s="82"/>
+      <c r="X47" s="80"/>
+      <c r="Y47" s="81"/>
+      <c r="Z47" s="81"/>
+      <c r="AA47" s="81"/>
+      <c r="AB47" s="81"/>
+      <c r="AC47" s="82"/>
       <c r="AD47" s="54"/>
       <c r="AE47" s="55"/>
       <c r="AF47" s="55"/>
@@ -5461,18 +5549,18 @@
       <c r="O48" s="4"/>
       <c r="P48" s="4"/>
       <c r="Q48" s="5"/>
-      <c r="R48" s="6"/>
-      <c r="S48" s="4"/>
-      <c r="T48" s="4"/>
-      <c r="U48" s="4"/>
-      <c r="V48" s="4"/>
-      <c r="W48" s="5"/>
-      <c r="X48" s="6"/>
-      <c r="Y48" s="4"/>
-      <c r="Z48" s="4"/>
-      <c r="AA48" s="4"/>
-      <c r="AB48" s="4"/>
-      <c r="AC48" s="5"/>
+      <c r="R48" s="80"/>
+      <c r="S48" s="81"/>
+      <c r="T48" s="81"/>
+      <c r="U48" s="81"/>
+      <c r="V48" s="81"/>
+      <c r="W48" s="82"/>
+      <c r="X48" s="80"/>
+      <c r="Y48" s="81"/>
+      <c r="Z48" s="81"/>
+      <c r="AA48" s="81"/>
+      <c r="AB48" s="81"/>
+      <c r="AC48" s="82"/>
       <c r="AD48" s="6"/>
       <c r="AE48" s="4"/>
       <c r="AF48" s="4"/>
@@ -5536,18 +5624,18 @@
       <c r="O49" s="49"/>
       <c r="P49" s="49"/>
       <c r="Q49" s="50"/>
-      <c r="R49" s="48"/>
-      <c r="S49" s="49"/>
-      <c r="T49" s="49"/>
-      <c r="U49" s="49"/>
-      <c r="V49" s="49"/>
-      <c r="W49" s="50"/>
-      <c r="X49" s="48"/>
-      <c r="Y49" s="49"/>
-      <c r="Z49" s="49"/>
-      <c r="AA49" s="49"/>
-      <c r="AB49" s="49"/>
-      <c r="AC49" s="50"/>
+      <c r="R49" s="80"/>
+      <c r="S49" s="81"/>
+      <c r="T49" s="81"/>
+      <c r="U49" s="81"/>
+      <c r="V49" s="81"/>
+      <c r="W49" s="82"/>
+      <c r="X49" s="80"/>
+      <c r="Y49" s="81"/>
+      <c r="Z49" s="81"/>
+      <c r="AA49" s="81"/>
+      <c r="AB49" s="81"/>
+      <c r="AC49" s="82"/>
       <c r="AD49" s="48"/>
       <c r="AE49" s="49"/>
       <c r="AF49" s="49"/>
@@ -5611,18 +5699,18 @@
       <c r="O50" s="52"/>
       <c r="P50" s="52"/>
       <c r="Q50" s="53"/>
-      <c r="R50" s="51"/>
-      <c r="S50" s="52"/>
-      <c r="T50" s="52"/>
-      <c r="U50" s="52"/>
-      <c r="V50" s="52"/>
-      <c r="W50" s="53"/>
-      <c r="X50" s="51"/>
-      <c r="Y50" s="52"/>
-      <c r="Z50" s="52"/>
-      <c r="AA50" s="52"/>
-      <c r="AB50" s="52"/>
-      <c r="AC50" s="53"/>
+      <c r="R50" s="80"/>
+      <c r="S50" s="81"/>
+      <c r="T50" s="81"/>
+      <c r="U50" s="81"/>
+      <c r="V50" s="81"/>
+      <c r="W50" s="82"/>
+      <c r="X50" s="80"/>
+      <c r="Y50" s="81"/>
+      <c r="Z50" s="81"/>
+      <c r="AA50" s="81"/>
+      <c r="AB50" s="81"/>
+      <c r="AC50" s="82"/>
       <c r="AD50" s="51"/>
       <c r="AE50" s="52"/>
       <c r="AF50" s="52"/>
@@ -5684,18 +5772,18 @@
       <c r="O51" s="52"/>
       <c r="P51" s="52"/>
       <c r="Q51" s="53"/>
-      <c r="R51" s="51"/>
-      <c r="S51" s="52"/>
-      <c r="T51" s="52"/>
-      <c r="U51" s="52"/>
-      <c r="V51" s="52"/>
-      <c r="W51" s="53"/>
-      <c r="X51" s="51"/>
-      <c r="Y51" s="52"/>
-      <c r="Z51" s="52"/>
-      <c r="AA51" s="52"/>
-      <c r="AB51" s="52"/>
-      <c r="AC51" s="53"/>
+      <c r="R51" s="80"/>
+      <c r="S51" s="81"/>
+      <c r="T51" s="81"/>
+      <c r="U51" s="81"/>
+      <c r="V51" s="81"/>
+      <c r="W51" s="82"/>
+      <c r="X51" s="80"/>
+      <c r="Y51" s="81"/>
+      <c r="Z51" s="81"/>
+      <c r="AA51" s="81"/>
+      <c r="AB51" s="81"/>
+      <c r="AC51" s="82"/>
       <c r="AD51" s="51"/>
       <c r="AE51" s="52"/>
       <c r="AF51" s="52"/>
@@ -5757,18 +5845,18 @@
       <c r="O52" s="52"/>
       <c r="P52" s="52"/>
       <c r="Q52" s="53"/>
-      <c r="R52" s="51"/>
-      <c r="S52" s="52"/>
-      <c r="T52" s="52"/>
-      <c r="U52" s="52"/>
-      <c r="V52" s="52"/>
-      <c r="W52" s="53"/>
-      <c r="X52" s="51"/>
-      <c r="Y52" s="52"/>
-      <c r="Z52" s="52"/>
-      <c r="AA52" s="52"/>
-      <c r="AB52" s="52"/>
-      <c r="AC52" s="53"/>
+      <c r="R52" s="80"/>
+      <c r="S52" s="81"/>
+      <c r="T52" s="81"/>
+      <c r="U52" s="81"/>
+      <c r="V52" s="81"/>
+      <c r="W52" s="82"/>
+      <c r="X52" s="80"/>
+      <c r="Y52" s="81"/>
+      <c r="Z52" s="81"/>
+      <c r="AA52" s="81"/>
+      <c r="AB52" s="81"/>
+      <c r="AC52" s="82"/>
       <c r="AD52" s="51"/>
       <c r="AE52" s="52"/>
       <c r="AF52" s="52"/>
@@ -5830,18 +5918,18 @@
       <c r="O53" s="52"/>
       <c r="P53" s="52"/>
       <c r="Q53" s="53"/>
-      <c r="R53" s="51"/>
-      <c r="S53" s="52"/>
-      <c r="T53" s="52"/>
-      <c r="U53" s="52"/>
-      <c r="V53" s="52"/>
-      <c r="W53" s="53"/>
-      <c r="X53" s="51"/>
-      <c r="Y53" s="52"/>
-      <c r="Z53" s="52"/>
-      <c r="AA53" s="52"/>
-      <c r="AB53" s="52"/>
-      <c r="AC53" s="53"/>
+      <c r="R53" s="80"/>
+      <c r="S53" s="81"/>
+      <c r="T53" s="81"/>
+      <c r="U53" s="81"/>
+      <c r="V53" s="81"/>
+      <c r="W53" s="82"/>
+      <c r="X53" s="80"/>
+      <c r="Y53" s="81"/>
+      <c r="Z53" s="81"/>
+      <c r="AA53" s="81"/>
+      <c r="AB53" s="81"/>
+      <c r="AC53" s="82"/>
       <c r="AD53" s="51"/>
       <c r="AE53" s="52"/>
       <c r="AF53" s="52"/>
@@ -5903,18 +5991,18 @@
       <c r="O54" s="52"/>
       <c r="P54" s="52"/>
       <c r="Q54" s="53"/>
-      <c r="R54" s="51"/>
-      <c r="S54" s="52"/>
-      <c r="T54" s="52"/>
-      <c r="U54" s="52"/>
-      <c r="V54" s="52"/>
-      <c r="W54" s="53"/>
-      <c r="X54" s="51"/>
-      <c r="Y54" s="52"/>
-      <c r="Z54" s="52"/>
-      <c r="AA54" s="52"/>
-      <c r="AB54" s="52"/>
-      <c r="AC54" s="53"/>
+      <c r="R54" s="80"/>
+      <c r="S54" s="81"/>
+      <c r="T54" s="81"/>
+      <c r="U54" s="81"/>
+      <c r="V54" s="81"/>
+      <c r="W54" s="82"/>
+      <c r="X54" s="80"/>
+      <c r="Y54" s="81"/>
+      <c r="Z54" s="81"/>
+      <c r="AA54" s="81"/>
+      <c r="AB54" s="81"/>
+      <c r="AC54" s="82"/>
       <c r="AD54" s="51"/>
       <c r="AE54" s="52"/>
       <c r="AF54" s="52"/>
@@ -5976,18 +6064,18 @@
       <c r="O55" s="52"/>
       <c r="P55" s="52"/>
       <c r="Q55" s="53"/>
-      <c r="R55" s="51"/>
-      <c r="S55" s="52"/>
-      <c r="T55" s="52"/>
-      <c r="U55" s="52"/>
-      <c r="V55" s="52"/>
-      <c r="W55" s="53"/>
-      <c r="X55" s="51"/>
-      <c r="Y55" s="52"/>
-      <c r="Z55" s="52"/>
-      <c r="AA55" s="52"/>
-      <c r="AB55" s="52"/>
-      <c r="AC55" s="53"/>
+      <c r="R55" s="80"/>
+      <c r="S55" s="81"/>
+      <c r="T55" s="81"/>
+      <c r="U55" s="81"/>
+      <c r="V55" s="81"/>
+      <c r="W55" s="82"/>
+      <c r="X55" s="80"/>
+      <c r="Y55" s="81"/>
+      <c r="Z55" s="81"/>
+      <c r="AA55" s="81"/>
+      <c r="AB55" s="81"/>
+      <c r="AC55" s="82"/>
       <c r="AD55" s="51"/>
       <c r="AE55" s="52"/>
       <c r="AF55" s="52"/>
@@ -6049,18 +6137,18 @@
       <c r="O56" s="52"/>
       <c r="P56" s="52"/>
       <c r="Q56" s="53"/>
-      <c r="R56" s="51"/>
-      <c r="S56" s="52"/>
-      <c r="T56" s="52"/>
-      <c r="U56" s="52"/>
-      <c r="V56" s="52"/>
-      <c r="W56" s="53"/>
-      <c r="X56" s="51"/>
-      <c r="Y56" s="52"/>
-      <c r="Z56" s="52"/>
-      <c r="AA56" s="52"/>
-      <c r="AB56" s="52"/>
-      <c r="AC56" s="53"/>
+      <c r="R56" s="80"/>
+      <c r="S56" s="81"/>
+      <c r="T56" s="81"/>
+      <c r="U56" s="81"/>
+      <c r="V56" s="81"/>
+      <c r="W56" s="82"/>
+      <c r="X56" s="80"/>
+      <c r="Y56" s="81"/>
+      <c r="Z56" s="81"/>
+      <c r="AA56" s="81"/>
+      <c r="AB56" s="81"/>
+      <c r="AC56" s="82"/>
       <c r="AD56" s="51"/>
       <c r="AE56" s="52"/>
       <c r="AF56" s="52"/>
@@ -6122,18 +6210,18 @@
       <c r="O57" s="52"/>
       <c r="P57" s="52"/>
       <c r="Q57" s="53"/>
-      <c r="R57" s="51"/>
-      <c r="S57" s="52"/>
-      <c r="T57" s="52"/>
-      <c r="U57" s="52"/>
-      <c r="V57" s="52"/>
-      <c r="W57" s="53"/>
-      <c r="X57" s="51"/>
-      <c r="Y57" s="52"/>
-      <c r="Z57" s="52"/>
-      <c r="AA57" s="52"/>
-      <c r="AB57" s="52"/>
-      <c r="AC57" s="53"/>
+      <c r="R57" s="80"/>
+      <c r="S57" s="81"/>
+      <c r="T57" s="81"/>
+      <c r="U57" s="81"/>
+      <c r="V57" s="81"/>
+      <c r="W57" s="82"/>
+      <c r="X57" s="80"/>
+      <c r="Y57" s="81"/>
+      <c r="Z57" s="81"/>
+      <c r="AA57" s="81"/>
+      <c r="AB57" s="81"/>
+      <c r="AC57" s="82"/>
       <c r="AD57" s="51"/>
       <c r="AE57" s="52"/>
       <c r="AF57" s="52"/>
@@ -6195,18 +6283,18 @@
       <c r="O58" s="55"/>
       <c r="P58" s="55"/>
       <c r="Q58" s="56"/>
-      <c r="R58" s="54"/>
-      <c r="S58" s="55"/>
-      <c r="T58" s="55"/>
-      <c r="U58" s="55"/>
-      <c r="V58" s="55"/>
-      <c r="W58" s="56"/>
-      <c r="X58" s="54"/>
-      <c r="Y58" s="55"/>
-      <c r="Z58" s="55"/>
-      <c r="AA58" s="55"/>
-      <c r="AB58" s="55"/>
-      <c r="AC58" s="56"/>
+      <c r="R58" s="80"/>
+      <c r="S58" s="81"/>
+      <c r="T58" s="81"/>
+      <c r="U58" s="81"/>
+      <c r="V58" s="81"/>
+      <c r="W58" s="82"/>
+      <c r="X58" s="80"/>
+      <c r="Y58" s="81"/>
+      <c r="Z58" s="81"/>
+      <c r="AA58" s="81"/>
+      <c r="AB58" s="81"/>
+      <c r="AC58" s="82"/>
       <c r="AD58" s="54"/>
       <c r="AE58" s="55"/>
       <c r="AF58" s="55"/>
@@ -6270,18 +6358,18 @@
       <c r="O59" s="4"/>
       <c r="P59" s="4"/>
       <c r="Q59" s="5"/>
-      <c r="R59" s="6"/>
-      <c r="S59" s="4"/>
-      <c r="T59" s="4"/>
-      <c r="U59" s="4"/>
-      <c r="V59" s="4"/>
-      <c r="W59" s="5"/>
-      <c r="X59" s="6"/>
-      <c r="Y59" s="4"/>
-      <c r="Z59" s="4"/>
-      <c r="AA59" s="4"/>
-      <c r="AB59" s="4"/>
-      <c r="AC59" s="5"/>
+      <c r="R59" s="80"/>
+      <c r="S59" s="81"/>
+      <c r="T59" s="81"/>
+      <c r="U59" s="81"/>
+      <c r="V59" s="81"/>
+      <c r="W59" s="82"/>
+      <c r="X59" s="80"/>
+      <c r="Y59" s="81"/>
+      <c r="Z59" s="81"/>
+      <c r="AA59" s="81"/>
+      <c r="AB59" s="81"/>
+      <c r="AC59" s="82"/>
       <c r="AD59" s="6"/>
       <c r="AE59" s="4"/>
       <c r="AF59" s="4"/>
@@ -6347,18 +6435,18 @@
       <c r="O60" s="49"/>
       <c r="P60" s="49"/>
       <c r="Q60" s="50"/>
-      <c r="R60" s="48"/>
-      <c r="S60" s="49"/>
-      <c r="T60" s="49"/>
-      <c r="U60" s="49"/>
-      <c r="V60" s="49"/>
-      <c r="W60" s="50"/>
-      <c r="X60" s="48"/>
-      <c r="Y60" s="49"/>
-      <c r="Z60" s="49"/>
-      <c r="AA60" s="49"/>
-      <c r="AB60" s="49"/>
-      <c r="AC60" s="50"/>
+      <c r="R60" s="80"/>
+      <c r="S60" s="81"/>
+      <c r="T60" s="81"/>
+      <c r="U60" s="81"/>
+      <c r="V60" s="81"/>
+      <c r="W60" s="82"/>
+      <c r="X60" s="80"/>
+      <c r="Y60" s="81"/>
+      <c r="Z60" s="81"/>
+      <c r="AA60" s="81"/>
+      <c r="AB60" s="81"/>
+      <c r="AC60" s="82"/>
       <c r="AD60" s="48"/>
       <c r="AE60" s="49"/>
       <c r="AF60" s="49"/>
@@ -6420,18 +6508,18 @@
       <c r="O61" s="52"/>
       <c r="P61" s="52"/>
       <c r="Q61" s="53"/>
-      <c r="R61" s="51"/>
-      <c r="S61" s="52"/>
-      <c r="T61" s="52"/>
-      <c r="U61" s="52"/>
-      <c r="V61" s="52"/>
-      <c r="W61" s="53"/>
-      <c r="X61" s="51"/>
-      <c r="Y61" s="52"/>
-      <c r="Z61" s="52"/>
-      <c r="AA61" s="52"/>
-      <c r="AB61" s="52"/>
-      <c r="AC61" s="53"/>
+      <c r="R61" s="80"/>
+      <c r="S61" s="81"/>
+      <c r="T61" s="81"/>
+      <c r="U61" s="81"/>
+      <c r="V61" s="81"/>
+      <c r="W61" s="82"/>
+      <c r="X61" s="80"/>
+      <c r="Y61" s="81"/>
+      <c r="Z61" s="81"/>
+      <c r="AA61" s="81"/>
+      <c r="AB61" s="81"/>
+      <c r="AC61" s="82"/>
       <c r="AD61" s="51"/>
       <c r="AE61" s="52"/>
       <c r="AF61" s="52"/>
@@ -6493,18 +6581,18 @@
       <c r="O62" s="52"/>
       <c r="P62" s="52"/>
       <c r="Q62" s="53"/>
-      <c r="R62" s="51"/>
-      <c r="S62" s="52"/>
-      <c r="T62" s="52"/>
-      <c r="U62" s="52"/>
-      <c r="V62" s="52"/>
-      <c r="W62" s="53"/>
-      <c r="X62" s="51"/>
-      <c r="Y62" s="52"/>
-      <c r="Z62" s="52"/>
-      <c r="AA62" s="52"/>
-      <c r="AB62" s="52"/>
-      <c r="AC62" s="53"/>
+      <c r="R62" s="80"/>
+      <c r="S62" s="81"/>
+      <c r="T62" s="81"/>
+      <c r="U62" s="81"/>
+      <c r="V62" s="81"/>
+      <c r="W62" s="82"/>
+      <c r="X62" s="80"/>
+      <c r="Y62" s="81"/>
+      <c r="Z62" s="81"/>
+      <c r="AA62" s="81"/>
+      <c r="AB62" s="81"/>
+      <c r="AC62" s="82"/>
       <c r="AD62" s="51"/>
       <c r="AE62" s="52"/>
       <c r="AF62" s="52"/>
@@ -6566,18 +6654,18 @@
       <c r="O63" s="52"/>
       <c r="P63" s="52"/>
       <c r="Q63" s="53"/>
-      <c r="R63" s="51"/>
-      <c r="S63" s="52"/>
-      <c r="T63" s="52"/>
-      <c r="U63" s="52"/>
-      <c r="V63" s="52"/>
-      <c r="W63" s="53"/>
-      <c r="X63" s="51"/>
-      <c r="Y63" s="52"/>
-      <c r="Z63" s="52"/>
-      <c r="AA63" s="52"/>
-      <c r="AB63" s="52"/>
-      <c r="AC63" s="53"/>
+      <c r="R63" s="80"/>
+      <c r="S63" s="81"/>
+      <c r="T63" s="81"/>
+      <c r="U63" s="81"/>
+      <c r="V63" s="81"/>
+      <c r="W63" s="82"/>
+      <c r="X63" s="80"/>
+      <c r="Y63" s="81"/>
+      <c r="Z63" s="81"/>
+      <c r="AA63" s="81"/>
+      <c r="AB63" s="81"/>
+      <c r="AC63" s="82"/>
       <c r="AD63" s="51"/>
       <c r="AE63" s="52"/>
       <c r="AF63" s="52"/>
@@ -6639,18 +6727,18 @@
       <c r="O64" s="52"/>
       <c r="P64" s="52"/>
       <c r="Q64" s="53"/>
-      <c r="R64" s="51"/>
-      <c r="S64" s="52"/>
-      <c r="T64" s="52"/>
-      <c r="U64" s="52"/>
-      <c r="V64" s="52"/>
-      <c r="W64" s="53"/>
-      <c r="X64" s="51"/>
-      <c r="Y64" s="52"/>
-      <c r="Z64" s="52"/>
-      <c r="AA64" s="52"/>
-      <c r="AB64" s="52"/>
-      <c r="AC64" s="53"/>
+      <c r="R64" s="80"/>
+      <c r="S64" s="81"/>
+      <c r="T64" s="81"/>
+      <c r="U64" s="81"/>
+      <c r="V64" s="81"/>
+      <c r="W64" s="82"/>
+      <c r="X64" s="80"/>
+      <c r="Y64" s="81"/>
+      <c r="Z64" s="81"/>
+      <c r="AA64" s="81"/>
+      <c r="AB64" s="81"/>
+      <c r="AC64" s="82"/>
       <c r="AD64" s="51"/>
       <c r="AE64" s="52"/>
       <c r="AF64" s="52"/>
@@ -6712,18 +6800,18 @@
       <c r="O65" s="52"/>
       <c r="P65" s="52"/>
       <c r="Q65" s="53"/>
-      <c r="R65" s="51"/>
-      <c r="S65" s="52"/>
-      <c r="T65" s="52"/>
-      <c r="U65" s="52"/>
-      <c r="V65" s="52"/>
-      <c r="W65" s="53"/>
-      <c r="X65" s="51"/>
-      <c r="Y65" s="52"/>
-      <c r="Z65" s="52"/>
-      <c r="AA65" s="52"/>
-      <c r="AB65" s="52"/>
-      <c r="AC65" s="53"/>
+      <c r="R65" s="80"/>
+      <c r="S65" s="81"/>
+      <c r="T65" s="81"/>
+      <c r="U65" s="81"/>
+      <c r="V65" s="81"/>
+      <c r="W65" s="82"/>
+      <c r="X65" s="80"/>
+      <c r="Y65" s="81"/>
+      <c r="Z65" s="81"/>
+      <c r="AA65" s="81"/>
+      <c r="AB65" s="81"/>
+      <c r="AC65" s="82"/>
       <c r="AD65" s="51"/>
       <c r="AE65" s="52"/>
       <c r="AF65" s="52"/>
@@ -6785,18 +6873,18 @@
       <c r="O66" s="52"/>
       <c r="P66" s="52"/>
       <c r="Q66" s="53"/>
-      <c r="R66" s="51"/>
-      <c r="S66" s="52"/>
-      <c r="T66" s="52"/>
-      <c r="U66" s="52"/>
-      <c r="V66" s="52"/>
-      <c r="W66" s="53"/>
-      <c r="X66" s="51"/>
-      <c r="Y66" s="52"/>
-      <c r="Z66" s="52"/>
-      <c r="AA66" s="52"/>
-      <c r="AB66" s="52"/>
-      <c r="AC66" s="53"/>
+      <c r="R66" s="80"/>
+      <c r="S66" s="81"/>
+      <c r="T66" s="81"/>
+      <c r="U66" s="81"/>
+      <c r="V66" s="81"/>
+      <c r="W66" s="82"/>
+      <c r="X66" s="80"/>
+      <c r="Y66" s="81"/>
+      <c r="Z66" s="81"/>
+      <c r="AA66" s="81"/>
+      <c r="AB66" s="81"/>
+      <c r="AC66" s="82"/>
       <c r="AD66" s="51"/>
       <c r="AE66" s="52"/>
       <c r="AF66" s="52"/>
@@ -6858,18 +6946,18 @@
       <c r="O67" s="52"/>
       <c r="P67" s="52"/>
       <c r="Q67" s="53"/>
-      <c r="R67" s="51"/>
-      <c r="S67" s="52"/>
-      <c r="T67" s="52"/>
-      <c r="U67" s="52"/>
-      <c r="V67" s="52"/>
-      <c r="W67" s="53"/>
-      <c r="X67" s="51"/>
-      <c r="Y67" s="52"/>
-      <c r="Z67" s="52"/>
-      <c r="AA67" s="52"/>
-      <c r="AB67" s="52"/>
-      <c r="AC67" s="53"/>
+      <c r="R67" s="80"/>
+      <c r="S67" s="81"/>
+      <c r="T67" s="81"/>
+      <c r="U67" s="81"/>
+      <c r="V67" s="81"/>
+      <c r="W67" s="82"/>
+      <c r="X67" s="80"/>
+      <c r="Y67" s="81"/>
+      <c r="Z67" s="81"/>
+      <c r="AA67" s="81"/>
+      <c r="AB67" s="81"/>
+      <c r="AC67" s="82"/>
       <c r="AD67" s="51"/>
       <c r="AE67" s="52"/>
       <c r="AF67" s="52"/>
@@ -6931,18 +7019,18 @@
       <c r="O68" s="52"/>
       <c r="P68" s="52"/>
       <c r="Q68" s="53"/>
-      <c r="R68" s="51"/>
-      <c r="S68" s="52"/>
-      <c r="T68" s="52"/>
-      <c r="U68" s="52"/>
-      <c r="V68" s="52"/>
-      <c r="W68" s="53"/>
-      <c r="X68" s="51"/>
-      <c r="Y68" s="52"/>
-      <c r="Z68" s="52"/>
-      <c r="AA68" s="52"/>
-      <c r="AB68" s="52"/>
-      <c r="AC68" s="53"/>
+      <c r="R68" s="80"/>
+      <c r="S68" s="81"/>
+      <c r="T68" s="81"/>
+      <c r="U68" s="81"/>
+      <c r="V68" s="81"/>
+      <c r="W68" s="82"/>
+      <c r="X68" s="80"/>
+      <c r="Y68" s="81"/>
+      <c r="Z68" s="81"/>
+      <c r="AA68" s="81"/>
+      <c r="AB68" s="81"/>
+      <c r="AC68" s="82"/>
       <c r="AD68" s="51"/>
       <c r="AE68" s="52"/>
       <c r="AF68" s="52"/>
@@ -7004,18 +7092,18 @@
       <c r="O69" s="55"/>
       <c r="P69" s="55"/>
       <c r="Q69" s="56"/>
-      <c r="R69" s="54"/>
-      <c r="S69" s="55"/>
-      <c r="T69" s="55"/>
-      <c r="U69" s="55"/>
-      <c r="V69" s="55"/>
-      <c r="W69" s="56"/>
-      <c r="X69" s="54"/>
-      <c r="Y69" s="55"/>
-      <c r="Z69" s="55"/>
-      <c r="AA69" s="55"/>
-      <c r="AB69" s="55"/>
-      <c r="AC69" s="56"/>
+      <c r="R69" s="83"/>
+      <c r="S69" s="84"/>
+      <c r="T69" s="84"/>
+      <c r="U69" s="84"/>
+      <c r="V69" s="84"/>
+      <c r="W69" s="85"/>
+      <c r="X69" s="83"/>
+      <c r="Y69" s="84"/>
+      <c r="Z69" s="84"/>
+      <c r="AA69" s="84"/>
+      <c r="AB69" s="84"/>
+      <c r="AC69" s="85"/>
       <c r="AD69" s="54"/>
       <c r="AE69" s="55"/>
       <c r="AF69" s="55"/>
@@ -7055,19 +7143,20 @@
     </row>
   </sheetData>
   <sheetProtection insertRows="0"/>
-  <mergeCells count="35">
-    <mergeCell ref="AP1:AU1"/>
-    <mergeCell ref="AV1:BA1"/>
-    <mergeCell ref="AV2:AX2"/>
-    <mergeCell ref="AY2:BA2"/>
-    <mergeCell ref="AS2:AU2"/>
-    <mergeCell ref="AP2:AR2"/>
-    <mergeCell ref="BB2:BD2"/>
-    <mergeCell ref="BE2:BG2"/>
-    <mergeCell ref="BH2:BJ2"/>
-    <mergeCell ref="BK2:BM2"/>
-    <mergeCell ref="BB1:BG1"/>
-    <mergeCell ref="BH1:BM1"/>
+  <mergeCells count="37">
+    <mergeCell ref="R4:W69"/>
+    <mergeCell ref="X4:AC69"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="L1:Q1"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="C1:C2"/>
     <mergeCell ref="R1:W1"/>
     <mergeCell ref="X1:AC1"/>
     <mergeCell ref="AJ2:AL2"/>
@@ -7080,19 +7169,20 @@
     <mergeCell ref="AG2:AI2"/>
     <mergeCell ref="AM2:AO2"/>
     <mergeCell ref="AA2:AC2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="L1:Q1"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="O2:Q2"/>
-    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="BB2:BD2"/>
+    <mergeCell ref="BE2:BG2"/>
+    <mergeCell ref="BH2:BJ2"/>
+    <mergeCell ref="BK2:BM2"/>
+    <mergeCell ref="BB1:BG1"/>
+    <mergeCell ref="BH1:BM1"/>
+    <mergeCell ref="AP1:AU1"/>
+    <mergeCell ref="AV1:BA1"/>
+    <mergeCell ref="AV2:AX2"/>
+    <mergeCell ref="AY2:BA2"/>
+    <mergeCell ref="AS2:AU2"/>
+    <mergeCell ref="AP2:AR2"/>
   </mergeCells>
-  <conditionalFormatting sqref="F5:BM14">
+  <conditionalFormatting sqref="F5:Q14 AD5:BM14">
     <cfRule type="cellIs" dxfId="11" priority="159" stopIfTrue="1" operator="equal">
       <formula>"p"</formula>
     </cfRule>
@@ -7100,7 +7190,7 @@
       <formula>"r"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F16:BM25">
+  <conditionalFormatting sqref="F16:Q25 AD16:BM25">
     <cfRule type="cellIs" dxfId="9" priority="157" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
@@ -7108,7 +7198,7 @@
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F27:BM36">
+  <conditionalFormatting sqref="F27:Q36 AD27:BM36">
     <cfRule type="cellIs" dxfId="7" priority="155" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
@@ -7116,7 +7206,7 @@
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F38:BM47">
+  <conditionalFormatting sqref="F38:Q47 AD38:BM47">
     <cfRule type="cellIs" dxfId="5" priority="153" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
@@ -7124,7 +7214,7 @@
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F49:BM58">
+  <conditionalFormatting sqref="F49:Q58 AD49:BM58">
     <cfRule type="cellIs" dxfId="3" priority="151" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
@@ -7132,7 +7222,7 @@
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F60:BM69">
+  <conditionalFormatting sqref="F60:Q69 AD60:BM69">
     <cfRule type="cellIs" dxfId="1" priority="149" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>

</xml_diff>